<commit_message>
updateInfo to dynamically load all fields into display ul
</commit_message>
<xml_diff>
--- a/SourceData/CountyData.xlsx
+++ b/SourceData/CountyData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
   <si>
     <t>Adams</t>
   </si>
@@ -253,24 +253,12 @@
     <t>food_banks</t>
   </si>
   <si>
-    <t>field name</t>
-  </si>
-  <si>
     <t>class</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
-    <t>demographic_data_header</t>
-  </si>
-  <si>
-    <t>demographic_data_primary</t>
-  </si>
-  <si>
-    <t>demographic_data_secondary</t>
-  </si>
-  <si>
     <t>Total population</t>
   </si>
   <si>
@@ -296,6 +284,21 @@
   </si>
   <si>
     <t>Number of State Food Purchase Program (Food Banks) participants</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -361,8 +364,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -407,7 +428,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -426,6 +447,15 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -444,6 +474,15 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -648,7 +687,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0">
   <autoFilter ref="A1:C11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="field name"/>
+    <tableColumn id="1" name="name"/>
     <tableColumn id="2" name="class"/>
     <tableColumn id="3" name="description"/>
   </tableColumns>
@@ -1034,39 +1073,39 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C33" ca="1" si="0">RAND()*100</f>
-        <v>34.831965858838196</v>
+        <v>92.756251544578589</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:D33" ca="1" si="1">RAND()/5*300</f>
-        <v>15.952266829454899</v>
+        <v>59.558114301736083</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E33" ca="1" si="2">RAND()*$B2</f>
-        <v>7656.8270369888251</v>
+        <v>8334.3019282013265</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" ref="F2:F33" ca="1" si="3">$E2/$B2*100</f>
-        <v>62.023710303676182</v>
+        <v>67.511558754162223</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" ref="G2:G33" ca="1" si="4">$B2*0.3*RAND()</f>
-        <v>2280.4439039654944</v>
+        <v>3296.477727178843</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H33" ca="1" si="5">$B2*0.4*RAND()</f>
-        <v>4258.7303028330925</v>
+        <v>4182.30004895399</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" ref="I2:I33" ca="1" si="6">$B2*0.1*RAND()</f>
-        <v>1131.1100407496083</v>
+        <v>332.17547819809926</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" ref="J2:J33" ca="1" si="7">$B2*0.5*RAND()</f>
-        <v>5616.3089049906166</v>
+        <v>295.62361719768853</v>
       </c>
       <c r="L2" t="str">
         <f ca="1">CONCATENATE("    {""",$A$1,""":""",$A2,""",""",$B$1,""":",$B2,",""",$C$1,""":",$C2,",""",$D$1,""":",$D2,",""",$E$1,""":",$E2,",""",$F$1,""":",$F2,",""",$G$1,""":",$G2,",""",$H$1,""":",$H2,",""",$I$1,""":",$I2,",""",$J$1,""":",$J2,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Adams","population":12345,"food_ins_rate":34.8319658588382,"food_ins_rate_child":15.9522668294549,"snap":7656.82703698883,"snap_percentage":62.0237103036762,"wic":2280.44390396549,"free_lunch":4258.73030283309,"free_breakfast":1131.11004074961,"food_banks":5616.30890499062},</v>
+        <v xml:space="preserve">    {"county_name":"Adams","population":12345,"food_ins_rate":92.7562515445786,"food_ins_rate_child":59.5581143017361,"snap":8334.30192820133,"snap_percentage":67.5115587541622,"wic":3296.47772717884,"free_lunch":4182.30004895399,"free_breakfast":332.175478198099,"food_banks":295.623617197689},</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1078,39 +1117,39 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>62.758167974016629</v>
+        <v>64.49039520813605</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>38.089783071701902</v>
+        <v>2.5865763260580854</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>8681.2507902372108</v>
+        <v>1376.3799377353157</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>37.010789521816214</v>
+        <v>5.8679226540557456</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>5701.042749961759</v>
+        <v>5276.7136402718406</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1629.1019011782919</v>
+        <v>3944.197985732359</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>401.79553127753212</v>
+        <v>719.266336526754</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>8489.0455786052771</v>
+        <v>43.732806196598659</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L66" ca="1" si="8">CONCATENATE("    {""",$A$1,""":""",$A3,""",""",$B$1,""":",$B3,",""",$C$1,""":",$C3,",""",$D$1,""":",$D3,",""",$E$1,""":",$E3,",""",$F$1,""":",$F3,",""",$G$1,""":",$G3,",""",$H$1,""":",$H3,",""",$I$1,""":",$I3,",""",$J$1,""":",$J3,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Allegheny","population":23456,"food_ins_rate":62.7581679740166,"food_ins_rate_child":38.0897830717019,"snap":8681.25079023721,"snap_percentage":37.0107895218162,"wic":5701.04274996176,"free_lunch":1629.10190117829,"free_breakfast":401.795531277532,"food_banks":8489.04557860528},</v>
+        <v xml:space="preserve">    {"county_name":"Allegheny","population":23456,"food_ins_rate":64.4903952081361,"food_ins_rate_child":2.58657632605809,"snap":1376.37993773532,"snap_percentage":5.86792265405575,"wic":5276.71364027184,"free_lunch":3944.19798573236,"free_breakfast":719.266336526754,"food_banks":43.7328061965987},</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1122,39 +1161,39 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>49.427599083198857</v>
+        <v>23.2707572167843</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>55.211143214118017</v>
+        <v>5.8688554043243997</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>258734.54539865331</v>
+        <v>216812.46263739443</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>75.821202309982411</v>
+        <v>63.536090890478171</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>71827.712041339939</v>
+        <v>25510.920589965295</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>27408.544776096518</v>
+        <v>94495.477727494581</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>7059.0962386318224</v>
+        <v>20547.780476296371</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>7288.2103324255631</v>
+        <v>88553.517617241203</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Armstrong","population":341243,"food_ins_rate":49.4275990831989,"food_ins_rate_child":55.211143214118,"snap":258734.545398653,"snap_percentage":75.8212023099824,"wic":71827.7120413399,"free_lunch":27408.5447760965,"free_breakfast":7059.09623863182,"food_banks":7288.21033242556},</v>
+        <v xml:space="preserve">    {"county_name":"Armstrong","population":341243,"food_ins_rate":23.2707572167843,"food_ins_rate_child":5.8688554043244,"snap":216812.462637394,"snap_percentage":63.5360908904782,"wic":25510.9205899653,"free_lunch":94495.4777274946,"free_breakfast":20547.7804762964,"food_banks":88553.5176172412},</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1166,39 +1205,39 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>78.31745346642326</v>
+        <v>0.60555098629375692</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>24.20962438464689</v>
+        <v>36.426903622675255</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>324.7464244975003</v>
+        <v>245227.20289236205</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>7.1438888810937407E-2</v>
+        <v>53.945963863813041</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>115541.92461499799</v>
+        <v>60786.734351469539</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>11081.789162694084</v>
+        <v>4328.8193490579497</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>843.89415595582102</v>
+        <v>34386.401038873926</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>77621.784469869352</v>
+        <v>192929.09825180547</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Beaver","population":454579.333333333,"food_ins_rate":78.3174534664233,"food_ins_rate_child":24.2096243846469,"snap":324.7464244975,"snap_percentage":0.0714388888109374,"wic":115541.924614998,"free_lunch":11081.7891626941,"free_breakfast":843.894155955821,"food_banks":77621.7844698694},</v>
+        <v xml:space="preserve">    {"county_name":"Beaver","population":454579.333333333,"food_ins_rate":0.605550986293757,"food_ins_rate_child":36.4269036226753,"snap":245227.202892362,"snap_percentage":53.945963863813,"wic":60786.7343514695,"free_lunch":4328.81934905795,"free_breakfast":34386.4010388739,"food_banks":192929.098251805},</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1210,39 +1249,39 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>91.991790236281958</v>
+        <v>29.932820134723602</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7409386439561017</v>
+        <v>30.761850251891936</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>330622.1660206003</v>
+        <v>485297.72342128202</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>53.409859972042284</v>
+        <v>78.396689988010607</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>174233.64244646503</v>
+        <v>124382.48118264077</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>55015.181371721003</v>
+        <v>118693.95813148777</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>11886.811689967444</v>
+        <v>21223.742714545886</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>285976.51608904509</v>
+        <v>157299.9590924638</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bedford","population":619028.333333333,"food_ins_rate":91.991790236282,"food_ins_rate_child":7.7409386439561,"snap":330622.1660206,"snap_percentage":53.4098599720423,"wic":174233.642446465,"free_lunch":55015.181371721,"free_breakfast":11886.8116899674,"food_banks":285976.516089045},</v>
+        <v xml:space="preserve">    {"county_name":"Bedford","population":619028.333333333,"food_ins_rate":29.9328201347236,"food_ins_rate_child":30.7618502518919,"snap":485297.723421282,"snap_percentage":78.3966899880106,"wic":124382.481182641,"free_lunch":118693.958131488,"free_breakfast":21223.7427145459,"food_banks":157299.959092464},</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1254,39 +1293,39 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>67.970746817700842</v>
+        <v>56.580041706770267</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>18.222908789630999</v>
+        <v>54.150415148587236</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>524017.77222663909</v>
+        <v>152305.53685185566</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>66.883590619933614</v>
+        <v>19.439686430220792</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>56039.422925952451</v>
+        <v>197912.26170990939</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>232225.01230239478</v>
+        <v>33187.641354540676</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>30090.414374438122</v>
+        <v>59865.545164988478</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>336113.48217604676</v>
+        <v>134742.88850915479</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Berks","population":783477.333333333,"food_ins_rate":67.9707468177008,"food_ins_rate_child":18.222908789631,"snap":524017.772226639,"snap_percentage":66.8835906199336,"wic":56039.4229259525,"free_lunch":232225.012302395,"free_breakfast":30090.4143744381,"food_banks":336113.482176047},</v>
+        <v xml:space="preserve">    {"county_name":"Berks","population":783477.333333333,"food_ins_rate":56.5800417067703,"food_ins_rate_child":54.1504151485872,"snap":152305.536851856,"snap_percentage":19.4396864302208,"wic":197912.261709909,"free_lunch":33187.6413545407,"free_breakfast":59865.5451649885,"food_banks":134742.888509155},</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1298,39 +1337,39 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>21.988519391737839</v>
+        <v>86.127850759372905</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>22.322326603064337</v>
+        <v>56.582428318058426</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>363243.36118831957</v>
+        <v>556293.13695606205</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>38.319787985105705</v>
+        <v>58.685270932382117</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>244912.56117390137</v>
+        <v>213763.72674727155</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>341463.68789709598</v>
+        <v>133131.2922601602</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>21526.154731942326</v>
+        <v>62839.911989814769</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>187871.34724799677</v>
+        <v>115978.52819521575</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Blair","population":947926.333333333,"food_ins_rate":21.9885193917378,"food_ins_rate_child":22.3223266030643,"snap":363243.36118832,"snap_percentage":38.3197879851057,"wic":244912.561173901,"free_lunch":341463.687897096,"free_breakfast":21526.1547319423,"food_banks":187871.347247997},</v>
+        <v xml:space="preserve">    {"county_name":"Blair","population":947926.333333333,"food_ins_rate":86.1278507593729,"food_ins_rate_child":56.5824283180584,"snap":556293.136956062,"snap_percentage":58.6852709323821,"wic":213763.726747272,"free_lunch":133131.29226016,"free_breakfast":62839.9119898148,"food_banks":115978.528195216},</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1342,39 +1381,39 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>63.416113905642661</v>
+        <v>38.523871116018526</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>25.878883442805236</v>
+        <v>21.277866603343227</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>794209.6743291592</v>
+        <v>258778.00696301763</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>71.397634461134658</v>
+        <v>23.263551357936596</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>40366.021355422075</v>
+        <v>127090.00004986818</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>758.66334377649537</v>
+        <v>77517.441292853226</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>55620.417828992977</v>
+        <v>80683.089985379105</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>190795.27560875833</v>
+        <v>139365.35690083471</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bradford","population":1112375.33333333,"food_ins_rate":63.4161139056427,"food_ins_rate_child":25.8788834428052,"snap":794209.674329159,"snap_percentage":71.3976344611347,"wic":40366.0213554221,"free_lunch":758.663343776495,"free_breakfast":55620.417828993,"food_banks":190795.275608758},</v>
+        <v xml:space="preserve">    {"county_name":"Bradford","population":1112375.33333333,"food_ins_rate":38.5238711160185,"food_ins_rate_child":21.2778666033432,"snap":258778.006963018,"snap_percentage":23.2635513579366,"wic":127090.000049868,"free_lunch":77517.4412928532,"free_breakfast":80683.0899853791,"food_banks":139365.356900835},</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1386,39 +1425,39 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0432243838306432</v>
+        <v>67.527782700276788</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>15.046290203407214</v>
+        <v>57.226204719600418</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>999662.2888658857</v>
+        <v>1127948.2549744041</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>78.292860087975171</v>
+        <v>88.340128358122385</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>37399.718773300818</v>
+        <v>12820.703250480836</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>230219.74819304669</v>
+        <v>416997.33390751941</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>72321.19666154818</v>
+        <v>6788.9592842509719</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>587159.61140982236</v>
+        <v>353170.31281887856</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bucks","population":1276824.33333333,"food_ins_rate":1.04322438383064,"food_ins_rate_child":15.0462902034072,"snap":999662.288865886,"snap_percentage":78.2928600879752,"wic":37399.7187733008,"free_lunch":230219.748193047,"free_breakfast":72321.1966615482,"food_banks":587159.611409822},</v>
+        <v xml:space="preserve">    {"county_name":"Bucks","population":1276824.33333333,"food_ins_rate":67.5277827002768,"food_ins_rate_child":57.2262047196004,"snap":1127948.2549744,"snap_percentage":88.3401283581224,"wic":12820.7032504808,"free_lunch":416997.333907519,"free_breakfast":6788.95928425097,"food_banks":353170.312818879},</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1430,39 +1469,39 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3575564328193241</v>
+        <v>81.697893268554907</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>14.044448076448518</v>
+        <v>29.34346170506231</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>255157.02371771392</v>
+        <v>638275.90589440323</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>17.703583200807238</v>
+        <v>44.285555774366514</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>399358.24716746702</v>
+        <v>368074.62311222096</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>58262.396698634453</v>
+        <v>387499.05186652025</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>109272.55952067957</v>
+        <v>76047.156136368692</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>299277.97675973707</v>
+        <v>147230.96295708013</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Butler","population":1441273.33333333,"food_ins_rate":8.35755643281932,"food_ins_rate_child":14.0444480764485,"snap":255157.023717714,"snap_percentage":17.7035832008072,"wic":399358.247167467,"free_lunch":58262.3966986345,"free_breakfast":109272.55952068,"food_banks":299277.976759737},</v>
+        <v xml:space="preserve">    {"county_name":"Butler","population":1441273.33333333,"food_ins_rate":81.6978932685549,"food_ins_rate_child":29.3434617050623,"snap":638275.905894403,"snap_percentage":44.2855557743665,"wic":368074.623112221,"free_lunch":387499.05186652,"free_breakfast":76047.1561363687,"food_banks":147230.96295708},</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1474,39 +1513,39 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>92.094173537708912</v>
+        <v>75.341867748628388</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>29.605282239654375</v>
+        <v>31.906456374155756</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1002343.8222607374</v>
+        <v>226105.77538322879</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>62.423234793027071</v>
+        <v>14.081249957696873</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>416729.39327413251</v>
+        <v>75807.542780792646</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>482372.38857734494</v>
+        <v>401117.90258185269</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>142361.54457996078</v>
+        <v>100676.8920948234</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>222118.00050106589</v>
+        <v>222306.67299844811</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cambria","population":1605722.33333333,"food_ins_rate":92.0941735377089,"food_ins_rate_child":29.6052822396544,"snap":1002343.82226074,"snap_percentage":62.4232347930271,"wic":416729.393274133,"free_lunch":482372.388577345,"free_breakfast":142361.544579961,"food_banks":222118.000501066},</v>
+        <v xml:space="preserve">    {"county_name":"Cambria","population":1605722.33333333,"food_ins_rate":75.3418677486284,"food_ins_rate_child":31.9064563741558,"snap":226105.775383229,"snap_percentage":14.0812499576969,"wic":75807.5427807926,"free_lunch":401117.902581853,"free_breakfast":100676.892094823,"food_banks":222306.672998448},</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1518,39 +1557,39 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>54.458156922650232</v>
+        <v>38.134046561662558</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>13.61018608845932</v>
+        <v>24.662211530804292</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>403668.1861398883</v>
+        <v>992461.83723988326</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>22.803904827662016</v>
+        <v>56.065863148457105</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>125773.41763702886</v>
+        <v>358442.7209046536</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>447636.89306760993</v>
+        <v>420174.64830475254</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>87877.392415157519</v>
+        <v>170227.45106904415</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>868401.43658185564</v>
+        <v>490409.32142889855</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cameron","population":1770171.33333333,"food_ins_rate":54.4581569226502,"food_ins_rate_child":13.6101860884593,"snap":403668.186139888,"snap_percentage":22.803904827662,"wic":125773.417637029,"free_lunch":447636.89306761,"free_breakfast":87877.3924151575,"food_banks":868401.436581856},</v>
+        <v xml:space="preserve">    {"county_name":"Cameron","population":1770171.33333333,"food_ins_rate":38.1340465616626,"food_ins_rate_child":24.6622115308043,"snap":992461.837239883,"snap_percentage":56.0658631484571,"wic":358442.720904654,"free_lunch":420174.648304753,"free_breakfast":170227.451069044,"food_banks":490409.321428899},</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1562,39 +1601,39 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>65.906617527830477</v>
+        <v>4.8700379885052598</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>59.807160384319822</v>
+        <v>28.374220004301176</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1002669.7658436188</v>
+        <v>1348844.1044593393</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>51.827728085335977</v>
+        <v>69.721385701312016</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>193444.03653964144</v>
+        <v>384962.9464100498</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>677286.89858983434</v>
+        <v>743806.69523913716</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>48561.452547547648</v>
+        <v>65739.366778945987</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>249986.51393084339</v>
+        <v>864921.80457238248</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Carbon","population":1934620.33333333,"food_ins_rate":65.9066175278305,"food_ins_rate_child":59.8071603843198,"snap":1002669.76584362,"snap_percentage":51.827728085336,"wic":193444.036539641,"free_lunch":677286.898589834,"free_breakfast":48561.4525475476,"food_banks":249986.513930843},</v>
+        <v xml:space="preserve">    {"county_name":"Carbon","population":1934620.33333333,"food_ins_rate":4.87003798850526,"food_ins_rate_child":28.3742200043012,"snap":1348844.10445934,"snap_percentage":69.721385701312,"wic":384962.94641005,"free_lunch":743806.695239137,"free_breakfast":65739.366778946,"food_banks":864921.804572382},</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1606,39 +1645,39 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>30.573885344557528</v>
+        <v>70.099414279187741</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>58.970805836393225</v>
+        <v>7.4311653733325622</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1936517.1886029118</v>
+        <v>1707567.3441062048</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>92.255989730825846</v>
+        <v>81.348782386076849</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>65231.525165013983</v>
+        <v>70227.771893377765</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>813307.46306404332</v>
+        <v>21221.490945559795</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>900.49144812753161</v>
+        <v>165963.65869472962</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>407263.0326328529</v>
+        <v>547932.91815381229</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Centre","population":2099069.33333333,"food_ins_rate":30.5738853445575,"food_ins_rate_child":58.9708058363932,"snap":1936517.18860291,"snap_percentage":92.2559897308258,"wic":65231.525165014,"free_lunch":813307.463064043,"free_breakfast":900.491448127532,"food_banks":407263.032632853},</v>
+        <v xml:space="preserve">    {"county_name":"Centre","population":2099069.33333333,"food_ins_rate":70.0994142791877,"food_ins_rate_child":7.43116537333256,"snap":1707567.3441062,"snap_percentage":81.3487823860768,"wic":70227.7718933778,"free_lunch":21221.4909455598,"free_breakfast":165963.65869473,"food_banks":547932.918153812},</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1650,39 +1689,39 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>71.219076858044033</v>
+        <v>71.521597221200835</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>19.651449743579384</v>
+        <v>39.370642580058728</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2044419.0501040211</v>
+        <v>836912.06106121023</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>90.320410486507683</v>
+        <v>36.973946653603932</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>226086.35184468518</v>
+        <v>143143.04186279801</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>564343.54597247415</v>
+        <v>648637.39478696825</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>153073.9858439875</v>
+        <v>213856.02728038051</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>547204.89826817519</v>
+        <v>112211.63746291237</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Chester","population":2263518.33333333,"food_ins_rate":71.219076858044,"food_ins_rate_child":19.6514497435794,"snap":2044419.05010402,"snap_percentage":90.3204104865077,"wic":226086.351844685,"free_lunch":564343.545972474,"free_breakfast":153073.985843987,"food_banks":547204.898268175},</v>
+        <v xml:space="preserve">    {"county_name":"Chester","population":2263518.33333333,"food_ins_rate":71.5215972212008,"food_ins_rate_child":39.3706425800587,"snap":836912.06106121,"snap_percentage":36.9739466536039,"wic":143143.041862798,"free_lunch":648637.394786968,"free_breakfast":213856.027280381,"food_banks":112211.637462912},</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1694,39 +1733,39 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>32.247392020714116</v>
+        <v>28.589968966786628</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>12.007586210157966</v>
+        <v>49.533828549767598</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2378905.2246064278</v>
+        <v>2230160.7449360644</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>97.979292882019735</v>
+        <v>91.852996303467577</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>566038.81064174604</v>
+        <v>593009.50525712897</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>166818.05245775747</v>
+        <v>453639.43057577172</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>172984.66349664051</v>
+        <v>112847.17668011806</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>994177.33800835034</v>
+        <v>624910.72956116113</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clarion","population":2427967.33333333,"food_ins_rate":32.2473920207141,"food_ins_rate_child":12.007586210158,"snap":2378905.22460643,"snap_percentage":97.9792928820197,"wic":566038.810641746,"free_lunch":166818.052457757,"free_breakfast":172984.663496641,"food_banks":994177.33800835},</v>
+        <v xml:space="preserve">    {"county_name":"Clarion","population":2427967.33333333,"food_ins_rate":28.5899689667866,"food_ins_rate_child":49.5338285497676,"snap":2230160.74493606,"snap_percentage":91.8529963034676,"wic":593009.505257129,"free_lunch":453639.430575772,"free_breakfast":112847.176680118,"food_banks":624910.729561161},</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1738,39 +1777,39 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>99.326990331541893</v>
+        <v>29.851374779291739</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>21.576226592202687</v>
+        <v>5.92760229816363</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>719006.42688134336</v>
+        <v>1021547.8724151935</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>27.734990619999856</v>
+        <v>39.405239786530998</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>21271.328940801683</v>
+        <v>106987.3643454159</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>690432.29081979755</v>
+        <v>249201.86577876742</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>15900.778037145383</v>
+        <v>244994.86104935201</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>209299.16504326696</v>
+        <v>1033451.7051553151</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clearfield","population":2592416.33333333,"food_ins_rate":99.3269903315419,"food_ins_rate_child":21.5762265922027,"snap":719006.426881343,"snap_percentage":27.7349906199999,"wic":21271.3289408017,"free_lunch":690432.290819798,"free_breakfast":15900.7780371454,"food_banks":209299.165043267},</v>
+        <v xml:space="preserve">    {"county_name":"Clearfield","population":2592416.33333333,"food_ins_rate":29.8513747792917,"food_ins_rate_child":5.92760229816363,"snap":1021547.87241519,"snap_percentage":39.405239786531,"wic":106987.364345416,"free_lunch":249201.865778767,"free_breakfast":244994.861049352,"food_banks":1033451.70515532},</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1782,39 +1821,39 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>50.770010548691104</v>
+        <v>84.652791492701638</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>31.08563600272397</v>
+        <v>59.490024655491851</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1605087.457437739</v>
+        <v>1274087.9817612434</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>58.221467622323985</v>
+        <v>46.215096775174786</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>382279.81632252835</v>
+        <v>49961.351258848204</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>758744.88196305477</v>
+        <v>442498.56033688219</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>182871.17631487382</v>
+        <v>54503.87279164722</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>845395.68564313918</v>
+        <v>766228.89658283931</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clinton","population":2756865.33333333,"food_ins_rate":50.7700105486911,"food_ins_rate_child":31.085636002724,"snap":1605087.45743774,"snap_percentage":58.221467622324,"wic":382279.816322528,"free_lunch":758744.881963055,"free_breakfast":182871.176314874,"food_banks":845395.685643139},</v>
+        <v xml:space="preserve">    {"county_name":"Clinton","population":2756865.33333333,"food_ins_rate":84.6527914927016,"food_ins_rate_child":59.4900246554919,"snap":1274087.98176124,"snap_percentage":46.2150967751748,"wic":49961.3512588482,"free_lunch":442498.560336882,"free_breakfast":54503.8727916472,"food_banks":766228.896582839},</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1826,39 +1865,39 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45.100395713815253</v>
+        <v>49.943727895393508</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>13.81418797679606</v>
+        <v>2.1067342427125113</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1304611.6353756392</v>
+        <v>614974.16707989189</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>44.658379294878138</v>
+        <v>21.051283665807475</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>54060.024330194407</v>
+        <v>460499.83594519453</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>143388.15314123919</v>
+        <v>750260.26449828804</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>290976.5096536646</v>
+        <v>47292.667877733271</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>42524.380394188833</v>
+        <v>1091704.7421344467</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Columbia","population":2921314.33333333,"food_ins_rate":45.1003957138153,"food_ins_rate_child":13.8141879767961,"snap":1304611.63537564,"snap_percentage":44.6583792948781,"wic":54060.0243301944,"free_lunch":143388.153141239,"free_breakfast":290976.509653665,"food_banks":42524.3803941888},</v>
+        <v xml:space="preserve">    {"county_name":"Columbia","population":2921314.33333333,"food_ins_rate":49.9437278953935,"food_ins_rate_child":2.10673424271251,"snap":614974.167079892,"snap_percentage":21.0512836658075,"wic":460499.835945195,"free_lunch":750260.264498288,"free_breakfast":47292.6678777333,"food_banks":1091704.74213445},</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1870,39 +1909,39 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>88.982099970339263</v>
+        <v>0.96502070912795057</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>54.788754178421676</v>
+        <v>20.69998708994628</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1956533.5875442408</v>
+        <v>1600500.2356333649</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>63.405173248679993</v>
+        <v>51.86723875886031</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>574349.16653038724</v>
+        <v>622363.61905787943</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>610728.27003941068</v>
+        <v>601206.56172056985</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>292807.43797921663</v>
+        <v>79949.482718338666</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>257166.23590789025</v>
+        <v>1398625.2664674569</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Crawford","population":3085763.33333333,"food_ins_rate":88.9820999703393,"food_ins_rate_child":54.7887541784217,"snap":1956533.58754424,"snap_percentage":63.40517324868,"wic":574349.166530387,"free_lunch":610728.270039411,"free_breakfast":292807.437979217,"food_banks":257166.23590789},</v>
+        <v xml:space="preserve">    {"county_name":"Crawford","population":3085763.33333333,"food_ins_rate":0.965020709127951,"food_ins_rate_child":20.6999870899463,"snap":1600500.23563336,"snap_percentage":51.8672387588603,"wic":622363.619057879,"free_lunch":601206.56172057,"free_breakfast":79949.4827183387,"food_banks":1398625.26646746},</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1914,39 +1953,39 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45.462865319519487</v>
+        <v>72.56816807793345</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>36.674838620736729</v>
+        <v>14.614000146704718</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1377488.900066264</v>
+        <v>2370104.2973788744</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>42.38150492320446</v>
+        <v>72.921521867100893</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>731594.06388834922</v>
+        <v>454810.40959077328</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>69759.213470109753</v>
+        <v>170715.18036703553</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>277012.39018540649</v>
+        <v>285708.72832434269</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1519064.7938821027</v>
+        <v>487442.12612526753</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cumberland","population":3250212.33333333,"food_ins_rate":45.4628653195195,"food_ins_rate_child":36.6748386207367,"snap":1377488.90006626,"snap_percentage":42.3815049232045,"wic":731594.063888349,"free_lunch":69759.2134701098,"free_breakfast":277012.390185406,"food_banks":1519064.7938821},</v>
+        <v xml:space="preserve">    {"county_name":"Cumberland","population":3250212.33333333,"food_ins_rate":72.5681680779334,"food_ins_rate_child":14.6140001467047,"snap":2370104.29737887,"snap_percentage":72.9215218671009,"wic":454810.409590773,"free_lunch":170715.180367036,"free_breakfast":285708.728324343,"food_banks":487442.126125268},</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1958,39 +1997,39 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1521754087103009</v>
+        <v>89.645956095821973</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>28.425415355325843</v>
+        <v>40.581299520869258</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1919230.0482133385</v>
+        <v>142464.61482609625</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>56.205575337095617</v>
+        <v>4.1721447874019439</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>272157.40367527615</v>
+        <v>200786.95162778336</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>628773.95081538986</v>
+        <v>630032.38026304962</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>297362.21282811189</v>
+        <v>214671.17625738721</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>457772.77182640258</v>
+        <v>1563932.7707039155</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Dauphin","population":3414661.33333333,"food_ins_rate":4.1521754087103,"food_ins_rate_child":28.4254153553258,"snap":1919230.04821334,"snap_percentage":56.2055753370956,"wic":272157.403675276,"free_lunch":628773.95081539,"free_breakfast":297362.212828112,"food_banks":457772.771826403},</v>
+        <v xml:space="preserve">    {"county_name":"Dauphin","population":3414661.33333333,"food_ins_rate":89.645956095822,"food_ins_rate_child":40.5812995208693,"snap":142464.614826096,"snap_percentage":4.17214478740194,"wic":200786.951627783,"free_lunch":630032.38026305,"free_breakfast":214671.176257387,"food_banks":1563932.77070392},</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2002,39 +2041,39 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>85.482225164435178</v>
+        <v>5.8177849231610734</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>34.229919864243499</v>
+        <v>18.205637498330944</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3546560.2136595342</v>
+        <v>307687.80073979642</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>99.090552773111042</v>
+        <v>8.5967676904008083</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>142553.47716749852</v>
+        <v>186883.74458600985</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>378110.38212532923</v>
+        <v>200660.91697181782</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>111825.06301996291</v>
+        <v>351328.3504216033</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>178666.92799124916</v>
+        <v>520500.09584041371</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Delaware","population":3579110.33333333,"food_ins_rate":85.4822251644352,"food_ins_rate_child":34.2299198642435,"snap":3546560.21365953,"snap_percentage":99.090552773111,"wic":142553.477167499,"free_lunch":378110.382125329,"free_breakfast":111825.063019963,"food_banks":178666.927991249},</v>
+        <v xml:space="preserve">    {"county_name":"Delaware","population":3579110.33333333,"food_ins_rate":5.81778492316107,"food_ins_rate_child":18.2056374983309,"snap":307687.800739796,"snap_percentage":8.59676769040081,"wic":186883.74458601,"free_lunch":200660.916971818,"free_breakfast":351328.350421603,"food_banks":520500.095840414},</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2046,39 +2085,39 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>52.946341437103541</v>
+        <v>49.2727813155444</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>41.102061996554973</v>
+        <v>10.323824742323938</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2408995.926588729</v>
+        <v>2541061.1233604848</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>64.350413926623077</v>
+        <v>67.878211538799889</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>403113.17856362165</v>
+        <v>311652.77803548292</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1266772.9632840136</v>
+        <v>591.34155417246359</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>286192.49133728672</v>
+        <v>91903.620417733255</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>171559.25308063507</v>
+        <v>1803017.1060861631</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Elk","population":3743559.33333333,"food_ins_rate":52.9463414371035,"food_ins_rate_child":41.102061996555,"snap":2408995.92658873,"snap_percentage":64.3504139266231,"wic":403113.178563622,"free_lunch":1266772.96328401,"free_breakfast":286192.491337287,"food_banks":171559.253080635},</v>
+        <v xml:space="preserve">    {"county_name":"Elk","population":3743559.33333333,"food_ins_rate":49.2727813155444,"food_ins_rate_child":10.3238247423239,"snap":2541061.12336048,"snap_percentage":67.8782115387999,"wic":311652.778035483,"free_lunch":591.341554172464,"free_breakfast":91903.6204177333,"food_banks":1803017.10608616},</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2090,39 +2129,39 @@
       </c>
       <c r="C26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7.2051310027883897</v>
+        <v>89.096524914476845</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10.977145348527724</v>
+        <v>43.824166062771546</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2317663.9399412614</v>
+        <v>1386588.3750417384</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>59.305501479430397</v>
+        <v>35.480691359198048</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>723037.28026232531</v>
+        <v>693436.1350419576</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>814002.30049674737</v>
+        <v>1417966.050821594</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>234500.66643289494</v>
+        <v>388347.97897378146</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1025937.4217467635</v>
+        <v>1400782.528847815</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Erie","population":3908008.33333333,"food_ins_rate":7.20513100278839,"food_ins_rate_child":10.9771453485277,"snap":2317663.93994126,"snap_percentage":59.3055014794304,"wic":723037.280262325,"free_lunch":814002.300496747,"free_breakfast":234500.666432895,"food_banks":1025937.42174676},</v>
+        <v xml:space="preserve">    {"county_name":"Erie","population":3908008.33333333,"food_ins_rate":89.0965249144768,"food_ins_rate_child":43.8241660627715,"snap":1386588.37504174,"snap_percentage":35.480691359198,"wic":693436.135041958,"free_lunch":1417966.05082159,"free_breakfast":388347.978973781,"food_banks":1400782.52884782},</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2134,39 +2173,39 @@
       </c>
       <c r="C27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>27.245227340817159</v>
+        <v>51.438090024838559</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.381931904542498</v>
+        <v>15.194813990384056</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>888147.10018948163</v>
+        <v>3497353.9933760753</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>21.808628734301017</v>
+        <v>85.878223075537306</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>208417.18289431799</v>
+        <v>44014.336781915808</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>682473.7999202779</v>
+        <v>425649.34802979603</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>302609.91992044658</v>
+        <v>373538.33205101505</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>401626.34383832727</v>
+        <v>1022535.6209283222</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Fayette","population":4072457.33333333,"food_ins_rate":27.2452273408172,"food_ins_rate_child":48.3819319045425,"snap":888147.100189482,"snap_percentage":21.808628734301,"wic":208417.182894318,"free_lunch":682473.799920278,"free_breakfast":302609.919920447,"food_banks":401626.343838327},</v>
+        <v xml:space="preserve">    {"county_name":"Fayette","population":4072457.33333333,"food_ins_rate":51.4380900248386,"food_ins_rate_child":15.1948139903841,"snap":3497353.99337608,"snap_percentage":85.8782230755373,"wic":44014.3367819158,"free_lunch":425649.348029796,"free_breakfast":373538.332051015,"food_banks":1022535.62092832},</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2178,39 +2217,39 @@
       </c>
       <c r="C28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>15.735078635929078</v>
+        <v>20.05682418765441</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.154969745178697</v>
+        <v>47.041204852181551</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3762112.9223805098</v>
+        <v>720695.80300702294</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>88.79386576905317</v>
+        <v>17.009953638508335</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>1163734.6946620722</v>
+        <v>427518.70631584001</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1106183.0172566113</v>
+        <v>799963.30032625922</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>411066.26885374397</v>
+        <v>232814.73879101317</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1226284.5263335789</v>
+        <v>1867520.9378366976</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Forest","population":4236906.33333333,"food_ins_rate":15.7350786359291,"food_ins_rate_child":48.1549697451787,"snap":3762112.92238051,"snap_percentage":88.7938657690532,"wic":1163734.69466207,"free_lunch":1106183.01725661,"free_breakfast":411066.268853744,"food_banks":1226284.52633358},</v>
+        <v xml:space="preserve">    {"county_name":"Forest","population":4236906.33333333,"food_ins_rate":20.0568241876544,"food_ins_rate_child":47.0412048521816,"snap":720695.803007023,"snap_percentage":17.0099536385083,"wic":427518.70631584,"free_lunch":799963.300326259,"free_breakfast":232814.738791013,"food_banks":1867520.9378367},</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2222,39 +2261,39 @@
       </c>
       <c r="C29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>10.92300297761355</v>
+        <v>8.7192100647170978E-2</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>18.098552747692501</v>
+        <v>24.158189775222603</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3621147.3187041939</v>
+        <v>3423833.3299321928</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>82.273459979013964</v>
+        <v>77.790432051737596</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>751288.02079628897</v>
+        <v>292386.26382714976</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1656612.8947708376</v>
+        <v>139836.05000280868</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>415762.06960696215</v>
+        <v>191244.68711819238</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1701492.2758881112</v>
+        <v>1161299.9394038785</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Franklin","population":4401355.33333333,"food_ins_rate":10.9230029776135,"food_ins_rate_child":18.0985527476925,"snap":3621147.31870419,"snap_percentage":82.273459979014,"wic":751288.020796289,"free_lunch":1656612.89477084,"free_breakfast":415762.069606962,"food_banks":1701492.27588811},</v>
+        <v xml:space="preserve">    {"county_name":"Franklin","population":4401355.33333333,"food_ins_rate":0.087192100647171,"food_ins_rate_child":24.1581897752226,"snap":3423833.32993219,"snap_percentage":77.7904320517376,"wic":292386.26382715,"free_lunch":139836.050002809,"free_breakfast":191244.687118192,"food_banks":1161299.93940388},</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2266,39 +2305,39 @@
       </c>
       <c r="C30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>93.284097154077827</v>
+        <v>80.651475298826</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>59.998268473298481</v>
+        <v>13.304370806284505</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3549788.2814060496</v>
+        <v>1670525.604388718</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>77.747271285593527</v>
+        <v>36.587761595318455</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>685315.52831670595</v>
+        <v>839139.9879821965</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>210087.37918328366</v>
+        <v>506955.13066096185</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>420952.14403548522</v>
+        <v>409722.39555227954</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>814515.25782433141</v>
+        <v>1433760.8205880818</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Fulton","population":4565804.33333333,"food_ins_rate":93.2840971540778,"food_ins_rate_child":59.9982684732985,"snap":3549788.28140605,"snap_percentage":77.7472712855935,"wic":685315.528316706,"free_lunch":210087.379183284,"free_breakfast":420952.144035485,"food_banks":814515.257824331},</v>
+        <v xml:space="preserve">    {"county_name":"Fulton","population":4565804.33333333,"food_ins_rate":80.651475298826,"food_ins_rate_child":13.3043708062845,"snap":1670525.60438872,"snap_percentage":36.5877615953185,"wic":839139.987982197,"free_lunch":506955.130660962,"free_breakfast":409722.39555228,"food_banks":1433760.82058808},</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2310,39 +2349,39 @@
       </c>
       <c r="C31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>55.798527846249499</v>
+        <v>11.106545890528963</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2992747942697993</v>
+        <v>2.8232855580284921</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2844166.1438590051</v>
+        <v>475401.67380845587</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>60.127142109210652</v>
+        <v>10.050237065705915</v>
       </c>
       <c r="G31" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>360103.2895744213</v>
+        <v>266409.31473433832</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1062746.930346152</v>
+        <v>1429606.6309363532</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>328206.37120067759</v>
+        <v>7904.5136682769917</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1456049.6073512998</v>
+        <v>655662.5631563043</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Greene","population":4730253.33333333,"food_ins_rate":55.7985278462495,"food_ins_rate_child":0.299274794269799,"snap":2844166.14385901,"snap_percentage":60.1271421092107,"wic":360103.289574421,"free_lunch":1062746.93034615,"free_breakfast":328206.371200678,"food_banks":1456049.6073513},</v>
+        <v xml:space="preserve">    {"county_name":"Greene","population":4730253.33333333,"food_ins_rate":11.106545890529,"food_ins_rate_child":2.82328555802849,"snap":475401.673808456,"snap_percentage":10.0502370657059,"wic":266409.314734338,"free_lunch":1429606.63093635,"free_breakfast":7904.51366827699,"food_banks":655662.563156304},</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2354,39 +2393,39 @@
       </c>
       <c r="C32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>67.661732904240353</v>
+        <v>14.686879799744535</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9.4258848669711899</v>
+        <v>6.5151830168353824</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2056861.7108290733</v>
+        <v>1855969.2949651813</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>42.022202184220149</v>
+        <v>37.917919590857977</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>312344.6019194441</v>
+        <v>98206.261953561232</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>38571.900636973238</v>
+        <v>1032104.9496315263</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>84659.455812591739</v>
+        <v>385392.57583819423</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2068869.8414036324</v>
+        <v>56055.706117421898</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Huntingdon","population":4894702.33333333,"food_ins_rate":67.6617329042404,"food_ins_rate_child":9.42588486697119,"snap":2056861.71082907,"snap_percentage":42.0222021842201,"wic":312344.601919444,"free_lunch":38571.9006369732,"free_breakfast":84659.4558125917,"food_banks":2068869.84140363},</v>
+        <v xml:space="preserve">    {"county_name":"Huntingdon","population":4894702.33333333,"food_ins_rate":14.6868797997445,"food_ins_rate_child":6.51518301683538,"snap":1855969.29496518,"snap_percentage":37.917919590858,"wic":98206.2619535612,"free_lunch":1032104.94963153,"free_breakfast":385392.575838194,"food_banks":56055.7061174219},</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2398,39 +2437,39 @@
       </c>
       <c r="C33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>79.413917789529876</v>
+        <v>84.834962668950524</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>51.816291663023144</v>
+        <v>11.447564472599101</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>58915.100320697471</v>
+        <v>2846433.1880624811</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>1.16452536085494</v>
+        <v>56.263056795872672</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>788825.8900129532</v>
+        <v>4265.5452763885505</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>157876.67975883026</v>
+        <v>345445.37592903827</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>417473.19614127028</v>
+        <v>334495.81259141711</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2298955.1574439444</v>
+        <v>854923.93870175991</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Indiana","population":5059151.33333333,"food_ins_rate":79.4139177895299,"food_ins_rate_child":51.8162916630231,"snap":58915.1003206975,"snap_percentage":1.16452536085494,"wic":788825.890012953,"free_lunch":157876.67975883,"free_breakfast":417473.19614127,"food_banks":2298955.15744394},</v>
+        <v xml:space="preserve">    {"county_name":"Indiana","population":5059151.33333333,"food_ins_rate":84.8349626689505,"food_ins_rate_child":11.4475644725991,"snap":2846433.18806248,"snap_percentage":56.2630567958727,"wic":4265.54527638855,"free_lunch":345445.375929038,"free_breakfast":334495.812591417,"food_banks":854923.93870176},</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2442,39 +2481,39 @@
       </c>
       <c r="C34" s="2">
         <f t="shared" ref="C34:C68" ca="1" si="9">RAND()*100</f>
-        <v>47.249844958505371</v>
+        <v>55.059749152596041</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" ref="D34:D68" ca="1" si="10">RAND()/5*300</f>
-        <v>25.838980334794837</v>
+        <v>17.991779764334673</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" ref="E34:E68" ca="1" si="11">RAND()*$B34</f>
-        <v>1142911.336571052</v>
+        <v>3482071.2543614809</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" ref="F34:F68" ca="1" si="12">$E34/$B34*100</f>
-        <v>21.879762302598049</v>
+        <v>66.660368944028122</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" ref="G34:G68" ca="1" si="13">$B34*0.3*RAND()</f>
-        <v>976289.36164716084</v>
+        <v>1431908.8570525141</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" ref="H34:H68" ca="1" si="14">$B34*0.4*RAND()</f>
-        <v>877746.87376518291</v>
+        <v>72666.455673304939</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" ref="I34:I68" ca="1" si="15">$B34*0.1*RAND()</f>
-        <v>433536.61434181529</v>
+        <v>192708.25997016695</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" ref="J34:J68" ca="1" si="16">$B34*0.5*RAND()</f>
-        <v>1461692.0345559495</v>
+        <v>1675417.3348687429</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Jefferson","population":5223600.33333333,"food_ins_rate":47.2498449585054,"food_ins_rate_child":25.8389803347948,"snap":1142911.33657105,"snap_percentage":21.879762302598,"wic":976289.361647161,"free_lunch":877746.873765183,"free_breakfast":433536.614341815,"food_banks":1461692.03455595},</v>
+        <v xml:space="preserve">    {"county_name":"Jefferson","population":5223600.33333333,"food_ins_rate":55.059749152596,"food_ins_rate_child":17.9917797643347,"snap":3482071.25436148,"snap_percentage":66.6603689440281,"wic":1431908.85705251,"free_lunch":72666.4556733049,"free_breakfast":192708.259970167,"food_banks":1675417.33486874},</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2486,39 +2525,39 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>78.290341283578414</v>
+        <v>63.649099370543041</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>6.7932974420626984</v>
+        <v>29.566790074770275</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2547764.1110030212</v>
+        <v>3385999.6431109076</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>47.285463687965915</v>
+        <v>62.842773583443609</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>237711.93903616772</v>
+        <v>1222356.0542760221</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>641966.15743064799</v>
+        <v>1103425.0618792744</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>199199.17623593981</v>
+        <v>413964.72215132398</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>136325.89788914335</v>
+        <v>2412871.2350605237</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Juniata","population":5388049.33333333,"food_ins_rate":78.2903412835784,"food_ins_rate_child":6.7932974420627,"snap":2547764.11100302,"snap_percentage":47.2854636879659,"wic":237711.939036168,"free_lunch":641966.157430648,"free_breakfast":199199.17623594,"food_banks":136325.897889143},</v>
+        <v xml:space="preserve">    {"county_name":"Juniata","population":5388049.33333333,"food_ins_rate":63.649099370543,"food_ins_rate_child":29.5667900747703,"snap":3385999.64311091,"snap_percentage":62.8427735834436,"wic":1222356.05427602,"free_lunch":1103425.06187927,"free_breakfast":413964.722151324,"food_banks":2412871.23506052},</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2530,39 +2569,39 @@
       </c>
       <c r="C36" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>13.889899334773759</v>
+        <v>34.420698996373375</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>52.012571481805566</v>
+        <v>4.970270309388372</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2085175.160101684</v>
+        <v>988053.77611282864</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>37.553818748287512</v>
+        <v>17.794760426693735</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1178765.7112279162</v>
+        <v>301561.94203527598</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1110582.7275893488</v>
+        <v>1606527.3670250587</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>177793.18037443026</v>
+        <v>5037.0302682048887</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>919608.3788678979</v>
+        <v>514854.1199436966</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lackawanna","population":5552498.33333333,"food_ins_rate":13.8898993347738,"food_ins_rate_child":52.0125714818056,"snap":2085175.16010168,"snap_percentage":37.5538187482875,"wic":1178765.71122792,"free_lunch":1110582.72758935,"free_breakfast":177793.18037443,"food_banks":919608.378867898},</v>
+        <v xml:space="preserve">    {"county_name":"Lackawanna","population":5552498.33333333,"food_ins_rate":34.4206989963734,"food_ins_rate_child":4.97027030938837,"snap":988053.776112829,"snap_percentage":17.7947604266937,"wic":301561.942035276,"free_lunch":1606527.36702506,"free_breakfast":5037.03026820489,"food_banks":514854.119943697},</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2574,39 +2613,39 @@
       </c>
       <c r="C37" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>30.771935891596947</v>
+        <v>66.781170340724998</v>
       </c>
       <c r="D37" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>28.946633053069363</v>
+        <v>5.6615912469312102</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5386071.9134016577</v>
+        <v>5131927.7349409927</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>94.212375930027122</v>
+        <v>89.766923424651608</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>932755.3154786221</v>
+        <v>1143910.0541994791</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1390681.5982289151</v>
+        <v>1214379.7787916136</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>192921.79582494131</v>
+        <v>295686.7722447007</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>854.7973444509156</v>
+        <v>1114006.1588544871</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lancaster","population":5716947.33333333,"food_ins_rate":30.7719358915969,"food_ins_rate_child":28.9466330530694,"snap":5386071.91340166,"snap_percentage":94.2123759300271,"wic":932755.315478622,"free_lunch":1390681.59822892,"free_breakfast":192921.795824941,"food_banks":854.797344450916},</v>
+        <v xml:space="preserve">    {"county_name":"Lancaster","population":5716947.33333333,"food_ins_rate":66.781170340725,"food_ins_rate_child":5.66159124693121,"snap":5131927.73494099,"snap_percentage":89.7669234246516,"wic":1143910.05419948,"free_lunch":1214379.77879161,"free_breakfast":295686.772244701,"food_banks":1114006.15885449},</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2618,39 +2657,39 @@
       </c>
       <c r="C38" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>21.915197992909096</v>
+        <v>19.863543664751081</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>29.400999002080042</v>
+        <v>11.754745862385745</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2850779.2727837297</v>
+        <v>5539749.0890253698</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>48.471130174082774</v>
+        <v>94.191052176306428</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1477351.9829611713</v>
+        <v>1413680.6234434894</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1174660.6361823336</v>
+        <v>151258.11493518521</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>530674.30604544689</v>
+        <v>385169.03475361288</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1975459.7626708124</v>
+        <v>2387951.4846098917</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lawrence","population":5881396.33333333,"food_ins_rate":21.9151979929091,"food_ins_rate_child":29.40099900208,"snap":2850779.27278373,"snap_percentage":48.4711301740828,"wic":1477351.98296117,"free_lunch":1174660.63618233,"free_breakfast":530674.306045447,"food_banks":1975459.76267081},</v>
+        <v xml:space="preserve">    {"county_name":"Lawrence","population":5881396.33333333,"food_ins_rate":19.8635436647511,"food_ins_rate_child":11.7547458623857,"snap":5539749.08902537,"snap_percentage":94.1910521763064,"wic":1413680.62344349,"free_lunch":151258.114935185,"free_breakfast":385169.034753613,"food_banks":2387951.48460989},</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2662,39 +2701,39 @@
       </c>
       <c r="C39" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>80.712682635675975</v>
+        <v>61.124542564162411</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>18.886361889351424</v>
+        <v>28.573714909367389</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5654914.4137225235</v>
+        <v>5603133.9551276807</v>
       </c>
       <c r="F39" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>93.533891489822992</v>
+        <v>92.677427989022604</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>340066.11218506319</v>
+        <v>704026.85268107103</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1011193.711588194</v>
+        <v>1859366.0158749353</v>
       </c>
       <c r="I39" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>575811.51798375603</v>
+        <v>4775.5598452275426</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1363805.4491557919</v>
+        <v>240057.88545909507</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lebanon","population":6045845.33333333,"food_ins_rate":80.712682635676,"food_ins_rate_child":18.8863618893514,"snap":5654914.41372252,"snap_percentage":93.533891489823,"wic":340066.112185063,"free_lunch":1011193.71158819,"free_breakfast":575811.517983756,"food_banks":1363805.44915579},</v>
+        <v xml:space="preserve">    {"county_name":"Lebanon","population":6045845.33333333,"food_ins_rate":61.1245425641624,"food_ins_rate_child":28.5737149093674,"snap":5603133.95512768,"snap_percentage":92.6774279890226,"wic":704026.852681071,"free_lunch":1859366.01587494,"free_breakfast":4775.55984522754,"food_banks":240057.885459095},</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2706,39 +2745,39 @@
       </c>
       <c r="C40" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>29.707249163733263</v>
+        <v>96.189434253017723</v>
       </c>
       <c r="D40" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>36.213303186113869</v>
+        <v>22.762219439256082</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3286661.2439910793</v>
+        <v>4527964.5149853025</v>
       </c>
       <c r="F40" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>52.922793471319864</v>
+        <v>72.910626645854165</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>407738.6832792497</v>
+        <v>848104.04833907448</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>243395.7918970286</v>
+        <v>1297050.5333524821</v>
       </c>
       <c r="I40" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>64359.691549657975</v>
+        <v>409953.48902855266</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1246721.9224549942</v>
+        <v>997833.8736251134</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lehigh","population":6210294.33333333,"food_ins_rate":29.7072491637333,"food_ins_rate_child":36.2133031861139,"snap":3286661.24399108,"snap_percentage":52.9227934713199,"wic":407738.68327925,"free_lunch":243395.791897029,"free_breakfast":64359.691549658,"food_banks":1246721.92245499},</v>
+        <v xml:space="preserve">    {"county_name":"Lehigh","population":6210294.33333333,"food_ins_rate":96.1894342530177,"food_ins_rate_child":22.7622194392561,"snap":4527964.5149853,"snap_percentage":72.9106266458542,"wic":848104.048339074,"free_lunch":1297050.53335248,"free_breakfast":409953.489028553,"food_banks":997833.873625113},</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2750,39 +2789,39 @@
       </c>
       <c r="C41" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>39.98080788564743</v>
+        <v>57.475782675003416</v>
       </c>
       <c r="D41" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>36.443261975395657</v>
+        <v>0.42299102939695965</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2550545.0850557997</v>
+        <v>223068.92146882814</v>
       </c>
       <c r="F41" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>40.010161220438171</v>
+        <v>3.4992612220543506</v>
       </c>
       <c r="G41" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1846103.3883488667</v>
+        <v>1178564.9897764837</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1490082.1028250454</v>
+        <v>1349260.7057789052</v>
       </c>
       <c r="I41" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>201499.90822631135</v>
+        <v>30789.172427491394</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2088184.9265660006</v>
+        <v>2334204.2674571122</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Luzerne","population":6374743.33333333,"food_ins_rate":39.9808078856474,"food_ins_rate_child":36.4432619753957,"snap":2550545.0850558,"snap_percentage":40.0101612204382,"wic":1846103.38834887,"free_lunch":1490082.10282505,"free_breakfast":201499.908226311,"food_banks":2088184.926566},</v>
+        <v xml:space="preserve">    {"county_name":"Luzerne","population":6374743.33333333,"food_ins_rate":57.4757826750034,"food_ins_rate_child":0.42299102939696,"snap":223068.921468828,"snap_percentage":3.49926122205435,"wic":1178564.98977648,"free_lunch":1349260.70577891,"free_breakfast":30789.1724274914,"food_banks":2334204.26745711},</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2794,39 +2833,39 @@
       </c>
       <c r="C42" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>38.982533869607295</v>
+        <v>69.46503571530242</v>
       </c>
       <c r="D42" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>25.773964731519943</v>
+        <v>8.7273749417300284</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>169414.18485833943</v>
+        <v>6190272.7397357346</v>
       </c>
       <c r="F42" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>2.5907509096307795</v>
+        <v>94.664179063536807</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1303034.3620099106</v>
+        <v>1554948.5997698104</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1687909.5503489012</v>
+        <v>503561.15475332085</v>
       </c>
       <c r="I42" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>431494.32689260092</v>
+        <v>283851.18679363921</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1772574.4998946635</v>
+        <v>645157.35903580231</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lycoming","population":6539192.33333333,"food_ins_rate":38.9825338696073,"food_ins_rate_child":25.7739647315199,"snap":169414.184858339,"snap_percentage":2.59075090963078,"wic":1303034.36200991,"free_lunch":1687909.5503489,"free_breakfast":431494.326892601,"food_banks":1772574.49989466},</v>
+        <v xml:space="preserve">    {"county_name":"Lycoming","population":6539192.33333333,"food_ins_rate":69.4650357153024,"food_ins_rate_child":8.72737494173003,"snap":6190272.73973573,"snap_percentage":94.6641790635368,"wic":1554948.59976981,"free_lunch":503561.154753321,"free_breakfast":283851.186793639,"food_banks":645157.359035802},</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2838,39 +2877,39 @@
       </c>
       <c r="C43" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>46.053677243965041</v>
+        <v>48.024959616675268</v>
       </c>
       <c r="D43" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>9.5998417279545656</v>
+        <v>25.166229780062018</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4161740.4978836258</v>
+        <v>4237370.1625756444</v>
       </c>
       <c r="F43" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>62.081789447620025</v>
+        <v>63.20997726274009</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1026860.7848503704</v>
+        <v>962197.38947925228</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1080871.4999231647</v>
+        <v>1022380.5680689694</v>
       </c>
       <c r="I43" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>196807.03481363037</v>
+        <v>638841.23348843539</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1210885.0195724969</v>
+        <v>703808.96048077557</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"McKean","population":6703641.33333333,"food_ins_rate":46.053677243965,"food_ins_rate_child":9.59984172795457,"snap":4161740.49788363,"snap_percentage":62.08178944762,"wic":1026860.78485037,"free_lunch":1080871.49992316,"free_breakfast":196807.03481363,"food_banks":1210885.0195725},</v>
+        <v xml:space="preserve">    {"county_name":"McKean","population":6703641.33333333,"food_ins_rate":48.0249596166753,"food_ins_rate_child":25.166229780062,"snap":4237370.16257564,"snap_percentage":63.2099772627401,"wic":962197.389479252,"free_lunch":1022380.56806897,"free_breakfast":638841.233488435,"food_banks":703808.960480776},</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2882,39 +2921,39 @@
       </c>
       <c r="C44" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>68.948309810639913</v>
+        <v>20.550816389122083</v>
       </c>
       <c r="D44" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>53.676302447413839</v>
+        <v>39.220201405015253</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4351962.4525134042</v>
+        <v>2324271.211186294</v>
       </c>
       <c r="F44" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>63.364956506057503</v>
+        <v>33.841593490781037</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>806934.50265890977</v>
+        <v>1303428.3467335126</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>359719.28473183251</v>
+        <v>2722616.4040181818</v>
       </c>
       <c r="I44" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>660765.65900765778</v>
+        <v>534785.28877169022</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>591870.42172334983</v>
+        <v>3162234.362006722</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Mercer","population":6868090.33333333,"food_ins_rate":68.9483098106399,"food_ins_rate_child":53.6763024474138,"snap":4351962.4525134,"snap_percentage":63.3649565060575,"wic":806934.50265891,"free_lunch":359719.284731833,"free_breakfast":660765.659007658,"food_banks":591870.42172335},</v>
+        <v xml:space="preserve">    {"county_name":"Mercer","population":6868090.33333333,"food_ins_rate":20.5508163891221,"food_ins_rate_child":39.2202014050153,"snap":2324271.21118629,"snap_percentage":33.841593490781,"wic":1303428.34673351,"free_lunch":2722616.40401818,"free_breakfast":534785.28877169,"food_banks":3162234.36200672},</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2926,39 +2965,39 @@
       </c>
       <c r="C45" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>45.802434367047454</v>
+        <v>3.2814223684058952</v>
       </c>
       <c r="D45" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>23.069370958889422</v>
+        <v>27.290101263109754</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2293761.4839643822</v>
+        <v>2720635.5224772962</v>
       </c>
       <c r="F45" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>32.616404619199898</v>
+        <v>38.686388991552946</v>
       </c>
       <c r="G45" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>165530.62354325815</v>
+        <v>662953.30125279899</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>502395.51805629698</v>
+        <v>2507007.2664569509</v>
       </c>
       <c r="I45" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>408036.64500351436</v>
+        <v>1747.9180062484584</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2174183.3817979321</v>
+        <v>2530616.5802709744</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Mifflin","population":7032539.33333333,"food_ins_rate":45.8024343670475,"food_ins_rate_child":23.0693709588894,"snap":2293761.48396438,"snap_percentage":32.6164046191999,"wic":165530.623543258,"free_lunch":502395.518056297,"free_breakfast":408036.645003514,"food_banks":2174183.38179793},</v>
+        <v xml:space="preserve">    {"county_name":"Mifflin","population":7032539.33333333,"food_ins_rate":3.2814223684059,"food_ins_rate_child":27.2901012631098,"snap":2720635.5224773,"snap_percentage":38.6863889915529,"wic":662953.301252799,"free_lunch":2507007.26645695,"free_breakfast":1747.91800624846,"food_banks":2530616.58027097},</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2970,39 +3009,39 @@
       </c>
       <c r="C46" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>69.649503726190318</v>
+        <v>94.085962216456537</v>
       </c>
       <c r="D46" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>31.079682185076273</v>
+        <v>57.181084415022461</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5587411.7377470797</v>
+        <v>1003121.2459348366</v>
       </c>
       <c r="F46" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>77.635414689622479</v>
+        <v>13.93806964072477</v>
       </c>
       <c r="G46" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2088357.7383850575</v>
+        <v>1335809.7779281323</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2511313.209779006</v>
+        <v>2843910.3665599888</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>312588.29453925946</v>
+        <v>208716.81632158431</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3356087.5074835783</v>
+        <v>847709.01114017272</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Monroe","population":7196988.33333333,"food_ins_rate":69.6495037261903,"food_ins_rate_child":31.0796821850763,"snap":5587411.73774708,"snap_percentage":77.6354146896225,"wic":2088357.73838506,"free_lunch":2511313.20977901,"free_breakfast":312588.294539259,"food_banks":3356087.50748358},</v>
+        <v xml:space="preserve">    {"county_name":"Monroe","population":7196988.33333333,"food_ins_rate":94.0859622164565,"food_ins_rate_child":57.1810844150225,"snap":1003121.24593484,"snap_percentage":13.9380696407248,"wic":1335809.77792813,"free_lunch":2843910.36655999,"free_breakfast":208716.816321584,"food_banks":847709.011140173},</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -3014,39 +3053,39 @@
       </c>
       <c r="C47" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>59.117869572441492</v>
+        <v>10.383189357405575</v>
       </c>
       <c r="D47" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>33.400300449448672</v>
+        <v>38.493281887635426</v>
       </c>
       <c r="E47" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2204133.1330428557</v>
+        <v>3403038.6807030607</v>
       </c>
       <c r="F47" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>29.941613753367413</v>
+        <v>46.227910754517445</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1113706.518955719</v>
+        <v>972497.54982456064</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>447457.60510158766</v>
+        <v>2665611.7778034159</v>
       </c>
       <c r="I47" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>262196.6965800281</v>
+        <v>8183.8722165670533</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>533938.50567974511</v>
+        <v>960953.68848289014</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Montgomery","population":7361437.33333333,"food_ins_rate":59.1178695724415,"food_ins_rate_child":33.4003004494487,"snap":2204133.13304286,"snap_percentage":29.9416137533674,"wic":1113706.51895572,"free_lunch":447457.605101588,"free_breakfast":262196.696580028,"food_banks":533938.505679745},</v>
+        <v xml:space="preserve">    {"county_name":"Montgomery","population":7361437.33333333,"food_ins_rate":10.3831893574056,"food_ins_rate_child":38.4932818876354,"snap":3403038.68070306,"snap_percentage":46.2279107545174,"wic":972497.549824561,"free_lunch":2665611.77780342,"free_breakfast":8183.87221656705,"food_banks":960953.68848289},</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -3058,39 +3097,39 @@
       </c>
       <c r="C48" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>34.549602478416041</v>
+        <v>9.9569548510615391</v>
       </c>
       <c r="D48" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>37.381856708371252</v>
+        <v>8.121304876960842</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3153911.1840765309</v>
+        <v>4664953.7043175874</v>
       </c>
       <c r="F48" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>41.9075049022115</v>
+        <v>61.985439291791799</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>918383.86164164566</v>
+        <v>1865656.5557115865</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2117491.0176344682</v>
+        <v>615602.33965402551</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>33461.001983088674</v>
+        <v>613373.42102164601</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>832571.04357281537</v>
+        <v>629778.98156608967</v>
       </c>
       <c r="L48" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Montour","population":7525886.33333333,"food_ins_rate":34.549602478416,"food_ins_rate_child":37.3818567083713,"snap":3153911.18407653,"snap_percentage":41.9075049022115,"wic":918383.861641646,"free_lunch":2117491.01763447,"free_breakfast":33461.0019830886,"food_banks":832571.043572815},</v>
+        <v xml:space="preserve">    {"county_name":"Montour","population":7525886.33333333,"food_ins_rate":9.95695485106154,"food_ins_rate_child":8.12130487696084,"snap":4664953.70431759,"snap_percentage":61.9854392917918,"wic":1865656.55571159,"free_lunch":615602.339654026,"free_breakfast":613373.421021646,"food_banks":629778.98156609},</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3102,39 +3141,39 @@
       </c>
       <c r="C49" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>24.468188963460811</v>
+        <v>59.372740463642515</v>
       </c>
       <c r="D49" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>50.820283653918061</v>
+        <v>12.730978144935225</v>
       </c>
       <c r="E49" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>8487.808821636454</v>
+        <v>5708108.0876432918</v>
       </c>
       <c r="F49" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0.11036981423744319</v>
+        <v>74.224436779782749</v>
       </c>
       <c r="G49" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>924993.72067320347</v>
+        <v>719518.67424157902</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>368695.33822200203</v>
+        <v>2161568.6364618968</v>
       </c>
       <c r="I49" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>475376.02794426907</v>
+        <v>727278.99711729342</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2992757.9690710478</v>
+        <v>1832919.5863351703</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Northampton","population":7690335.33333333,"food_ins_rate":24.4681889634608,"food_ins_rate_child":50.8202836539181,"snap":8487.80882163645,"snap_percentage":0.110369814237443,"wic":924993.720673203,"free_lunch":368695.338222002,"free_breakfast":475376.027944269,"food_banks":2992757.96907105},</v>
+        <v xml:space="preserve">    {"county_name":"Northampton","population":7690335.33333333,"food_ins_rate":59.3727404636425,"food_ins_rate_child":12.7309781449352,"snap":5708108.08764329,"snap_percentage":74.2244367797827,"wic":719518.674241579,"free_lunch":2161568.6364619,"free_breakfast":727278.997117293,"food_banks":1832919.58633517},</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3146,39 +3185,39 @@
       </c>
       <c r="C50" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>49.487063357453678</v>
+        <v>41.329995279532163</v>
       </c>
       <c r="D50" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>9.796454790909646</v>
+        <v>42.408357442591388</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>6010971.806173211</v>
+        <v>4768648.0792382509</v>
       </c>
       <c r="F50" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>76.526248857838951</v>
+        <v>60.710108347616242</v>
       </c>
       <c r="G50" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1385895.3960565964</v>
+        <v>2140356.704671572</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2139155.154569272</v>
+        <v>1442084.7911914014</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>556066.09304069087</v>
+        <v>549409.61369316012</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3377248.0797209698</v>
+        <v>1695651.9896081046</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Northumberland","population":7854784.33333333,"food_ins_rate":49.4870633574537,"food_ins_rate_child":9.79645479090965,"snap":6010971.80617321,"snap_percentage":76.526248857839,"wic":1385895.3960566,"free_lunch":2139155.15456927,"free_breakfast":556066.093040691,"food_banks":3377248.07972097},</v>
+        <v xml:space="preserve">    {"county_name":"Northumberland","population":7854784.33333333,"food_ins_rate":41.3299952795322,"food_ins_rate_child":42.4083574425914,"snap":4768648.07923825,"snap_percentage":60.7101083476162,"wic":2140356.70467157,"free_lunch":1442084.7911914,"free_breakfast":549409.61369316,"food_banks":1695651.9896081},</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3190,39 +3229,39 @@
       </c>
       <c r="C51" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>18.549142343799339</v>
+        <v>54.025892940211996</v>
       </c>
       <c r="D51" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>54.277978046053157</v>
+        <v>1.0772665724561237</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3712383.1323365499</v>
+        <v>5383281.3524088375</v>
       </c>
       <c r="F51" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>46.293491884135449</v>
+        <v>67.129626095705405</v>
       </c>
       <c r="G51" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>891030.71229618369</v>
+        <v>2402308.2472634921</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1309382.3524922747</v>
+        <v>2004504.1642911229</v>
       </c>
       <c r="I51" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>681126.8636103234</v>
+        <v>91557.264201568454</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3811846.6617861111</v>
+        <v>2896447.9924099618</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Perry","population":8019233.33333333,"food_ins_rate":18.5491423437993,"food_ins_rate_child":54.2779780460532,"snap":3712383.13233655,"snap_percentage":46.2934918841354,"wic":891030.712296184,"free_lunch":1309382.35249227,"free_breakfast":681126.863610323,"food_banks":3811846.66178611},</v>
+        <v xml:space="preserve">    {"county_name":"Perry","population":8019233.33333333,"food_ins_rate":54.025892940212,"food_ins_rate_child":1.07726657245612,"snap":5383281.35240884,"snap_percentage":67.1296260957054,"wic":2402308.24726349,"free_lunch":2004504.16429112,"free_breakfast":91557.2642015685,"food_banks":2896447.99240996},</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3234,39 +3273,39 @@
       </c>
       <c r="C52" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>34.018377421971543</v>
+        <v>93.125361953822676</v>
       </c>
       <c r="D52" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>56.021661592662802</v>
+        <v>33.795459326040586</v>
       </c>
       <c r="E52" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>724248.43924221303</v>
+        <v>439160.48490264826</v>
       </c>
       <c r="F52" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>8.8499089986941897</v>
+        <v>5.3662943772130989</v>
       </c>
       <c r="G52" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>599508.78341070504</v>
+        <v>1149807.1214485238</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3132751.7517405408</v>
+        <v>1535041.0763809416</v>
       </c>
       <c r="I52" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>246443.43889821981</v>
+        <v>770963.12371124176</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1109727.4063324314</v>
+        <v>1490462.8298619576</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Philadelphia","population":8183682.33333333,"food_ins_rate":34.0183774219715,"food_ins_rate_child":56.0216615926628,"snap":724248.439242213,"snap_percentage":8.84990899869419,"wic":599508.783410705,"free_lunch":3132751.75174054,"free_breakfast":246443.43889822,"food_banks":1109727.40633243},</v>
+        <v xml:space="preserve">    {"county_name":"Philadelphia","population":8183682.33333333,"food_ins_rate":93.1253619538227,"food_ins_rate_child":33.7954593260406,"snap":439160.484902648,"snap_percentage":5.3662943772131,"wic":1149807.12144852,"free_lunch":1535041.07638094,"free_breakfast":770963.123711242,"food_banks":1490462.82986196},</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3278,39 +3317,39 @@
       </c>
       <c r="C53" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>35.988934471145441</v>
+        <v>55.881442389923706</v>
       </c>
       <c r="D53" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>27.613015145044102</v>
+        <v>33.113354877336427</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2270970.8609426836</v>
+        <v>1195045.6988237679</v>
       </c>
       <c r="F53" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>27.203343721665028</v>
+        <v>14.315128153914625</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1902441.3192301653</v>
+        <v>269526.56582912261</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2980056.9551764354</v>
+        <v>2910203.8821488703</v>
       </c>
       <c r="I53" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>35812.319645756281</v>
+        <v>699248.96099625225</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>457399.24093569419</v>
+        <v>947805.52716013289</v>
       </c>
       <c r="L53" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Pike","population":8348131.33333333,"food_ins_rate":35.9889344711454,"food_ins_rate_child":27.6130151450441,"snap":2270970.86094268,"snap_percentage":27.203343721665,"wic":1902441.31923017,"free_lunch":2980056.95517644,"free_breakfast":35812.3196457563,"food_banks":457399.240935694},</v>
+        <v xml:space="preserve">    {"county_name":"Pike","population":8348131.33333333,"food_ins_rate":55.8814423899237,"food_ins_rate_child":33.1133548773364,"snap":1195045.69882377,"snap_percentage":14.3151281539146,"wic":269526.565829123,"free_lunch":2910203.88214887,"free_breakfast":699248.960996252,"food_banks":947805.527160133},</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3322,39 +3361,39 @@
       </c>
       <c r="C54" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>71.573950519931316</v>
+        <v>40.223069329853935</v>
       </c>
       <c r="D54" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>15.355592977159688</v>
+        <v>52.730236363878007</v>
       </c>
       <c r="E54" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1897893.0168622923</v>
+        <v>5792031.2715049786</v>
       </c>
       <c r="F54" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>22.295155435192481</v>
+        <v>68.040841257317723</v>
       </c>
       <c r="G54" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>353528.87635373179</v>
+        <v>35561.707649740943</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2132460.7785708555</v>
+        <v>2332486.6759848092</v>
       </c>
       <c r="I54" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>76171.621462040086</v>
+        <v>498522.52159848413</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3663440.4542142153</v>
+        <v>359208.59008803213</v>
       </c>
       <c r="L54" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Potter","population":8512580.33333333,"food_ins_rate":71.5739505199313,"food_ins_rate_child":15.3555929771597,"snap":1897893.01686229,"snap_percentage":22.2951554351925,"wic":353528.876353732,"free_lunch":2132460.77857086,"free_breakfast":76171.6214620401,"food_banks":3663440.45421422},</v>
+        <v xml:space="preserve">    {"county_name":"Potter","population":8512580.33333333,"food_ins_rate":40.2230693298539,"food_ins_rate_child":52.730236363878,"snap":5792031.27150498,"snap_percentage":68.0408412573177,"wic":35561.7076497409,"free_lunch":2332486.67598481,"free_breakfast":498522.521598484,"food_banks":359208.590088032},</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3366,39 +3405,39 @@
       </c>
       <c r="C55" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>51.751836502032823</v>
+        <v>22.17679149609809</v>
       </c>
       <c r="D55" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>39.154107384347249</v>
+        <v>11.99060480433412</v>
       </c>
       <c r="E55" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4404089.9431145322</v>
+        <v>358915.11725658074</v>
       </c>
       <c r="F55" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>50.755734179622458</v>
+        <v>4.1363824353778167</v>
       </c>
       <c r="G55" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1139732.9950009522</v>
+        <v>404045.47030139907</v>
       </c>
       <c r="H55" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1862827.9230418692</v>
+        <v>1641650.1247649728</v>
       </c>
       <c r="I55" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>301109.43759135029</v>
+        <v>584466.83360217733</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3235632.4223474907</v>
+        <v>852171.38637713634</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Schuylkill","population":8677029.33333333,"food_ins_rate":51.7518365020328,"food_ins_rate_child":39.1541073843472,"snap":4404089.94311453,"snap_percentage":50.7557341796225,"wic":1139732.99500095,"free_lunch":1862827.92304187,"free_breakfast":301109.43759135,"food_banks":3235632.42234749},</v>
+        <v xml:space="preserve">    {"county_name":"Schuylkill","population":8677029.33333333,"food_ins_rate":22.1767914960981,"food_ins_rate_child":11.9906048043341,"snap":358915.117256581,"snap_percentage":4.13638243537782,"wic":404045.470301399,"free_lunch":1641650.12476497,"free_breakfast":584466.833602177,"food_banks":852171.386377136},</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3410,39 +3449,39 @@
       </c>
       <c r="C56" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>63.673972262507448</v>
+        <v>28.463980126071952</v>
       </c>
       <c r="D56" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>53.256436595960579</v>
+        <v>33.951642378789046</v>
       </c>
       <c r="E56" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1926060.9613577181</v>
+        <v>2014139.960592675</v>
       </c>
       <c r="F56" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>21.784376873901955</v>
+        <v>22.780579046369986</v>
       </c>
       <c r="G56" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1249378.9504690357</v>
+        <v>1078695.8724877089</v>
       </c>
       <c r="H56" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1225599.9102093566</v>
+        <v>3329319.4196541491</v>
       </c>
       <c r="I56" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>196386.05319491684</v>
+        <v>50451.968550907273</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1089038.1375357541</v>
+        <v>2023189.1536129799</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Snyder","population":8841478.33333333,"food_ins_rate":63.6739722625074,"food_ins_rate_child":53.2564365959606,"snap":1926060.96135772,"snap_percentage":21.784376873902,"wic":1249378.95046904,"free_lunch":1225599.91020936,"free_breakfast":196386.053194917,"food_banks":1089038.13753575},</v>
+        <v xml:space="preserve">    {"county_name":"Snyder","population":8841478.33333333,"food_ins_rate":28.463980126072,"food_ins_rate_child":33.951642378789,"snap":2014139.96059268,"snap_percentage":22.78057904637,"wic":1078695.87248771,"free_lunch":3329319.41965415,"free_breakfast":50451.9685509073,"food_banks":2023189.15361298},</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3454,39 +3493,39 @@
       </c>
       <c r="C57" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>59.552995694285492</v>
+        <v>44.813689156181184</v>
       </c>
       <c r="D57" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>30.91325892603717</v>
+        <v>57.938626918174577</v>
       </c>
       <c r="E57" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4082167.3274963391</v>
+        <v>3710983.7266886816</v>
       </c>
       <c r="F57" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>45.327562353153269</v>
+        <v>41.206014542814984</v>
       </c>
       <c r="G57" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2372289.4252800755</v>
+        <v>2442726.1339120092</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>185002.81602479628</v>
+        <v>3026976.4085473414</v>
       </c>
       <c r="I57" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>871943.01037191739</v>
+        <v>287.70453553532417</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3867778.1109044603</v>
+        <v>122504.52684971396</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Somerset","population":9005927.33333333,"food_ins_rate":59.5529956942855,"food_ins_rate_child":30.9132589260372,"snap":4082167.32749634,"snap_percentage":45.3275623531533,"wic":2372289.42528008,"free_lunch":185002.816024796,"free_breakfast":871943.010371917,"food_banks":3867778.11090446},</v>
+        <v xml:space="preserve">    {"county_name":"Somerset","population":9005927.33333333,"food_ins_rate":44.8136891561812,"food_ins_rate_child":57.9386269181746,"snap":3710983.72668868,"snap_percentage":41.206014542815,"wic":2442726.13391201,"free_lunch":3026976.40854734,"free_breakfast":287.704535535324,"food_banks":122504.526849714},</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3498,39 +3537,39 @@
       </c>
       <c r="C58" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>17.207364811169889</v>
+        <v>76.288874764110261</v>
       </c>
       <c r="D58" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>2.0057938331618708</v>
+        <v>49.993703063562855</v>
       </c>
       <c r="E58" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>701550.62813754554</v>
+        <v>6472153.422805693</v>
       </c>
       <c r="F58" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>7.6501836199184599</v>
+        <v>70.576748298541602</v>
       </c>
       <c r="G58" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>808183.05865864141</v>
+        <v>1185505.015177306</v>
       </c>
       <c r="H58" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>839774.29612293118</v>
+        <v>2972753.1486685816</v>
       </c>
       <c r="I58" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>832435.92029221146</v>
+        <v>98974.303003886773</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1311824.6023803828</v>
+        <v>3779719.0266723889</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Sullivan","population":9170376.33333333,"food_ins_rate":17.2073648111699,"food_ins_rate_child":2.00579383316187,"snap":701550.628137546,"snap_percentage":7.65018361991846,"wic":808183.058658641,"free_lunch":839774.296122931,"free_breakfast":832435.920292211,"food_banks":1311824.60238038},</v>
+        <v xml:space="preserve">    {"county_name":"Sullivan","population":9170376.33333333,"food_ins_rate":76.2888747641103,"food_ins_rate_child":49.9937030635629,"snap":6472153.42280569,"snap_percentage":70.5767482985416,"wic":1185505.01517731,"free_lunch":2972753.14866858,"free_breakfast":98974.3030038868,"food_banks":3779719.02667239},</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3542,39 +3581,39 @@
       </c>
       <c r="C59" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>9.174221090262936</v>
+        <v>74.379411174411132</v>
       </c>
       <c r="D59" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>53.647127915941539</v>
+        <v>39.116388225653424</v>
       </c>
       <c r="E59" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>9282498.3057895135</v>
+        <v>7489843.2215907387</v>
       </c>
       <c r="F59" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>99.439442885375001</v>
+        <v>80.235494014500489</v>
       </c>
       <c r="G59" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2586268.366989038</v>
+        <v>1079023.614261793</v>
       </c>
       <c r="H59" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>553871.58888175117</v>
+        <v>3096797.6617940888</v>
       </c>
       <c r="I59" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>424735.56466532068</v>
+        <v>369500.47950371943</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2149554.7685056329</v>
+        <v>4551014.1128483657</v>
       </c>
       <c r="L59" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Susquehanna","population":9334825.33333333,"food_ins_rate":9.17422109026294,"food_ins_rate_child":53.6471279159415,"snap":9282498.30578951,"snap_percentage":99.439442885375,"wic":2586268.36698904,"free_lunch":553871.588881751,"free_breakfast":424735.564665321,"food_banks":2149554.76850563},</v>
+        <v xml:space="preserve">    {"county_name":"Susquehanna","population":9334825.33333333,"food_ins_rate":74.3794111744111,"food_ins_rate_child":39.1163882256534,"snap":7489843.22159074,"snap_percentage":80.2354940145005,"wic":1079023.61426179,"free_lunch":3096797.66179409,"free_breakfast":369500.479503719,"food_banks":4551014.11284837},</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3586,39 +3625,39 @@
       </c>
       <c r="C60" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>43.62305694217936</v>
+        <v>75.946479343870521</v>
       </c>
       <c r="D60" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>43.565596514531322</v>
+        <v>43.358152991691945</v>
       </c>
       <c r="E60" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4744137.5608758293</v>
+        <v>7057559.2496937877</v>
       </c>
       <c r="F60" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>49.942104990361869</v>
+        <v>74.295772519470589</v>
       </c>
       <c r="G60" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1897018.3193300553</v>
+        <v>1774110.0975894216</v>
       </c>
       <c r="H60" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2140673.4513300089</v>
+        <v>3743832.8544846936</v>
       </c>
       <c r="I60" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>637654.83487912163</v>
+        <v>683296.28896097501</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>4066547.1381431092</v>
+        <v>4316169.7692294577</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Tioga","population":9499274.33333333,"food_ins_rate":43.6230569421794,"food_ins_rate_child":43.5655965145313,"snap":4744137.56087583,"snap_percentage":49.9421049903619,"wic":1897018.31933006,"free_lunch":2140673.45133001,"free_breakfast":637654.834879122,"food_banks":4066547.13814311},</v>
+        <v xml:space="preserve">    {"county_name":"Tioga","population":9499274.33333333,"food_ins_rate":75.9464793438705,"food_ins_rate_child":43.3581529916919,"snap":7057559.24969379,"snap_percentage":74.2957725194706,"wic":1774110.09758942,"free_lunch":3743832.85448469,"free_breakfast":683296.288960975,"food_banks":4316169.76922946},</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3630,39 +3669,39 @@
       </c>
       <c r="C61" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>37.389950095348468</v>
+        <v>28.086674051838944</v>
       </c>
       <c r="D61" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>43.534976200337091</v>
+        <v>32.820185378194822</v>
       </c>
       <c r="E61" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>7373248.2469005976</v>
+        <v>4534367.7453341335</v>
       </c>
       <c r="F61" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>76.298213354969107</v>
+        <v>46.921539337675597</v>
       </c>
       <c r="G61" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1037914.5718864286</v>
+        <v>1673653.9478234197</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>374935.86135313037</v>
+        <v>2177316.6178183355</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>912487.68792306376</v>
+        <v>68757.922882404906</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1442020.3910032723</v>
+        <v>577095.56621781993</v>
       </c>
       <c r="L61" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Union","population":9663723.33333333,"food_ins_rate":37.3899500953485,"food_ins_rate_child":43.5349762003371,"snap":7373248.2469006,"snap_percentage":76.2982133549691,"wic":1037914.57188643,"free_lunch":374935.86135313,"free_breakfast":912487.687923064,"food_banks":1442020.39100327},</v>
+        <v xml:space="preserve">    {"county_name":"Union","population":9663723.33333333,"food_ins_rate":28.0866740518389,"food_ins_rate_child":32.8201853781948,"snap":4534367.74533413,"snap_percentage":46.9215393376756,"wic":1673653.94782342,"free_lunch":2177316.61781834,"free_breakfast":68757.9228824049,"food_banks":577095.56621782},</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3674,39 +3713,39 @@
       </c>
       <c r="C62" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>3.461034272421204</v>
+        <v>57.200120112866259</v>
       </c>
       <c r="D62" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>55.905993508175847</v>
+        <v>54.939211195095645</v>
       </c>
       <c r="E62" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5380717.8397102524</v>
+        <v>3841303.1940189116</v>
       </c>
       <c r="F62" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>54.747898767108047</v>
+        <v>39.084613738311326</v>
       </c>
       <c r="G62" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2631080.6886843997</v>
+        <v>2445762.7199229058</v>
       </c>
       <c r="H62" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2814311.348093146</v>
+        <v>311652.8585545462</v>
       </c>
       <c r="I62" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>411039.26004875009</v>
+        <v>531842.41971454991</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>511304.36608822009</v>
+        <v>976227.87758321967</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Venango","population":9828172.33333333,"food_ins_rate":3.4610342724212,"food_ins_rate_child":55.9059935081758,"snap":5380717.83971025,"snap_percentage":54.747898767108,"wic":2631080.6886844,"free_lunch":2814311.34809315,"free_breakfast":411039.26004875,"food_banks":511304.36608822},</v>
+        <v xml:space="preserve">    {"county_name":"Venango","population":9828172.33333333,"food_ins_rate":57.2001201128663,"food_ins_rate_child":54.9392111950956,"snap":3841303.19401891,"snap_percentage":39.0846137383113,"wic":2445762.71992291,"free_lunch":311652.858554546,"free_breakfast":531842.41971455,"food_banks":976227.87758322},</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3718,39 +3757,39 @@
       </c>
       <c r="C63" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>63.070544866351128</v>
+        <v>81.99617897321022</v>
       </c>
       <c r="D63" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>9.6625808745547452</v>
+        <v>9.9895453980221163</v>
       </c>
       <c r="E63" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>9716720.7895102706</v>
+        <v>7637908.7929871734</v>
       </c>
       <c r="F63" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>97.238957280381356</v>
+        <v>76.435487127973929</v>
       </c>
       <c r="G63" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2971806.1324918023</v>
+        <v>116830.6532663945</v>
       </c>
       <c r="H63" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>91242.140172775573</v>
+        <v>1363699.8665837566</v>
       </c>
       <c r="I63" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>245946.25524226381</v>
+        <v>742364.9282946795</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3122346.9498273246</v>
+        <v>415123.7727597105</v>
       </c>
       <c r="L63" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Warren","population":9992621.33333333,"food_ins_rate":63.0705448663511,"food_ins_rate_child":9.66258087455475,"snap":9716720.78951027,"snap_percentage":97.2389572803814,"wic":2971806.1324918,"free_lunch":91242.1401727756,"free_breakfast":245946.255242264,"food_banks":3122346.94982732},</v>
+        <v xml:space="preserve">    {"county_name":"Warren","population":9992621.33333333,"food_ins_rate":81.9961789732102,"food_ins_rate_child":9.98954539802212,"snap":7637908.79298717,"snap_percentage":76.4354871279739,"wic":116830.653266394,"free_lunch":1363699.86658376,"free_breakfast":742364.928294679,"food_banks":415123.77275971},</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3762,39 +3801,39 @@
       </c>
       <c r="C64" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>74.224468656615784</v>
+        <v>7.0422167714005663</v>
       </c>
       <c r="D64" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>31.418377728082017</v>
+        <v>15.477019133299645</v>
       </c>
       <c r="E64" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4935763.2975500748</v>
+        <v>4949471.316586229</v>
       </c>
       <c r="F64" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>48.594359747140579</v>
+        <v>48.729320110574982</v>
       </c>
       <c r="G64" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2333846.285611399</v>
+        <v>1991886.1178664085</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3926211.7814918277</v>
+        <v>1464897.7751045206</v>
       </c>
       <c r="I64" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>31304.334046284162</v>
+        <v>957675.99894861667</v>
       </c>
       <c r="J64" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2926618.4892796576</v>
+        <v>4772998.1019045915</v>
       </c>
       <c r="L64" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Washington","population":10157070.3333333,"food_ins_rate":74.2244686566158,"food_ins_rate_child":31.418377728082,"snap":4935763.29755007,"snap_percentage":48.5943597471406,"wic":2333846.2856114,"free_lunch":3926211.78149183,"free_breakfast":31304.3340462842,"food_banks":2926618.48927966},</v>
+        <v xml:space="preserve">    {"county_name":"Washington","population":10157070.3333333,"food_ins_rate":7.04221677140057,"food_ins_rate_child":15.4770191332996,"snap":4949471.31658623,"snap_percentage":48.729320110575,"wic":1991886.11786641,"free_lunch":1464897.77510452,"free_breakfast":957675.998948617,"food_banks":4772998.10190459},</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3806,39 +3845,39 @@
       </c>
       <c r="C65" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>70.23641817088577</v>
+        <v>3.1129384217432499</v>
       </c>
       <c r="D65" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>38.320264605696472</v>
+        <v>34.715360139856784</v>
       </c>
       <c r="E65" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3253800.0509319976</v>
+        <v>1586278.1799094435</v>
       </c>
       <c r="F65" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>31.524429164453196</v>
+        <v>15.36864998921782</v>
       </c>
       <c r="G65" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>783816.83761372638</v>
+        <v>3043440.5071311458</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>974349.94440446678</v>
+        <v>61142.272681937437</v>
       </c>
       <c r="I65" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>349084.94687337248</v>
+        <v>268216.96419205109</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>693840.74512404448</v>
+        <v>2897527.0156096602</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Wayne","population":10321519.3333333,"food_ins_rate":70.2364181708858,"food_ins_rate_child":38.3202646056965,"snap":3253800.050932,"snap_percentage":31.5244291644532,"wic":783816.837613726,"free_lunch":974349.944404467,"free_breakfast":349084.946873372,"food_banks":693840.745124044},</v>
+        <v xml:space="preserve">    {"county_name":"Wayne","population":10321519.3333333,"food_ins_rate":3.11293842174325,"food_ins_rate_child":34.7153601398568,"snap":1586278.17990944,"snap_percentage":15.3686499892178,"wic":3043440.50713115,"free_lunch":61142.2726819374,"free_breakfast":268216.964192051,"food_banks":2897527.01560966},</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3850,39 +3889,39 @@
       </c>
       <c r="C66" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>65.216886207137449</v>
+        <v>94.279541178793352</v>
       </c>
       <c r="D66" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>54.493048144106048</v>
+        <v>25.58818807841299</v>
       </c>
       <c r="E66" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4734638.693516328</v>
+        <v>456178.04103445617</v>
       </c>
       <c r="F66" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>45.152136102353381</v>
+        <v>4.3503663804165367</v>
       </c>
       <c r="G66" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2711582.28507081</v>
+        <v>1955473.4523287117</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3982016.7330462127</v>
+        <v>2546118.6278750505</v>
       </c>
       <c r="I66" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>312988.32762537815</v>
+        <v>890254.75150695536</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>105131.77067995266</v>
+        <v>3913695.6767583173</v>
       </c>
       <c r="L66" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Westmoreland","population":10485968.3333333,"food_ins_rate":65.2168862071374,"food_ins_rate_child":54.493048144106,"snap":4734638.69351633,"snap_percentage":45.1521361023534,"wic":2711582.28507081,"free_lunch":3982016.73304621,"free_breakfast":312988.327625378,"food_banks":105131.770679953},</v>
+        <v xml:space="preserve">    {"county_name":"Westmoreland","population":10485968.3333333,"food_ins_rate":94.2795411787934,"food_ins_rate_child":25.588188078413,"snap":456178.041034456,"snap_percentage":4.35036638041654,"wic":1955473.45232871,"free_lunch":2546118.62787505,"free_breakfast":890254.751506955,"food_banks":3913695.67675832},</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3894,39 +3933,39 @@
       </c>
       <c r="C67" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>25.606008968966243</v>
+        <v>75.766840099682739</v>
       </c>
       <c r="D67" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>47.88747509716579</v>
+        <v>35.080024423154981</v>
       </c>
       <c r="E67" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>9029573.4652613942</v>
+        <v>605024.30575401813</v>
       </c>
       <c r="F67" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>84.781405109835035</v>
+        <v>5.680756789317865</v>
       </c>
       <c r="G67" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2913871.301698328</v>
+        <v>710114.26924511581</v>
       </c>
       <c r="H67" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>127895.53806533302</v>
+        <v>129531.85601927016</v>
       </c>
       <c r="I67" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>101519.82746147062</v>
+        <v>55000.812616852745</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2289452.697852971</v>
+        <v>24432.553347320903</v>
       </c>
       <c r="L67" t="str">
         <f t="shared" ref="L67:L68" ca="1" si="17">CONCATENATE("    {""",$A$1,""":""",$A67,""",""",$B$1,""":",$B67,",""",$C$1,""":",$C67,",""",$D$1,""":",$D67,",""",$E$1,""":",$E67,",""",$F$1,""":",$F67,",""",$G$1,""":",$G67,",""",$H$1,""":",$H67,",""",$I$1,""":",$I67,",""",$J$1,""":",$J67,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Wyoming","population":10650417.3333333,"food_ins_rate":25.6060089689662,"food_ins_rate_child":47.8874750971658,"snap":9029573.46526139,"snap_percentage":84.781405109835,"wic":2913871.30169833,"free_lunch":127895.538065333,"free_breakfast":101519.827461471,"food_banks":2289452.69785297},</v>
+        <v xml:space="preserve">    {"county_name":"Wyoming","population":10650417.3333333,"food_ins_rate":75.7668400996827,"food_ins_rate_child":35.080024423155,"snap":605024.305754018,"snap_percentage":5.68075678931786,"wic":710114.269245116,"free_lunch":129531.85601927,"free_breakfast":55000.8126168527,"food_banks":24432.5533473209},</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -3938,39 +3977,39 @@
       </c>
       <c r="C68" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>50.426734837840968</v>
+        <v>90.754414281962795</v>
       </c>
       <c r="D68" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>3.1720009732246779</v>
+        <v>30.344968633205681</v>
       </c>
       <c r="E68" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>869451.96189402766</v>
+        <v>4453011.2069274187</v>
       </c>
       <c r="F68" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>8.0394147749586651</v>
+        <v>41.174907480848496</v>
       </c>
       <c r="G68" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1392620.3494496003</v>
+        <v>1968936.4433793824</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3369904.4465737804</v>
+        <v>3424998.2476301272</v>
       </c>
       <c r="I68" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>118553.54604796803</v>
+        <v>174186.09697669206</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1503905.6000827565</v>
+        <v>1281090.3470434612</v>
       </c>
       <c r="L68" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v xml:space="preserve">    {"county_name":"York","population":10814866.3333333,"food_ins_rate":50.426734837841,"food_ins_rate_child":3.17200097322468,"snap":869451.961894028,"snap_percentage":8.03941477495867,"wic":1392620.3494496,"free_lunch":3369904.44657378,"free_breakfast":118553.546047968,"food_banks":1503905.60008276},</v>
+        <v xml:space="preserve">    {"county_name":"York","population":10814866.3333333,"food_ins_rate":90.7544142819628,"food_ins_rate_child":30.3449686332057,"snap":4453011.20692742,"snap_percentage":41.1749074808485,"wic":1968936.44337938,"free_lunch":3424998.24763013,"free_breakfast":174186.096976692,"food_banks":1281090.34704346},</v>
       </c>
     </row>
   </sheetData>
@@ -3992,7 +4031,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4000,18 +4039,18 @@
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.33203125" customWidth="1"/>
-    <col min="5" max="5" width="124" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="127.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>78</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4019,11 +4058,14 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("    {""",$A$1,""":""",$A2,""",""",$B$1,""":",$B2,",""",$C$1,""":",$C2,"},")</f>
-        <v xml:space="preserve">    {"field name":"county_name","class":demographic_data_header,"description":},</v>
+        <f>CONCATENATE("    {""",$A$1,""":""",$A2,""",""",$B$1,""":""",$B2,""",""",$C$1,""":""",$C2,"""},")</f>
+        <v xml:space="preserve">    {"name":"county_name","class":"header","description":"County"},</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4031,14 +4073,14 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E11" si="0">CONCATENATE("    {""",$A$1,""":""",$A3,""",""",$B$1,""":",$B3,",""",$C$1,""":",$C3,"},")</f>
-        <v xml:space="preserve">    {"field name":"population","class":demographic_data_primary,"description":Total population},</v>
+        <f t="shared" ref="E3:E11" si="0">CONCATENATE("    {""",$A$1,""":""",$A3,""",""",$B$1,""":""",$B3,""",""",$C$1,""":""",$C3,"""},")</f>
+        <v xml:space="preserve">    {"name":"population","class":"primary","description":"Total population"},</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4046,14 +4088,14 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"field name":"food_ins_rate","class":demographic_data_primary,"description":Food insecurity rate},</v>
+        <v xml:space="preserve">    {"name":"food_ins_rate","class":"primary","description":"Food insecurity rate"},</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4061,14 +4103,14 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"field name":"food_ins_rate_child","class":demographic_data_primary,"description":Child food insecurity rate},</v>
+        <v xml:space="preserve">    {"name":"food_ins_rate_child","class":"primary","description":"Child food insecurity rate"},</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4076,14 +4118,14 @@
         <v>68</v>
       </c>
       <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"field name":"snap","class":demographic_data_secondary,"description":SNAP participants},</v>
+        <v xml:space="preserve">    {"name":"snap","class":"secondary","description":"SNAP participants"},</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4091,14 +4133,14 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"field name":"snap_percentage","class":demographic_data_secondary,"description":Percentage of population receiving SNAP},</v>
+        <v xml:space="preserve">    {"name":"snap_percentage","class":"secondary","description":"Percentage of population receiving SNAP"},</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4106,14 +4148,14 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"field name":"wic","class":demographic_data_secondary,"description":Number of WIC participants},</v>
+        <v xml:space="preserve">    {"name":"wic","class":"secondary","description":"Number of WIC participants"},</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -4121,14 +4163,14 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"field name":"free_lunch","class":demographic_data_secondary,"description":Number Free and Reduced-Price School Lunch recipients},</v>
+        <v xml:space="preserve">    {"name":"free_lunch","class":"secondary","description":"Number Free and Reduced-Price School Lunch recipients"},</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4136,14 +4178,14 @@
         <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"field name":"free_breakfast","class":demographic_data_secondary,"description":Number of Free and Reduced-Price School Breakfast recipients},</v>
+        <v xml:space="preserve">    {"name":"free_breakfast","class":"secondary","description":"Number of Free and Reduced-Price School Breakfast recipients"},</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4151,14 +4193,14 @@
         <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"field name":"food_banks","class":demographic_data_secondary,"description":Number of State Food Purchase Program (Food Banks) participants},</v>
+        <v xml:space="preserve">    {"name":"food_banks","class":"secondary","description":"Number of State Food Purchase Program (Food Banks) participants"},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added external libraries changed highlight color to green added "Hunger In" to county_name
</commit_message>
<xml_diff>
--- a/SourceData/CountyData.xlsx
+++ b/SourceData/CountyData.xlsx
@@ -283,9 +283,6 @@
     <t>Number of State Food Purchase Program (Food Banks) participants</t>
   </si>
   <si>
-    <t>County</t>
-  </si>
-  <si>
     <t>header</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>Number Free and Reduced-Price School Lunch recipients</t>
+  </si>
+  <si>
+    <t>Hunger In</t>
   </si>
 </sst>
 </file>
@@ -364,8 +364,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -432,7 +434,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -462,6 +464,7 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -491,6 +494,7 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -1028,7 +1032,7 @@
   <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L2" sqref="L2:L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1081,39 +1085,39 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C33" ca="1" si="0">RAND()*100</f>
-        <v>72.138040995754665</v>
+        <v>41.458591741032095</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:D33" ca="1" si="1">RAND()/5*300</f>
-        <v>33.419423747825967</v>
+        <v>31.274913856770159</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E33" ca="1" si="2">RAND()*$B2</f>
-        <v>6408.1375931966695</v>
+        <v>12239.720248255968</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" ref="F2:F33" ca="1" si="3">$E2/$B2*100</f>
-        <v>51.908769487214826</v>
+        <v>99.147187106164182</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" ref="G2:G33" ca="1" si="4">$B2*0.3*RAND()</f>
-        <v>1654.2590012863502</v>
+        <v>2179.3673440666043</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H33" ca="1" si="5">$B2*0.4*RAND()</f>
-        <v>1661.9016086703252</v>
+        <v>3097.1719656339255</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" ref="I2:I33" ca="1" si="6">$B2*0.1*RAND()</f>
-        <v>951.84393864812921</v>
+        <v>607.47543320553302</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" ref="J2:J33" ca="1" si="7">$B2*0.5*RAND()</f>
-        <v>3581.4220894638829</v>
+        <v>4983.2365000011632</v>
       </c>
       <c r="L2" t="str">
         <f ca="1">CONCATENATE("    {""",$A$1,""":""",$A2,""",""",$B$1,""":",$B2,",""",$C$1,""":",$C2,",""",$D$1,""":",$D2,",""",$E$1,""":",$E2,",""",$F$1,""":",$F2,",""",$G$1,""":",$G2,",""",$H$1,""":",$H2,",""",$I$1,""":",$I2,",""",$J$1,""":",$J2,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Adams","population":12345,"food_ins_rate":72.1380409957547,"food_ins_rate_child":33.419423747826,"snap":6408.13759319667,"snap_percentage":51.9087694872148,"wic":1654.25900128635,"free_lunch":1661.90160867033,"free_breakfast":951.843938648129,"food_banks":3581.42208946388},</v>
+        <v xml:space="preserve">    {"county_name":"Adams","population":12345,"food_ins_rate":41.4585917410321,"food_ins_rate_child":31.2749138567702,"snap":12239.720248256,"snap_percentage":99.1471871061642,"wic":2179.3673440666,"free_lunch":3097.17196563393,"free_breakfast":607.475433205533,"food_banks":4983.23650000116},</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1125,39 +1129,39 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>76.770623757791483</v>
+        <v>58.586738287738207</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>17.670503266190213</v>
+        <v>5.6737893234927554</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>19190.780878782327</v>
+        <v>22790.018591152901</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>81.816084919774596</v>
+        <v>97.160720460235765</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>6751.3231739682087</v>
+        <v>5368.0507982040463</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>6925.6814557125717</v>
+        <v>7029.4031370170605</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>303.37940386583426</v>
+        <v>1002.2953689311696</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>4605.3756859144014</v>
+        <v>4862.2385507056661</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L66" ca="1" si="8">CONCATENATE("    {""",$A$1,""":""",$A3,""",""",$B$1,""":",$B3,",""",$C$1,""":",$C3,",""",$D$1,""":",$D3,",""",$E$1,""":",$E3,",""",$F$1,""":",$F3,",""",$G$1,""":",$G3,",""",$H$1,""":",$H3,",""",$I$1,""":",$I3,",""",$J$1,""":",$J3,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Allegheny","population":23456,"food_ins_rate":76.7706237577915,"food_ins_rate_child":17.6705032661902,"snap":19190.7808787823,"snap_percentage":81.8160849197746,"wic":6751.32317396821,"free_lunch":6925.68145571257,"free_breakfast":303.379403865834,"food_banks":4605.3756859144},</v>
+        <v xml:space="preserve">    {"county_name":"Allegheny","population":23456,"food_ins_rate":58.5867382877382,"food_ins_rate_child":5.67378932349276,"snap":22790.0185911529,"snap_percentage":97.1607204602358,"wic":5368.05079820405,"free_lunch":7029.40313701706,"free_breakfast":1002.29536893117,"food_banks":4862.23855070567},</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1169,39 +1173,39 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>13.874558906362477</v>
+        <v>94.513255511326292</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>14.794433134200656</v>
+        <v>5.2858513243607046</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>318600.97301549331</v>
+        <v>90504.628955998021</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>93.36483767154003</v>
+        <v>26.522047032759065</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>42536.602141968513</v>
+        <v>56770.231414441449</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>59669.479165689016</v>
+        <v>93843.195586220711</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>20641.416284673873</v>
+        <v>32573.392037855225</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>145780.04177663935</v>
+        <v>82890.687714335319</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Armstrong","population":341243,"food_ins_rate":13.8745589063625,"food_ins_rate_child":14.7944331342007,"snap":318600.973015493,"snap_percentage":93.36483767154,"wic":42536.6021419685,"free_lunch":59669.479165689,"free_breakfast":20641.4162846739,"food_banks":145780.041776639},</v>
+        <v xml:space="preserve">    {"county_name":"Armstrong","population":341243,"food_ins_rate":94.5132555113263,"food_ins_rate_child":5.2858513243607,"snap":90504.628955998,"snap_percentage":26.5220470327591,"wic":56770.2314144414,"free_lunch":93843.1955862207,"free_breakfast":32573.3920378552,"food_banks":82890.6877143353},</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1213,39 +1217,39 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>28.294047821108016</v>
+        <v>56.581886944944472</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>35.222699412291206</v>
+        <v>47.603211762799432</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>223252.0799437009</v>
+        <v>421639.68990952399</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>49.111797121668758</v>
+        <v>92.753818528821</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>17238.956764568418</v>
+        <v>27830.594149276505</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>51978.978833142508</v>
+        <v>66539.778264051274</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>40785.232096040585</v>
+        <v>1108.1639928854734</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>39451.693245922033</v>
+        <v>199765.7188124939</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Beaver","population":454579.333333333,"food_ins_rate":28.294047821108,"food_ins_rate_child":35.2226994122912,"snap":223252.079943701,"snap_percentage":49.1117971216688,"wic":17238.9567645684,"free_lunch":51978.9788331425,"free_breakfast":40785.2320960406,"food_banks":39451.693245922},</v>
+        <v xml:space="preserve">    {"county_name":"Beaver","population":454579.333333333,"food_ins_rate":56.5818869449445,"food_ins_rate_child":47.6032117627994,"snap":421639.689909524,"snap_percentage":92.753818528821,"wic":27830.5941492765,"free_lunch":66539.7782640513,"free_breakfast":1108.16399288547,"food_banks":199765.718812494},</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1257,39 +1261,39 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>90.675378611761332</v>
+        <v>45.899516795551008</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>22.033575045670599</v>
+        <v>7.9157804186767038</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>322369.34319033497</v>
+        <v>305883.45262168068</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>52.076670134700642</v>
+        <v>49.413481766588099</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>107120.26211515586</v>
+        <v>74477.259246345915</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>149051.82894568224</v>
+        <v>177386.77353426843</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>44347.395163985762</v>
+        <v>22913.216332209875</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>269484.2210566451</v>
+        <v>178904.29326439206</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bedford","population":619028.333333333,"food_ins_rate":90.6753786117613,"food_ins_rate_child":22.0335750456706,"snap":322369.343190335,"snap_percentage":52.0766701347006,"wic":107120.262115156,"free_lunch":149051.828945682,"free_breakfast":44347.3951639858,"food_banks":269484.221056645},</v>
+        <v xml:space="preserve">    {"county_name":"Bedford","population":619028.333333333,"food_ins_rate":45.899516795551,"food_ins_rate_child":7.9157804186767,"snap":305883.452621681,"snap_percentage":49.4134817665881,"wic":74477.2592463459,"free_lunch":177386.773534268,"free_breakfast":22913.2163322099,"food_banks":178904.293264392},</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1301,39 +1305,39 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>75.500414350364849</v>
+        <v>56.47881632384356</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>46.127755031368018</v>
+        <v>21.109767593956054</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>144666.12823669886</v>
+        <v>58880.584349551289</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>18.464622023104553</v>
+        <v>7.5152888085532332</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>41084.609823642575</v>
+        <v>182931.95261308568</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>146418.45322834144</v>
+        <v>125232.27912124846</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>59640.673869921826</v>
+        <v>59457.879040148451</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>197559.05892190558</v>
+        <v>28720.736980854439</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Berks","population":783477.333333333,"food_ins_rate":75.5004143503648,"food_ins_rate_child":46.127755031368,"snap":144666.128236699,"snap_percentage":18.4646220231046,"wic":41084.6098236426,"free_lunch":146418.453228341,"free_breakfast":59640.6738699218,"food_banks":197559.058921906},</v>
+        <v xml:space="preserve">    {"county_name":"Berks","population":783477.333333333,"food_ins_rate":56.4788163238436,"food_ins_rate_child":21.1097675939561,"snap":58880.5843495513,"snap_percentage":7.51528880855323,"wic":182931.952613086,"free_lunch":125232.279121248,"free_breakfast":59457.8790401485,"food_banks":28720.7369808544},</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1345,39 +1349,39 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>53.853193693907372</v>
+        <v>8.4736347759086001</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>25.601274808065497</v>
+        <v>36.877130370352496</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>5493.0752336973719</v>
+        <v>899043.88035218557</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>0.57948334596648055</v>
+        <v>94.843222383193549</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>213519.69312186266</v>
+        <v>43902.728531639194</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>208833.62387990102</v>
+        <v>236988.5180768529</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>41655.389883377989</v>
+        <v>44743.753710414239</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>287567.50700000691</v>
+        <v>311513.73591563554</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Blair","population":947926.333333333,"food_ins_rate":53.8531936939074,"food_ins_rate_child":25.6012748080655,"snap":5493.07523369737,"snap_percentage":0.579483345966481,"wic":213519.693121863,"free_lunch":208833.623879901,"free_breakfast":41655.389883378,"food_banks":287567.507000007},</v>
+        <v xml:space="preserve">    {"county_name":"Blair","population":947926.333333333,"food_ins_rate":8.4736347759086,"food_ins_rate_child":36.8771303703525,"snap":899043.880352186,"snap_percentage":94.8432223831935,"wic":43902.7285316392,"free_lunch":236988.518076853,"free_breakfast":44743.7537104142,"food_banks":311513.735915636},</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1389,39 +1393,39 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>98.345821660898153</v>
+        <v>50.676975974154281</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.446949189081344</v>
+        <v>57.279512126615309</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>399582.42935065163</v>
+        <v>781168.11945482565</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>35.921547105262384</v>
+        <v>70.225228485963186</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>62990.269084811407</v>
+        <v>136273.02425281669</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>101933.4061391891</v>
+        <v>247333.59015703891</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>40636.899232543088</v>
+        <v>86334.768695962426</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>463685.14982098358</v>
+        <v>546876.39744595427</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bradford","population":1112375.33333333,"food_ins_rate":98.3458216608982,"food_ins_rate_child":48.4469491890813,"snap":399582.429350652,"snap_percentage":35.9215471052624,"wic":62990.2690848114,"free_lunch":101933.406139189,"free_breakfast":40636.8992325431,"food_banks":463685.149820984},</v>
+        <v xml:space="preserve">    {"county_name":"Bradford","population":1112375.33333333,"food_ins_rate":50.6769759741543,"food_ins_rate_child":57.2795121266153,"snap":781168.119454826,"snap_percentage":70.2252284859632,"wic":136273.024252817,"free_lunch":247333.590157039,"free_breakfast":86334.7686959624,"food_banks":546876.397445954},</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1433,39 +1437,39 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>26.04002611186862</v>
+        <v>19.881181278818062</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>51.355043337247643</v>
+        <v>40.205084339713231</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>986413.61671390408</v>
+        <v>261603.76059079988</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>77.255233234687211</v>
+        <v>20.488625863500452</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>21610.870230794397</v>
+        <v>302598.42361355858</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>503724.08727766993</v>
+        <v>153158.72268451584</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>127075.51358701993</v>
+        <v>20729.296624419483</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>109466.8099603177</v>
+        <v>225101.46560588505</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bucks","population":1276824.33333333,"food_ins_rate":26.0400261118686,"food_ins_rate_child":51.3550433372476,"snap":986413.616713904,"snap_percentage":77.2552332346872,"wic":21610.8702307944,"free_lunch":503724.08727767,"free_breakfast":127075.51358702,"food_banks":109466.809960318},</v>
+        <v xml:space="preserve">    {"county_name":"Bucks","population":1276824.33333333,"food_ins_rate":19.8811812788181,"food_ins_rate_child":40.2050843397132,"snap":261603.7605908,"snap_percentage":20.4886258635005,"wic":302598.423613559,"free_lunch":153158.722684516,"free_breakfast":20729.2966244195,"food_banks":225101.465605885},</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1477,39 +1481,39 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>69.181102885725537</v>
+        <v>2.3217218137683626</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>55.351509117268009</v>
+        <v>3.0208298444934489</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>831780.03647527122</v>
+        <v>440427.97141340445</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>57.711470630734382</v>
+        <v>30.558254373221281</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>725.0347713037105</v>
+        <v>188138.17964668403</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>331626.28127437615</v>
+        <v>489129.38639565045</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>90670.860715189556</v>
+        <v>85486.276891398171</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>221037.50242871183</v>
+        <v>592587.55994570826</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Butler","population":1441273.33333333,"food_ins_rate":69.1811028857255,"food_ins_rate_child":55.351509117268,"snap":831780.036475271,"snap_percentage":57.7114706307344,"wic":725.03477130371,"free_lunch":331626.281274376,"free_breakfast":90670.8607151896,"food_banks":221037.502428712},</v>
+        <v xml:space="preserve">    {"county_name":"Butler","population":1441273.33333333,"food_ins_rate":2.32172181376836,"food_ins_rate_child":3.02082984449345,"snap":440427.971413404,"snap_percentage":30.5582543732213,"wic":188138.179646684,"free_lunch":489129.38639565,"free_breakfast":85486.2768913982,"food_banks":592587.559945708},</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1521,39 +1525,39 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43.39306860650953</v>
+        <v>38.593428923603355</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>15.858771836675931</v>
+        <v>13.435754364250553</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>71381.214424975697</v>
+        <v>1297297.5677333244</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4454270170605987</v>
+        <v>80.792148231522404</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>210023.30399597037</v>
+        <v>115681.08081299183</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>22440.59194074924</v>
+        <v>368560.31438890874</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>22835.383734765735</v>
+        <v>81518.844377948088</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>518397.63414993149</v>
+        <v>414433.79298880242</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cambria","population":1605722.33333333,"food_ins_rate":43.3930686065095,"food_ins_rate_child":15.8587718366759,"snap":71381.2144249757,"snap_percentage":4.4454270170606,"wic":210023.30399597,"free_lunch":22440.5919407492,"free_breakfast":22835.3837347657,"food_banks":518397.634149931},</v>
+        <v xml:space="preserve">    {"county_name":"Cambria","population":1605722.33333333,"food_ins_rate":38.5934289236034,"food_ins_rate_child":13.4357543642506,"snap":1297297.56773332,"snap_percentage":80.7921482315224,"wic":115681.080812992,"free_lunch":368560.314388909,"free_breakfast":81518.8443779481,"food_banks":414433.792988802},</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1565,39 +1569,39 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>77.324558695767948</v>
+        <v>51.779471037875688</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>6.776587864871642</v>
+        <v>12.975612044169669</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1235242.0172600995</v>
+        <v>603492.71140806691</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>69.780929902083031</v>
+        <v>34.092333326382423</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>267724.91370425344</v>
+        <v>118460.17858342091</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>166148.48756640707</v>
+        <v>258778.51112531463</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>174371.16783562323</v>
+        <v>122370.78763868658</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>579798.02956530743</v>
+        <v>189789.7819991718</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cameron","population":1770171.33333333,"food_ins_rate":77.3245586957679,"food_ins_rate_child":6.77658786487164,"snap":1235242.0172601,"snap_percentage":69.780929902083,"wic":267724.913704253,"free_lunch":166148.487566407,"free_breakfast":174371.167835623,"food_banks":579798.029565307},</v>
+        <v xml:space="preserve">    {"county_name":"Cameron","population":1770171.33333333,"food_ins_rate":51.7794710378757,"food_ins_rate_child":12.9756120441697,"snap":603492.711408067,"snap_percentage":34.0923333263824,"wic":118460.178583421,"free_lunch":258778.511125315,"free_breakfast":122370.787638687,"food_banks":189789.781999172},</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1609,39 +1613,39 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>90.401659411968808</v>
+        <v>68.573162920680247</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1143812870902812</v>
+        <v>43.217661994883578</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>808000.13387645304</v>
+        <v>1595518.342079649</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>41.765307639679229</v>
+        <v>82.47191009982761</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>490132.90456598555</v>
+        <v>442811.76732089167</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>13947.777706805688</v>
+        <v>261921.71898879687</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>46818.018931908293</v>
+        <v>52044.906932278398</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>93366.635516304232</v>
+        <v>778232.31670944078</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Carbon","population":1934620.33333333,"food_ins_rate":90.4016594119688,"food_ins_rate_child":4.11438128709028,"snap":808000.133876453,"snap_percentage":41.7653076396792,"wic":490132.904565986,"free_lunch":13947.7777068057,"free_breakfast":46818.0189319083,"food_banks":93366.6355163042},</v>
+        <v xml:space="preserve">    {"county_name":"Carbon","population":1934620.33333333,"food_ins_rate":68.5731629206802,"food_ins_rate_child":43.2176619948836,"snap":1595518.34207965,"snap_percentage":82.4719100998276,"wic":442811.767320892,"free_lunch":261921.718988797,"free_breakfast":52044.9069322784,"food_banks":778232.316709441},</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1653,39 +1657,39 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>68.107476738886348</v>
+        <v>11.296793773441715</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60586694900129467</v>
+        <v>31.98124283274413</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1516336.672810893</v>
+        <v>102263.72679936053</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>72.238522507636489</v>
+        <v>4.8718603609422146</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>496738.50946991588</v>
+        <v>195551.55150139079</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>512367.27483277634</v>
+        <v>491849.63150304882</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>156249.51862125256</v>
+        <v>22424.102726983372</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>133050.95232921597</v>
+        <v>859709.16333065892</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Centre","population":2099069.33333333,"food_ins_rate":68.1074767388863,"food_ins_rate_child":0.605866949001295,"snap":1516336.67281089,"snap_percentage":72.2385225076365,"wic":496738.509469916,"free_lunch":512367.274832776,"free_breakfast":156249.518621253,"food_banks":133050.952329216},</v>
+        <v xml:space="preserve">    {"county_name":"Centre","population":2099069.33333333,"food_ins_rate":11.2967937734417,"food_ins_rate_child":31.9812428327441,"snap":102263.726799361,"snap_percentage":4.87186036094221,"wic":195551.551501391,"free_lunch":491849.631503049,"free_breakfast":22424.1027269833,"food_banks":859709.163330659},</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1697,39 +1701,39 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>59.410858251587975</v>
+        <v>60.315375912119627</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>29.271285650810761</v>
+        <v>44.715757457821418</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>486058.2781124484</v>
+        <v>256577.08404640897</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>21.473573726114392</v>
+        <v>11.335321665743493</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>585797.64615443698</v>
+        <v>486498.10431539797</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>359216.80508171889</v>
+        <v>188472.58198415465</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>44426.477629443507</v>
+        <v>2899.1447693190576</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>559826.96982298524</v>
+        <v>643192.25084018265</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Chester","population":2263518.33333333,"food_ins_rate":59.410858251588,"food_ins_rate_child":29.2712856508108,"snap":486058.278112448,"snap_percentage":21.4735737261144,"wic":585797.646154437,"free_lunch":359216.805081719,"free_breakfast":44426.4776294435,"food_banks":559826.969822985},</v>
+        <v xml:space="preserve">    {"county_name":"Chester","population":2263518.33333333,"food_ins_rate":60.3153759121196,"food_ins_rate_child":44.7157574578214,"snap":256577.084046409,"snap_percentage":11.3353216657435,"wic":486498.104315398,"free_lunch":188472.581984155,"free_breakfast":2899.14476931906,"food_banks":643192.250840183},</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1741,39 +1745,39 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43.648800209669972</v>
+        <v>47.347627565587224</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>49.652411277804248</v>
+        <v>32.110899248668332</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>256463.11766099973</v>
+        <v>196093.29022783783</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>10.562873484335732</v>
+        <v>8.0764385721212921</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>549951.0791060878</v>
+        <v>322542.14685696951</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>27561.426575445712</v>
+        <v>173776.13143341703</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>82198.004671900431</v>
+        <v>229539.30277967794</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>269929.19442820508</v>
+        <v>423254.16163344914</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clarion","population":2427967.33333333,"food_ins_rate":43.64880020967,"food_ins_rate_child":49.6524112778042,"snap":256463.117661,"snap_percentage":10.5628734843357,"wic":549951.079106088,"free_lunch":27561.4265754457,"free_breakfast":82198.0046719004,"food_banks":269929.194428205},</v>
+        <v xml:space="preserve">    {"county_name":"Clarion","population":2427967.33333333,"food_ins_rate":47.3476275655872,"food_ins_rate_child":32.1108992486683,"snap":196093.290227838,"snap_percentage":8.07643857212129,"wic":322542.14685697,"free_lunch":173776.131433417,"free_breakfast":229539.302779678,"food_banks":423254.161633449},</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1785,39 +1789,39 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>72.143804371859886</v>
+        <v>51.468138509750183</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>57.553080925495301</v>
+        <v>50.426488508328454</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1338489.6572941747</v>
+        <v>1911504.7527465736</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>51.630968378182686</v>
+        <v>73.734481925932002</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>130144.24994156674</v>
+        <v>646421.70623156417</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>893330.64505714132</v>
+        <v>209380.00815711074</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>47019.839626793066</v>
+        <v>126921.14267116688</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>938676.33005868096</v>
+        <v>1168412.4925603913</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clearfield","population":2592416.33333333,"food_ins_rate":72.1438043718599,"food_ins_rate_child":57.5530809254953,"snap":1338489.65729417,"snap_percentage":51.6309683781827,"wic":130144.249941567,"free_lunch":893330.645057141,"free_breakfast":47019.8396267931,"food_banks":938676.330058681},</v>
+        <v xml:space="preserve">    {"county_name":"Clearfield","population":2592416.33333333,"food_ins_rate":51.4681385097502,"food_ins_rate_child":50.4264885083285,"snap":1911504.75274657,"snap_percentage":73.734481925932,"wic":646421.706231564,"free_lunch":209380.008157111,"free_breakfast":126921.142671167,"food_banks":1168412.49256039},</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1829,39 +1833,39 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>50.620544756137342</v>
+        <v>54.680404794449686</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>40.295526204772571</v>
+        <v>1.2979408417456684</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1805657.8428333185</v>
+        <v>2436332.8910841397</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>65.496773491293268</v>
+        <v>88.37330070592769</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>656410.77663275867</v>
+        <v>205140.06344506444</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>475141.92318009405</v>
+        <v>607496.43857938983</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>269950.97740470432</v>
+        <v>23190.385545499077</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>672526.41599255172</v>
+        <v>456024.29064497456</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clinton","population":2756865.33333333,"food_ins_rate":50.6205447561373,"food_ins_rate_child":40.2955262047726,"snap":1805657.84283332,"snap_percentage":65.4967734912933,"wic":656410.776632759,"free_lunch":475141.923180094,"free_breakfast":269950.977404704,"food_banks":672526.415992552},</v>
+        <v xml:space="preserve">    {"county_name":"Clinton","population":2756865.33333333,"food_ins_rate":54.6804047944497,"food_ins_rate_child":1.29794084174567,"snap":2436332.89108414,"snap_percentage":88.3733007059277,"wic":205140.063445064,"free_lunch":607496.43857939,"free_breakfast":23190.3855454991,"food_banks":456024.290644975},</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1873,39 +1877,39 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>60.979626733931227</v>
+        <v>41.818062852804395</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>34.988495386032149</v>
+        <v>3.9458525482828488</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2829587.4068828011</v>
+        <v>2821259.7608727496</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>96.860080224716356</v>
+        <v>96.57501518001952</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>52133.125673880051</v>
+        <v>154962.55415561868</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>118975.82588008439</v>
+        <v>515571.87058078591</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>229339.5280365911</v>
+        <v>232583.90151736033</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1176550.5336463735</v>
+        <v>835116.03076987411</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Columbia","population":2921314.33333333,"food_ins_rate":60.9796267339312,"food_ins_rate_child":34.9884953860321,"snap":2829587.4068828,"snap_percentage":96.8600802247164,"wic":52133.1256738801,"free_lunch":118975.825880084,"free_breakfast":229339.528036591,"food_banks":1176550.53364637},</v>
+        <v xml:space="preserve">    {"county_name":"Columbia","population":2921314.33333333,"food_ins_rate":41.8180628528044,"food_ins_rate_child":3.94585254828285,"snap":2821259.76087275,"snap_percentage":96.5750151800195,"wic":154962.554155619,"free_lunch":515571.870580786,"free_breakfast":232583.90151736,"food_banks":835116.030769874},</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1917,39 +1921,39 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>29.903018160986395</v>
+        <v>41.839628104515349</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2087865161579723</v>
+        <v>0.56677867150193517</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>90153.127039444444</v>
+        <v>1522454.3960007026</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9215826782820198</v>
+        <v>49.338015639589045</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>473082.1931481667</v>
+        <v>534735.2686316499</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1136010.0305134535</v>
+        <v>724262.05314076226</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>38061.869322962491</v>
+        <v>198080.49483495724</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1043742.3085605262</v>
+        <v>485854.8967208016</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Crawford","population":3085763.33333333,"food_ins_rate":29.9030181609864,"food_ins_rate_child":4.20878651615797,"snap":90153.1270394444,"snap_percentage":2.92158267828202,"wic":473082.193148167,"free_lunch":1136010.03051345,"free_breakfast":38061.8693229625,"food_banks":1043742.30856053},</v>
+        <v xml:space="preserve">    {"county_name":"Crawford","population":3085763.33333333,"food_ins_rate":41.8396281045153,"food_ins_rate_child":0.566778671501935,"snap":1522454.3960007,"snap_percentage":49.338015639589,"wic":534735.26863165,"free_lunch":724262.053140762,"free_breakfast":198080.494834957,"food_banks":485854.896720802},</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1961,39 +1965,39 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7.226640753754598</v>
+        <v>38.364073856350203</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>34.066474691465345</v>
+        <v>24.591605646303819</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1716438.7580330241</v>
+        <v>2290062.0670672641</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>52.81004999057064</v>
+        <v>70.458844906253802</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>327670.64267701312</v>
+        <v>137934.36821345365</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>611477.39312963781</v>
+        <v>1106323.767848134</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>268019.27451495733</v>
+        <v>83815.444611258237</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>973660.58863826585</v>
+        <v>1295183.3728501159</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cumberland","population":3250212.33333333,"food_ins_rate":7.2266407537546,"food_ins_rate_child":34.0664746914653,"snap":1716438.75803302,"snap_percentage":52.8100499905706,"wic":327670.642677013,"free_lunch":611477.393129638,"free_breakfast":268019.274514957,"food_banks":973660.588638266},</v>
+        <v xml:space="preserve">    {"county_name":"Cumberland","population":3250212.33333333,"food_ins_rate":38.3640738563502,"food_ins_rate_child":24.5916056463038,"snap":2290062.06706726,"snap_percentage":70.4588449062538,"wic":137934.368213454,"free_lunch":1106323.76784813,"free_breakfast":83815.4446112582,"food_banks":1295183.37285012},</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2005,39 +2009,39 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>66.597373627855745</v>
+        <v>61.43851179315093</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>47.577066142870528</v>
+        <v>38.623024262452994</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1031528.7096110887</v>
+        <v>1629967.5603367751</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>30.208814547477512</v>
+        <v>47.734384210384647</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>481999.04365239997</v>
+        <v>137194.1276644287</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1104336.2951705218</v>
+        <v>386078.39767081587</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>299791.3229817829</v>
+        <v>103168.86701338648</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1336846.1138623487</v>
+        <v>1517736.4029582578</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Dauphin","population":3414661.33333333,"food_ins_rate":66.5973736278557,"food_ins_rate_child":47.5770661428705,"snap":1031528.70961109,"snap_percentage":30.2088145474775,"wic":481999.0436524,"free_lunch":1104336.29517052,"free_breakfast":299791.322981783,"food_banks":1336846.11386235},</v>
+        <v xml:space="preserve">    {"county_name":"Dauphin","population":3414661.33333333,"food_ins_rate":61.4385117931509,"food_ins_rate_child":38.623024262453,"snap":1629967.56033678,"snap_percentage":47.7343842103846,"wic":137194.127664429,"free_lunch":386078.397670816,"free_breakfast":103168.867013386,"food_banks":1517736.40295826},</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2049,39 +2053,39 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>55.660082491943406</v>
+        <v>89.903335885593052</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2869726608955432</v>
+        <v>27.418590992797679</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1102358.9692374703</v>
+        <v>1892170.6641147637</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>30.799804045459844</v>
+        <v>52.8670671728784</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>526548.93142689427</v>
+        <v>390344.19551190373</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>613154.18601777067</v>
+        <v>1289922.8510374222</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>234643.92427031242</v>
+        <v>122203.38361026117</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1140993.7677004954</v>
+        <v>1707167.6486449135</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Delaware","population":3579110.33333333,"food_ins_rate":55.6600824919434,"food_ins_rate_child":9.28697266089554,"snap":1102358.96923747,"snap_percentage":30.7998040454598,"wic":526548.931426894,"free_lunch":613154.186017771,"free_breakfast":234643.924270312,"food_banks":1140993.7677005},</v>
+        <v xml:space="preserve">    {"county_name":"Delaware","population":3579110.33333333,"food_ins_rate":89.9033358855931,"food_ins_rate_child":27.4185909927977,"snap":1892170.66411476,"snap_percentage":52.8670671728784,"wic":390344.195511904,"free_lunch":1289922.85103742,"free_breakfast":122203.383610261,"food_banks":1707167.64864491},</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2093,39 +2097,39 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>61.215698045288015</v>
+        <v>80.38603761359704</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>37.646972366729891</v>
+        <v>31.303776632250667</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>458763.61073937087</v>
+        <v>3167256.1616043877</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>12.254743945273061</v>
+        <v>84.605475153086672</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>847807.38290777081</v>
+        <v>436049.64136435027</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1159071.5761694736</v>
+        <v>145998.88638813447</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>40008.960401347002</v>
+        <v>206180.45084098124</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>485232.03404100362</v>
+        <v>1853749.3749176369</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Elk","population":3743559.33333333,"food_ins_rate":61.215698045288,"food_ins_rate_child":37.6469723667299,"snap":458763.610739371,"snap_percentage":12.2547439452731,"wic":847807.382907771,"free_lunch":1159071.57616947,"free_breakfast":40008.960401347,"food_banks":485232.034041004},</v>
+        <v xml:space="preserve">    {"county_name":"Elk","population":3743559.33333333,"food_ins_rate":80.386037613597,"food_ins_rate_child":31.3037766322507,"snap":3167256.16160439,"snap_percentage":84.6054751530867,"wic":436049.64136435,"free_lunch":145998.886388134,"free_breakfast":206180.450840981,"food_banks":1853749.37491764},</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2137,39 +2141,39 @@
       </c>
       <c r="C26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>39.781865307032959</v>
+        <v>93.679390531095734</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>37.019136840113987</v>
+        <v>41.770976519016386</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3317932.2326968275</v>
+        <v>1293223.660872503</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>84.900848455120922</v>
+        <v>33.091630072586092</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>766125.18689543486</v>
+        <v>6865.9103293805356</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>85635.750625510176</v>
+        <v>29078.872946265121</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>73273.51646279062</v>
+        <v>149902.71520597814</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>56102.988992886945</v>
+        <v>199050.7279742728</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Erie","population":3908008.33333333,"food_ins_rate":39.781865307033,"food_ins_rate_child":37.019136840114,"snap":3317932.23269683,"snap_percentage":84.9008484551209,"wic":766125.186895435,"free_lunch":85635.7506255102,"free_breakfast":73273.5164627906,"food_banks":56102.9889928869},</v>
+        <v xml:space="preserve">    {"county_name":"Erie","population":3908008.33333333,"food_ins_rate":93.6793905310957,"food_ins_rate_child":41.7709765190164,"snap":1293223.6608725,"snap_percentage":33.0916300725861,"wic":6865.91032938054,"free_lunch":29078.8729462651,"free_breakfast":149902.715205978,"food_banks":199050.727974273},</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2181,39 +2185,39 @@
       </c>
       <c r="C27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>75.780544368471709</v>
+        <v>48.70266821296002</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>54.672547468567792</v>
+        <v>51.497153864789198</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1009404.5685472747</v>
+        <v>2805482.9710079636</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>24.786129992946325</v>
+        <v>68.889192479560236</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>575062.70100809552</v>
+        <v>543228.58846006833</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1185983.9424940187</v>
+        <v>341214.0611038811</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>371763.40997038904</v>
+        <v>308255.18696515099</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>322807.01739413838</v>
+        <v>435250.30638820247</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Fayette","population":4072457.33333333,"food_ins_rate":75.7805443684717,"food_ins_rate_child":54.6725474685678,"snap":1009404.56854727,"snap_percentage":24.7861299929463,"wic":575062.701008096,"free_lunch":1185983.94249402,"free_breakfast":371763.409970389,"food_banks":322807.017394138},</v>
+        <v xml:space="preserve">    {"county_name":"Fayette","population":4072457.33333333,"food_ins_rate":48.70266821296,"food_ins_rate_child":51.4971538647892,"snap":2805482.97100796,"snap_percentage":68.8891924795602,"wic":543228.588460068,"free_lunch":341214.061103881,"free_breakfast":308255.186965151,"food_banks":435250.306388202},</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2225,39 +2229,39 @@
       </c>
       <c r="C28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>79.175812894667203</v>
+        <v>95.806263696224931</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>37.776652381307926</v>
+        <v>59.370984513046665</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>511273.13883039943</v>
+        <v>1891984.279209807</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>12.067133389473872</v>
+        <v>44.65485262973263</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>847630.74223137856</v>
+        <v>450366.34627320309</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>931288.32361644914</v>
+        <v>1622658.8221280782</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>327027.50382689806</v>
+        <v>169714.81771502929</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>963606.29015424429</v>
+        <v>392333.20801926579</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Forest","population":4236906.33333333,"food_ins_rate":79.1758128946672,"food_ins_rate_child":37.7766523813079,"snap":511273.138830399,"snap_percentage":12.0671333894739,"wic":847630.742231379,"free_lunch":931288.323616449,"free_breakfast":327027.503826898,"food_banks":963606.290154244},</v>
+        <v xml:space="preserve">    {"county_name":"Forest","population":4236906.33333333,"food_ins_rate":95.8062636962249,"food_ins_rate_child":59.3709845130467,"snap":1891984.27920981,"snap_percentage":44.6548526297326,"wic":450366.346273203,"free_lunch":1622658.82212808,"free_breakfast":169714.817715029,"food_banks":392333.208019266},</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2269,39 +2273,39 @@
       </c>
       <c r="C29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>97.499468885031703</v>
+        <v>30.229130916711988</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>47.461480690124986</v>
+        <v>16.448941885608548</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3090314.5500097843</v>
+        <v>1320072.8147247946</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>70.212793922942822</v>
+        <v>29.992416307025326</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>1086444.7832108592</v>
+        <v>1194067.3112047827</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1373813.494975124</v>
+        <v>1513352.5369227033</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>337882.00871329493</v>
+        <v>236992.83423870758</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2074680.7628114705</v>
+        <v>986305.6699132059</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Franklin","population":4401355.33333333,"food_ins_rate":97.4994688850317,"food_ins_rate_child":47.461480690125,"snap":3090314.55000978,"snap_percentage":70.2127939229428,"wic":1086444.78321086,"free_lunch":1373813.49497512,"free_breakfast":337882.008713295,"food_banks":2074680.76281147},</v>
+        <v xml:space="preserve">    {"county_name":"Franklin","population":4401355.33333333,"food_ins_rate":30.229130916712,"food_ins_rate_child":16.4489418856085,"snap":1320072.81472479,"snap_percentage":29.9924163070253,"wic":1194067.31120478,"free_lunch":1513352.5369227,"free_breakfast":236992.834238708,"food_banks":986305.669913206},</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2313,39 +2317,39 @@
       </c>
       <c r="C30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>86.392628506838975</v>
+        <v>2.6739935099318712</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>30.769376104252302</v>
+        <v>12.571477069723207</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>537598.66178905475</v>
+        <v>4305937.4512145156</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>11.774456865447259</v>
+        <v>94.308409578097368</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>1130858.2319139999</v>
+        <v>1205003.6794596501</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>120117.56397234144</v>
+        <v>946178.9512248151</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>293306.6739362629</v>
+        <v>403467.84463105845</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1632622.5606983949</v>
+        <v>1218608.3558469079</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Fulton","population":4565804.33333333,"food_ins_rate":86.392628506839,"food_ins_rate_child":30.7693761042523,"snap":537598.661789055,"snap_percentage":11.7744568654473,"wic":1130858.231914,"free_lunch":120117.563972341,"free_breakfast":293306.673936263,"food_banks":1632622.56069839},</v>
+        <v xml:space="preserve">    {"county_name":"Fulton","population":4565804.33333333,"food_ins_rate":2.67399350993187,"food_ins_rate_child":12.5714770697232,"snap":4305937.45121452,"snap_percentage":94.3084095780974,"wic":1205003.67945965,"free_lunch":946178.951224815,"free_breakfast":403467.844631058,"food_banks":1218608.35584691},</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2357,39 +2361,39 @@
       </c>
       <c r="C31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>37.028584418242694</v>
+        <v>12.516217864354495</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>14.235922319519362</v>
+        <v>33.640679930523028</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2065274.8982296237</v>
+        <v>3498458.1526175006</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>43.660978655751173</v>
+        <v>73.95921330395629</v>
       </c>
       <c r="G31" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>1234309.9654958821</v>
+        <v>426092.88698302588</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1196929.0000552023</v>
+        <v>163811.55041054724</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>25701.341212556796</v>
+        <v>145009.80175187939</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>974061.80013729411</v>
+        <v>704441.00290789083</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Greene","population":4730253.33333333,"food_ins_rate":37.0285844182427,"food_ins_rate_child":14.2359223195194,"snap":2065274.89822962,"snap_percentage":43.6609786557512,"wic":1234309.96549588,"free_lunch":1196929.0000552,"free_breakfast":25701.3412125568,"food_banks":974061.800137294},</v>
+        <v xml:space="preserve">    {"county_name":"Greene","population":4730253.33333333,"food_ins_rate":12.5162178643545,"food_ins_rate_child":33.640679930523,"snap":3498458.1526175,"snap_percentage":73.9592133039563,"wic":426092.886983026,"free_lunch":163811.550410547,"free_breakfast":145009.801751879,"food_banks":704441.002907891},</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2401,39 +2405,39 @@
       </c>
       <c r="C32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>37.845614895704536</v>
+        <v>82.383630401516527</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>58.951378125038012</v>
+        <v>51.493260625558598</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1491.705085381094</v>
+        <v>3398321.2869454646</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>3.0475910153360264E-2</v>
+        <v>69.428558786968793</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>682350.5552634747</v>
+        <v>663339.38411554205</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1581029.1573789755</v>
+        <v>1036806.5742620346</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>227188.89808308956</v>
+        <v>433867.14831335563</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1323400.4160285022</v>
+        <v>1538468.9728849775</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Huntingdon","population":4894702.33333333,"food_ins_rate":37.8456148957045,"food_ins_rate_child":58.951378125038,"snap":1491.70508538109,"snap_percentage":0.0304759101533603,"wic":682350.555263475,"free_lunch":1581029.15737898,"free_breakfast":227188.89808309,"food_banks":1323400.4160285},</v>
+        <v xml:space="preserve">    {"county_name":"Huntingdon","population":4894702.33333333,"food_ins_rate":82.3836304015165,"food_ins_rate_child":51.4932606255586,"snap":3398321.28694546,"snap_percentage":69.4285587869688,"wic":663339.384115542,"free_lunch":1036806.57426203,"free_breakfast":433867.148313356,"food_banks":1538468.97288498},</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2445,39 +2449,39 @@
       </c>
       <c r="C33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>35.324640956709587</v>
+        <v>48.915967192353257</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11.22638350627067</v>
+        <v>36.408718241713693</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3759276.2065936103</v>
+        <v>1120030.371219743</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>74.306458907935664</v>
+        <v>22.138700691560199</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>1155800.4584690963</v>
+        <v>443920.61815436429</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>47247.497838223848</v>
+        <v>1841730.5174990506</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>292430.55300393014</v>
+        <v>24059.416483847232</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1536472.9295054094</v>
+        <v>1785357.219256324</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Indiana","population":5059151.33333333,"food_ins_rate":35.3246409567096,"food_ins_rate_child":11.2263835062707,"snap":3759276.20659361,"snap_percentage":74.3064589079357,"wic":1155800.4584691,"free_lunch":47247.4978382238,"free_breakfast":292430.55300393,"food_banks":1536472.92950541},</v>
+        <v xml:space="preserve">    {"county_name":"Indiana","population":5059151.33333333,"food_ins_rate":48.9159671923533,"food_ins_rate_child":36.4087182417137,"snap":1120030.37121974,"snap_percentage":22.1387006915602,"wic":443920.618154364,"free_lunch":1841730.51749905,"free_breakfast":24059.4164838472,"food_banks":1785357.21925632},</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2489,39 +2493,39 @@
       </c>
       <c r="C34" s="2">
         <f t="shared" ref="C34:C68" ca="1" si="9">RAND()*100</f>
-        <v>24.32151419013525</v>
+        <v>44.731856458085673</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" ref="D34:D68" ca="1" si="10">RAND()/5*300</f>
-        <v>12.485986007935256</v>
+        <v>59.247833974968849</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" ref="E34:E68" ca="1" si="11">RAND()*$B34</f>
-        <v>205322.28561597646</v>
+        <v>981924.24341598304</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" ref="F34:F68" ca="1" si="12">$E34/$B34*100</f>
-        <v>3.9306660638976254</v>
+        <v>18.797844030103828</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" ref="G34:G68" ca="1" si="13">$B34*0.3*RAND()</f>
-        <v>36175.527259826806</v>
+        <v>605799.90207983064</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" ref="H34:H68" ca="1" si="14">$B34*0.4*RAND()</f>
-        <v>1526533.8945175372</v>
+        <v>758313.28812728415</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" ref="I34:I68" ca="1" si="15">$B34*0.1*RAND()</f>
-        <v>12613.880808880616</v>
+        <v>333922.1017293387</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" ref="J34:J68" ca="1" si="16">$B34*0.5*RAND()</f>
-        <v>2582495.6488627954</v>
+        <v>1248694.4349055369</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Jefferson","population":5223600.33333333,"food_ins_rate":24.3215141901353,"food_ins_rate_child":12.4859860079353,"snap":205322.285615976,"snap_percentage":3.93066606389763,"wic":36175.5272598268,"free_lunch":1526533.89451754,"free_breakfast":12613.8808088806,"food_banks":2582495.6488628},</v>
+        <v xml:space="preserve">    {"county_name":"Jefferson","population":5223600.33333333,"food_ins_rate":44.7318564580857,"food_ins_rate_child":59.2478339749688,"snap":981924.243415983,"snap_percentage":18.7978440301038,"wic":605799.902079831,"free_lunch":758313.288127284,"free_breakfast":333922.101729339,"food_banks":1248694.43490554},</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2533,39 +2537,39 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>57.633828702262015</v>
+        <v>6.888969489726815</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>4.1401346453025445</v>
+        <v>28.906173598009666</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4161183.8809539517</v>
+        <v>66590.633857749301</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>77.229877150728029</v>
+        <v>1.2358950287590043</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>321993.24465361104</v>
+        <v>92536.750545643881</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>570950.76975449442</v>
+        <v>2115463.7459848314</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>180805.32730013184</v>
+        <v>50044.302370462559</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>948519.89371795603</v>
+        <v>2674893.9280303884</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Juniata","population":5388049.33333333,"food_ins_rate":57.633828702262,"food_ins_rate_child":4.14013464530254,"snap":4161183.88095395,"snap_percentage":77.229877150728,"wic":321993.244653611,"free_lunch":570950.769754494,"free_breakfast":180805.327300132,"food_banks":948519.893717956},</v>
+        <v xml:space="preserve">    {"county_name":"Juniata","population":5388049.33333333,"food_ins_rate":6.88896948972681,"food_ins_rate_child":28.9061735980097,"snap":66590.6338577493,"snap_percentage":1.235895028759,"wic":92536.7505456439,"free_lunch":2115463.74598483,"free_breakfast":50044.3023704626,"food_banks":2674893.92803039},</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2577,39 +2581,39 @@
       </c>
       <c r="C36" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>44.842223122585487</v>
+        <v>36.924354926925375</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>3.227831914887962</v>
+        <v>55.964479422340695</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4276146.275380413</v>
+        <v>4909714.9242876852</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>77.013013218021356</v>
+        <v>88.423528104694398</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1165983.240631243</v>
+        <v>1631949.8346156285</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>275563.58346224274</v>
+        <v>392898.33280602738</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>91061.077870632434</v>
+        <v>365775.08845406357</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>563078.52294822724</v>
+        <v>2278902.3877954967</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lackawanna","population":5552498.33333333,"food_ins_rate":44.8422231225855,"food_ins_rate_child":3.22783191488796,"snap":4276146.27538041,"snap_percentage":77.0130132180214,"wic":1165983.24063124,"free_lunch":275563.583462243,"free_breakfast":91061.0778706324,"food_banks":563078.522948227},</v>
+        <v xml:space="preserve">    {"county_name":"Lackawanna","population":5552498.33333333,"food_ins_rate":36.9243549269254,"food_ins_rate_child":55.9644794223407,"snap":4909714.92428769,"snap_percentage":88.4235281046944,"wic":1631949.83461563,"free_lunch":392898.332806027,"free_breakfast":365775.088454064,"food_banks":2278902.3877955},</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2621,39 +2625,39 @@
       </c>
       <c r="C37" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>6.3071648467672663</v>
+        <v>46.118830259914091</v>
       </c>
       <c r="D37" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>41.478613369809814</v>
+        <v>41.230600932094248</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4358902.9368920578</v>
+        <v>3072690.440455901</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>76.245287611396463</v>
+        <v>53.747048228697501</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1550984.2644183708</v>
+        <v>377938.92646138219</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>748254.84832000418</v>
+        <v>1364126.6316058948</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>19230.515792160906</v>
+        <v>245386.91429670493</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>406389.62800981413</v>
+        <v>1928589.3782266751</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lancaster","population":5716947.33333333,"food_ins_rate":6.30716484676727,"food_ins_rate_child":41.4786133698098,"snap":4358902.93689206,"snap_percentage":76.2452876113965,"wic":1550984.26441837,"free_lunch":748254.848320004,"free_breakfast":19230.5157921609,"food_banks":406389.628009814},</v>
+        <v xml:space="preserve">    {"county_name":"Lancaster","population":5716947.33333333,"food_ins_rate":46.1188302599141,"food_ins_rate_child":41.2306009320942,"snap":3072690.4404559,"snap_percentage":53.7470482286975,"wic":377938.926461382,"free_lunch":1364126.63160589,"free_breakfast":245386.914296705,"food_banks":1928589.37822668},</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2665,39 +2669,39 @@
       </c>
       <c r="C38" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>91.797471058612814</v>
+        <v>56.615964338046155</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>11.57692996027358</v>
+        <v>24.535695142204339</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2093684.259758075</v>
+        <v>1982972.1659658288</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>35.598421549861136</v>
+        <v>33.716009831324577</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1110248.9028955428</v>
+        <v>264257.02172350476</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>538107.17990154913</v>
+        <v>1288242.939057583</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>496274.30352203076</v>
+        <v>269945.07911961124</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1256378.7821778397</v>
+        <v>1444714.8766104914</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lawrence","population":5881396.33333333,"food_ins_rate":91.7974710586128,"food_ins_rate_child":11.5769299602736,"snap":2093684.25975808,"snap_percentage":35.5984215498611,"wic":1110248.90289554,"free_lunch":538107.179901549,"free_breakfast":496274.303522031,"food_banks":1256378.78217784},</v>
+        <v xml:space="preserve">    {"county_name":"Lawrence","population":5881396.33333333,"food_ins_rate":56.6159643380462,"food_ins_rate_child":24.5356951422043,"snap":1982972.16596583,"snap_percentage":33.7160098313246,"wic":264257.021723505,"free_lunch":1288242.93905758,"free_breakfast":269945.079119611,"food_banks":1444714.87661049},</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2709,39 +2713,39 @@
       </c>
       <c r="C39" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>6.4160571654428677</v>
+        <v>72.943690416952251</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>6.4321901185607055</v>
+        <v>20.895485158415294</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>56489.459666885203</v>
+        <v>2977980.7992989365</v>
       </c>
       <c r="F39" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0.93435171679689955</v>
+        <v>49.25664874157556</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1217624.6447146896</v>
+        <v>777243.43955729879</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1417113.0374988066</v>
+        <v>639099.33015494526</v>
       </c>
       <c r="I39" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>427696.88608166401</v>
+        <v>463336.11050948169</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1867376.3199371938</v>
+        <v>1154613.6833935184</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lebanon","population":6045845.33333333,"food_ins_rate":6.41605716544287,"food_ins_rate_child":6.43219011856071,"snap":56489.4596668852,"snap_percentage":0.9343517167969,"wic":1217624.64471469,"free_lunch":1417113.03749881,"free_breakfast":427696.886081664,"food_banks":1867376.31993719},</v>
+        <v xml:space="preserve">    {"county_name":"Lebanon","population":6045845.33333333,"food_ins_rate":72.9436904169523,"food_ins_rate_child":20.8954851584153,"snap":2977980.79929894,"snap_percentage":49.2566487415756,"wic":777243.439557299,"free_lunch":639099.330154945,"free_breakfast":463336.110509482,"food_banks":1154613.68339352},</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2753,39 +2757,39 @@
       </c>
       <c r="C40" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>0.16183849456163912</v>
+        <v>40.108838874294293</v>
       </c>
       <c r="D40" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>34.142616660893871</v>
+        <v>48.257868937441245</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1632212.7998114373</v>
+        <v>302372.03784377041</v>
       </c>
       <c r="F40" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>26.282374267684006</v>
+        <v>4.8688841722172356</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1332749.8666387226</v>
+        <v>572085.56078867323</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>679977.49199684395</v>
+        <v>2460669.0218399758</v>
       </c>
       <c r="I40" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>587105.44459347951</v>
+        <v>32083.365476021874</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2565756.7187069459</v>
+        <v>2707348.4224299248</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lehigh","population":6210294.33333333,"food_ins_rate":0.161838494561639,"food_ins_rate_child":34.1426166608939,"snap":1632212.79981144,"snap_percentage":26.282374267684,"wic":1332749.86663872,"free_lunch":679977.491996844,"free_breakfast":587105.44459348,"food_banks":2565756.71870695},</v>
+        <v xml:space="preserve">    {"county_name":"Lehigh","population":6210294.33333333,"food_ins_rate":40.1088388742943,"food_ins_rate_child":48.2578689374412,"snap":302372.03784377,"snap_percentage":4.86888417221724,"wic":572085.560788673,"free_lunch":2460669.02183998,"free_breakfast":32083.3654760219,"food_banks":2707348.42242992},</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2797,39 +2801,39 @@
       </c>
       <c r="C41" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>72.678057339020427</v>
+        <v>99.214153889587791</v>
       </c>
       <c r="D41" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>46.85832423304452</v>
+        <v>32.920585889815477</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2823964.0249092281</v>
+        <v>339582.35565585952</v>
       </c>
       <c r="F41" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>44.299258452380506</v>
+        <v>5.3269965220433928</v>
       </c>
       <c r="G41" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>599027.73154416727</v>
+        <v>1083003.8044366101</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>188636.28387481728</v>
+        <v>2366374.4771642587</v>
       </c>
       <c r="I41" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>300001.13630448608</v>
+        <v>446686.85199929815</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>257364.30748665956</v>
+        <v>1252864.9226978675</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Luzerne","population":6374743.33333333,"food_ins_rate":72.6780573390204,"food_ins_rate_child":46.8583242330445,"snap":2823964.02490923,"snap_percentage":44.2992584523805,"wic":599027.731544167,"free_lunch":188636.283874817,"free_breakfast":300001.136304486,"food_banks":257364.30748666},</v>
+        <v xml:space="preserve">    {"county_name":"Luzerne","population":6374743.33333333,"food_ins_rate":99.2141538895878,"food_ins_rate_child":32.9205858898155,"snap":339582.35565586,"snap_percentage":5.32699652204339,"wic":1083003.80443661,"free_lunch":2366374.47716426,"free_breakfast":446686.851999298,"food_banks":1252864.92269787},</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2841,39 +2845,39 @@
       </c>
       <c r="C42" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>92.518721687194187</v>
+        <v>68.809016941462829</v>
       </c>
       <c r="D42" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>21.237150895558575</v>
+        <v>49.185070532726307</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2921519.575475052</v>
+        <v>4037960.1819991581</v>
       </c>
       <c r="F42" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>44.677070600641251</v>
+        <v>61.750136349649495</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>114281.13708976394</v>
+        <v>1885714.739482658</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1925656.1724075966</v>
+        <v>2228603.7891797372</v>
       </c>
       <c r="I42" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>647878.63624443195</v>
+        <v>410537.61383130669</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2105854.8295429251</v>
+        <v>1606818.5769046447</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lycoming","population":6539192.33333333,"food_ins_rate":92.5187216871942,"food_ins_rate_child":21.2371508955586,"snap":2921519.57547505,"snap_percentage":44.6770706006413,"wic":114281.137089764,"free_lunch":1925656.1724076,"free_breakfast":647878.636244432,"food_banks":2105854.82954293},</v>
+        <v xml:space="preserve">    {"county_name":"Lycoming","population":6539192.33333333,"food_ins_rate":68.8090169414628,"food_ins_rate_child":49.1850705327263,"snap":4037960.18199916,"snap_percentage":61.7501363496495,"wic":1885714.73948266,"free_lunch":2228603.78917974,"free_breakfast":410537.613831307,"food_banks":1606818.57690464},</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2885,39 +2889,39 @@
       </c>
       <c r="C43" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>68.800878432834807</v>
+        <v>64.11973835365545</v>
       </c>
       <c r="D43" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>36.126488298431589</v>
+        <v>49.260256788505679</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5267590.8474341044</v>
+        <v>1379972.9022332281</v>
       </c>
       <c r="F43" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>78.57805311333442</v>
+        <v>20.585422662328622</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1017274.8903231488</v>
+        <v>1721163.2473356638</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1147418.5892480593</v>
+        <v>1198609.5782564161</v>
       </c>
       <c r="I43" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>561344.09729243303</v>
+        <v>430144.77972968336</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>664670.65328603622</v>
+        <v>1738260.3304354087</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"McKean","population":6703641.33333333,"food_ins_rate":68.8008784328348,"food_ins_rate_child":36.1264882984316,"snap":5267590.8474341,"snap_percentage":78.5780531133344,"wic":1017274.89032315,"free_lunch":1147418.58924806,"free_breakfast":561344.097292433,"food_banks":664670.653286036},</v>
+        <v xml:space="preserve">    {"county_name":"McKean","population":6703641.33333333,"food_ins_rate":64.1197383536554,"food_ins_rate_child":49.2602567885057,"snap":1379972.90223323,"snap_percentage":20.5854226623286,"wic":1721163.24733566,"free_lunch":1198609.57825642,"free_breakfast":430144.779729683,"food_banks":1738260.33043541},</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2929,39 +2933,39 @@
       </c>
       <c r="C44" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>93.021684610123046</v>
+        <v>88.875797565580626</v>
       </c>
       <c r="D44" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.71491273484673767</v>
+        <v>23.94250073217037</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5198001.6773716062</v>
+        <v>6215838.4431577194</v>
       </c>
       <c r="F44" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>75.683362115140227</v>
+        <v>90.503155047189807</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1687136.4212374927</v>
+        <v>1331100.042869149</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>855139.15919006243</v>
+        <v>556771.93253716989</v>
       </c>
       <c r="I44" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>15728.307024545877</v>
+        <v>122583.69661096467</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3055177.789755628</v>
+        <v>411769.32997853647</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Mercer","population":6868090.33333333,"food_ins_rate":93.021684610123,"food_ins_rate_child":0.714912734846738,"snap":5198001.67737161,"snap_percentage":75.6833621151402,"wic":1687136.42123749,"free_lunch":855139.159190062,"free_breakfast":15728.3070245459,"food_banks":3055177.78975563},</v>
+        <v xml:space="preserve">    {"county_name":"Mercer","population":6868090.33333333,"food_ins_rate":88.8757975655806,"food_ins_rate_child":23.9425007321704,"snap":6215838.44315772,"snap_percentage":90.5031550471898,"wic":1331100.04286915,"free_lunch":556771.93253717,"free_breakfast":122583.696610965,"food_banks":411769.329978536},</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2973,39 +2977,39 @@
       </c>
       <c r="C45" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>92.354174561033531</v>
+        <v>64.130920269302521</v>
       </c>
       <c r="D45" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>17.439326004036378</v>
+        <v>1.6927040766761814</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2958048.5957783088</v>
+        <v>1762353.5593061091</v>
       </c>
       <c r="F45" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>42.062311429351553</v>
+        <v>25.059988658048169</v>
       </c>
       <c r="G45" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1164859.7054603735</v>
+        <v>1045319.505735592</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1357598.5907624674</v>
+        <v>1811730.5296935572</v>
       </c>
       <c r="I45" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>239805.16203477178</v>
+        <v>76604.882598164302</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1081667.2056406927</v>
+        <v>179024.09826824785</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Mifflin","population":7032539.33333333,"food_ins_rate":92.3541745610335,"food_ins_rate_child":17.4393260040364,"snap":2958048.59577831,"snap_percentage":42.0623114293516,"wic":1164859.70546037,"free_lunch":1357598.59076247,"free_breakfast":239805.162034772,"food_banks":1081667.20564069},</v>
+        <v xml:space="preserve">    {"county_name":"Mifflin","population":7032539.33333333,"food_ins_rate":64.1309202693025,"food_ins_rate_child":1.69270407667618,"snap":1762353.55930611,"snap_percentage":25.0599886580482,"wic":1045319.50573559,"free_lunch":1811730.52969356,"free_breakfast":76604.8825981643,"food_banks":179024.098268248},</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -3017,39 +3021,39 @@
       </c>
       <c r="C46" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>13.54161894282514</v>
+        <v>77.741610975982354</v>
       </c>
       <c r="D46" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>39.539266472200026</v>
+        <v>59.492699159871165</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>6304054.1531229382</v>
+        <v>4724969.6939338176</v>
       </c>
       <c r="F46" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>87.59294667639368</v>
+        <v>65.652040479901927</v>
       </c>
       <c r="G46" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>400948.56744449481</v>
+        <v>494239.69471980806</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2075696.3200423827</v>
+        <v>1903412.4623580782</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>708686.4138413124</v>
+        <v>87972.99411920266</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>243625.88762594142</v>
+        <v>3524435.5007314938</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Monroe","population":7196988.33333333,"food_ins_rate":13.5416189428251,"food_ins_rate_child":39.5392664722,"snap":6304054.15312294,"snap_percentage":87.5929466763937,"wic":400948.567444495,"free_lunch":2075696.32004238,"free_breakfast":708686.413841312,"food_banks":243625.887625941},</v>
+        <v xml:space="preserve">    {"county_name":"Monroe","population":7196988.33333333,"food_ins_rate":77.7416109759824,"food_ins_rate_child":59.4926991598712,"snap":4724969.69393382,"snap_percentage":65.6520404799019,"wic":494239.694719808,"free_lunch":1903412.46235808,"free_breakfast":87972.9941192027,"food_banks":3524435.50073149},</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -3061,39 +3065,39 @@
       </c>
       <c r="C47" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>81.707814040661546</v>
+        <v>78.533398650850955</v>
       </c>
       <c r="D47" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>20.787594117306867</v>
+        <v>25.207713780928678</v>
       </c>
       <c r="E47" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>69873.724453906048</v>
+        <v>405911.5088391804</v>
       </c>
       <c r="F47" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0.94918588979234775</v>
+        <v>5.5140251890914316</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1274363.4787247514</v>
+        <v>725455.66868455661</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>892553.49168492388</v>
+        <v>1987419.379157176</v>
       </c>
       <c r="I47" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>84768.582042598238</v>
+        <v>137431.78845179122</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1634331.4490190186</v>
+        <v>1897313.7302020125</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Montgomery","population":7361437.33333333,"food_ins_rate":81.7078140406615,"food_ins_rate_child":20.7875941173069,"snap":69873.724453906,"snap_percentage":0.949185889792348,"wic":1274363.47872475,"free_lunch":892553.491684924,"free_breakfast":84768.5820425982,"food_banks":1634331.44901902},</v>
+        <v xml:space="preserve">    {"county_name":"Montgomery","population":7361437.33333333,"food_ins_rate":78.533398650851,"food_ins_rate_child":25.2077137809287,"snap":405911.50883918,"snap_percentage":5.51402518909143,"wic":725455.668684557,"free_lunch":1987419.37915718,"free_breakfast":137431.788451791,"food_banks":1897313.73020201},</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -3105,39 +3109,39 @@
       </c>
       <c r="C48" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>89.904021512148759</v>
+        <v>32.033953444423481</v>
       </c>
       <c r="D48" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>45.603263076186209</v>
+        <v>44.274480627992006</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4816427.5117544038</v>
+        <v>590189.08394904516</v>
       </c>
       <c r="F48" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>63.99814318775573</v>
+        <v>7.8421206195342759</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1660082.5830338879</v>
+        <v>1879318.8917117002</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2724326.5862716483</v>
+        <v>1288623.5051932479</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>583981.75198463397</v>
+        <v>625796.05463279621</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3516252.9275030135</v>
+        <v>2783741.8860831861</v>
       </c>
       <c r="L48" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Montour","population":7525886.33333333,"food_ins_rate":89.9040215121488,"food_ins_rate_child":45.6032630761862,"snap":4816427.5117544,"snap_percentage":63.9981431877557,"wic":1660082.58303389,"free_lunch":2724326.58627165,"free_breakfast":583981.751984634,"food_banks":3516252.92750301},</v>
+        <v xml:space="preserve">    {"county_name":"Montour","population":7525886.33333333,"food_ins_rate":32.0339534444235,"food_ins_rate_child":44.274480627992,"snap":590189.083949045,"snap_percentage":7.84212061953428,"wic":1879318.8917117,"free_lunch":1288623.50519325,"free_breakfast":625796.054632796,"food_banks":2783741.88608319},</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3149,39 +3153,39 @@
       </c>
       <c r="C49" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>52.032921625796789</v>
+        <v>46.346036951278322</v>
       </c>
       <c r="D49" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>58.231679357929586</v>
+        <v>18.713210291745007</v>
       </c>
       <c r="E49" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5327480.6976672644</v>
+        <v>5014152.8868177244</v>
       </c>
       <c r="F49" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>69.275011644493517</v>
+        <v>65.200705424172568</v>
       </c>
       <c r="G49" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>86024.784354080679</v>
+        <v>930236.58120120596</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2336758.6177607398</v>
+        <v>2493805.5139749702</v>
       </c>
       <c r="I49" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>597262.28003715794</v>
+        <v>479988.74249668611</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3281698.7189882086</v>
+        <v>256371.96038328324</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Northampton","population":7690335.33333333,"food_ins_rate":52.0329216257968,"food_ins_rate_child":58.2316793579296,"snap":5327480.69766726,"snap_percentage":69.2750116444935,"wic":86024.7843540807,"free_lunch":2336758.61776074,"free_breakfast":597262.280037158,"food_banks":3281698.71898821},</v>
+        <v xml:space="preserve">    {"county_name":"Northampton","population":7690335.33333333,"food_ins_rate":46.3460369512783,"food_ins_rate_child":18.713210291745,"snap":5014152.88681772,"snap_percentage":65.2007054241726,"wic":930236.581201206,"free_lunch":2493805.51397497,"free_breakfast":479988.742496686,"food_banks":256371.960383283},</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3193,39 +3197,39 @@
       </c>
       <c r="C50" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>34.104607871816548</v>
+        <v>13.804095799365268</v>
       </c>
       <c r="D50" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>59.681467856183289</v>
+        <v>9.352258607568908</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5571562.5923983678</v>
+        <v>2726349.0087564071</v>
       </c>
       <c r="F50" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>70.932088723993871</v>
+        <v>34.709406306505528</v>
       </c>
       <c r="G50" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1122449.4978964415</v>
+        <v>1924028.4956911982</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>361626.47805502632</v>
+        <v>3030073.0276890737</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>349565.85867122764</v>
+        <v>119332.42099400464</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>473871.5457795788</v>
+        <v>3478406.3120919853</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Northumberland","population":7854784.33333333,"food_ins_rate":34.1046078718165,"food_ins_rate_child":59.6814678561833,"snap":5571562.59239837,"snap_percentage":70.9320887239939,"wic":1122449.49789644,"free_lunch":361626.478055026,"free_breakfast":349565.858671228,"food_banks":473871.545779579},</v>
+        <v xml:space="preserve">    {"county_name":"Northumberland","population":7854784.33333333,"food_ins_rate":13.8040957993653,"food_ins_rate_child":9.35225860756891,"snap":2726349.00875641,"snap_percentage":34.7094063065055,"wic":1924028.4956912,"free_lunch":3030073.02768907,"free_breakfast":119332.420994005,"food_banks":3478406.31209199},</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3237,39 +3241,39 @@
       </c>
       <c r="C51" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>89.32203900592792</v>
+        <v>19.467559282520529</v>
       </c>
       <c r="D51" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>26.579574979031211</v>
+        <v>2.4441152726276072</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>7818714.519763846</v>
+        <v>2878011.8265890568</v>
       </c>
       <c r="F51" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>97.49952638569583</v>
+        <v>35.888865019379132</v>
       </c>
       <c r="G51" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>124576.53306281376</v>
+        <v>426841.92787125503</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1379643.0289187855</v>
+        <v>2778610.7969232621</v>
       </c>
       <c r="I51" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>563096.13559956639</v>
+        <v>781137.73232219962</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3973507.429393115</v>
+        <v>1788364.1637639969</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Perry","population":8019233.33333333,"food_ins_rate":89.3220390059279,"food_ins_rate_child":26.5795749790312,"snap":7818714.51976385,"snap_percentage":97.4995263856958,"wic":124576.533062814,"free_lunch":1379643.02891879,"free_breakfast":563096.135599566,"food_banks":3973507.42939311},</v>
+        <v xml:space="preserve">    {"county_name":"Perry","population":8019233.33333333,"food_ins_rate":19.4675592825205,"food_ins_rate_child":2.44411527262761,"snap":2878011.82658906,"snap_percentage":35.8888650193791,"wic":426841.927871255,"free_lunch":2778610.79692326,"free_breakfast":781137.7323222,"food_banks":1788364.163764},</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3281,39 +3285,39 @@
       </c>
       <c r="C52" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>43.980514851075469</v>
+        <v>52.955200689133228</v>
       </c>
       <c r="D52" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>5.7991380385561069</v>
+        <v>6.4745779502309864</v>
       </c>
       <c r="E52" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>619678.67235083738</v>
+        <v>6007440.3643432977</v>
       </c>
       <c r="F52" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>7.572125201228741</v>
+        <v>73.407545890119877</v>
       </c>
       <c r="G52" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2135786.2286221301</v>
+        <v>512145.35923983698</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2352225.8920502537</v>
+        <v>1706276.7988059928</v>
       </c>
       <c r="I52" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>703587.41815859673</v>
+        <v>197194.31017971894</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>784380.9948999465</v>
+        <v>1914217.8963067243</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Philadelphia","population":8183682.33333333,"food_ins_rate":43.9805148510755,"food_ins_rate_child":5.79913803855611,"snap":619678.672350837,"snap_percentage":7.57212520122874,"wic":2135786.22862213,"free_lunch":2352225.89205025,"free_breakfast":703587.418158597,"food_banks":784380.994899946},</v>
+        <v xml:space="preserve">    {"county_name":"Philadelphia","population":8183682.33333333,"food_ins_rate":52.9552006891332,"food_ins_rate_child":6.47457795023099,"snap":6007440.3643433,"snap_percentage":73.4075458901199,"wic":512145.359239837,"free_lunch":1706276.79880599,"free_breakfast":197194.310179719,"food_banks":1914217.89630672},</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3325,39 +3329,39 @@
       </c>
       <c r="C53" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>58.272454380408249</v>
+        <v>27.923125888230828</v>
       </c>
       <c r="D53" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>12.152353227737986</v>
+        <v>6.5115486422705837</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1517359.5060442896</v>
+        <v>7731112.6271932218</v>
       </c>
       <c r="F53" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>18.176037791662559</v>
+        <v>92.608900345441285</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1480408.0309383965</v>
+        <v>950577.32818299253</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1442819.7276408095</v>
+        <v>1149890.9772898918</v>
       </c>
       <c r="I53" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>555723.75421792339</v>
+        <v>367218.64164733252</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3678429.5546399439</v>
+        <v>2360907.12577115</v>
       </c>
       <c r="L53" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Pike","population":8348131.33333333,"food_ins_rate":58.2724543804082,"food_ins_rate_child":12.152353227738,"snap":1517359.50604429,"snap_percentage":18.1760377916626,"wic":1480408.0309384,"free_lunch":1442819.72764081,"free_breakfast":555723.754217923,"food_banks":3678429.55463994},</v>
+        <v xml:space="preserve">    {"county_name":"Pike","population":8348131.33333333,"food_ins_rate":27.9231258882308,"food_ins_rate_child":6.51154864227058,"snap":7731112.62719322,"snap_percentage":92.6089003454413,"wic":950577.328182993,"free_lunch":1149890.97728989,"free_breakfast":367218.641647333,"food_banks":2360907.12577115},</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3369,39 +3373,39 @@
       </c>
       <c r="C54" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>78.512156827194559</v>
+        <v>94.056470514778496</v>
       </c>
       <c r="D54" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>34.539594992546121</v>
+        <v>19.998652436865338</v>
       </c>
       <c r="E54" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>348747.39734886662</v>
+        <v>947247.56589432526</v>
       </c>
       <c r="F54" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4.0968470627319782</v>
+        <v>11.127619696992685</v>
       </c>
       <c r="G54" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>797503.42525273259</v>
+        <v>420006.33894499374</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>106223.96701897949</v>
+        <v>3195737.851179712</v>
       </c>
       <c r="I54" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>618240.23907067499</v>
+        <v>207571.46044182152</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3371350.7838000101</v>
+        <v>2884849.9460297157</v>
       </c>
       <c r="L54" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Potter","population":8512580.33333333,"food_ins_rate":78.5121568271946,"food_ins_rate_child":34.5395949925461,"snap":348747.397348867,"snap_percentage":4.09684706273198,"wic":797503.425252733,"free_lunch":106223.967018979,"free_breakfast":618240.239070675,"food_banks":3371350.78380001},</v>
+        <v xml:space="preserve">    {"county_name":"Potter","population":8512580.33333333,"food_ins_rate":94.0564705147785,"food_ins_rate_child":19.9986524368653,"snap":947247.565894325,"snap_percentage":11.1276196969927,"wic":420006.338944994,"free_lunch":3195737.85117971,"free_breakfast":207571.460441822,"food_banks":2884849.94602972},</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3413,39 +3417,39 @@
       </c>
       <c r="C55" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>69.252139998532201</v>
+        <v>20.647851957134343</v>
       </c>
       <c r="D55" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>18.149383634949629</v>
+        <v>52.798984006621225</v>
       </c>
       <c r="E55" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2983458.3058315264</v>
+        <v>2329462.0135621745</v>
       </c>
       <c r="F55" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>34.383406938252378</v>
+        <v>26.846307924918566</v>
       </c>
       <c r="G55" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>677986.34259063471</v>
+        <v>1450374.5716696521</v>
       </c>
       <c r="H55" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1231939.1747693741</v>
+        <v>1580811.4430431554</v>
       </c>
       <c r="I55" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>572697.4081209508</v>
+        <v>473466.75315397378</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>482231.19671120035</v>
+        <v>3762998.4408650701</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Schuylkill","population":8677029.33333333,"food_ins_rate":69.2521399985322,"food_ins_rate_child":18.1493836349496,"snap":2983458.30583153,"snap_percentage":34.3834069382524,"wic":677986.342590635,"free_lunch":1231939.17476937,"free_breakfast":572697.408120951,"food_banks":482231.1967112},</v>
+        <v xml:space="preserve">    {"county_name":"Schuylkill","population":8677029.33333333,"food_ins_rate":20.6478519571343,"food_ins_rate_child":52.7989840066212,"snap":2329462.01356217,"snap_percentage":26.8463079249186,"wic":1450374.57166965,"free_lunch":1580811.44304316,"free_breakfast":473466.753153974,"food_banks":3762998.44086507},</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3457,39 +3461,39 @@
       </c>
       <c r="C56" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>21.069146461240674</v>
+        <v>98.909555790010373</v>
       </c>
       <c r="D56" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>26.809728076437086</v>
+        <v>31.725351644094513</v>
       </c>
       <c r="E56" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3311134.9241957027</v>
+        <v>2030603.0264282504</v>
       </c>
       <c r="F56" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>37.450014571798086</v>
+        <v>22.966781683699399</v>
       </c>
       <c r="G56" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>993773.74103747262</v>
+        <v>2053169.7374524686</v>
       </c>
       <c r="H56" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>426203.39412143175</v>
+        <v>230425.20625236962</v>
       </c>
       <c r="I56" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>363254.48474225891</v>
+        <v>870654.94832878991</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3299254.7334141899</v>
+        <v>64948.970662837717</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Snyder","population":8841478.33333333,"food_ins_rate":21.0691464612407,"food_ins_rate_child":26.8097280764371,"snap":3311134.9241957,"snap_percentage":37.4500145717981,"wic":993773.741037473,"free_lunch":426203.394121432,"free_breakfast":363254.484742259,"food_banks":3299254.73341419},</v>
+        <v xml:space="preserve">    {"county_name":"Snyder","population":8841478.33333333,"food_ins_rate":98.9095557900104,"food_ins_rate_child":31.7253516440945,"snap":2030603.02642825,"snap_percentage":22.9667816836994,"wic":2053169.73745247,"free_lunch":230425.20625237,"free_breakfast":870654.94832879,"food_banks":64948.9706628377},</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3501,39 +3505,39 @@
       </c>
       <c r="C57" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>71.607034542923515</v>
+        <v>71.907951009291054</v>
       </c>
       <c r="D57" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>16.482482827137936</v>
+        <v>6.5474512534119089</v>
       </c>
       <c r="E57" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>6231379.3685395839</v>
+        <v>8552613.8724391852</v>
       </c>
       <c r="F57" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>69.191979214351335</v>
+        <v>94.96649879445161</v>
       </c>
       <c r="G57" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2145716.9282255932</v>
+        <v>1721735.989541217</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2299538.3565833261</v>
+        <v>1429488.5820979017</v>
       </c>
       <c r="I57" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>679177.05769020121</v>
+        <v>239235.05231682365</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3762317.7498065163</v>
+        <v>2000679.3594969308</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Somerset","population":9005927.33333333,"food_ins_rate":71.6070345429235,"food_ins_rate_child":16.4824828271379,"snap":6231379.36853958,"snap_percentage":69.1919792143513,"wic":2145716.92822559,"free_lunch":2299538.35658333,"free_breakfast":679177.057690201,"food_banks":3762317.74980652},</v>
+        <v xml:space="preserve">    {"county_name":"Somerset","population":9005927.33333333,"food_ins_rate":71.9079510092911,"food_ins_rate_child":6.54745125341191,"snap":8552613.87243919,"snap_percentage":94.9664987944516,"wic":1721735.98954122,"free_lunch":1429488.5820979,"free_breakfast":239235.052316824,"food_banks":2000679.35949693},</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3545,39 +3549,39 @@
       </c>
       <c r="C58" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>57.988972140274839</v>
+        <v>69.280485808247718</v>
       </c>
       <c r="D58" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.55610178065016003</v>
+        <v>46.840442392228837</v>
       </c>
       <c r="E58" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>6611330.062405616</v>
+        <v>1894938.8708386819</v>
       </c>
       <c r="F58" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>72.094424722507227</v>
+        <v>20.663697998421103</v>
       </c>
       <c r="G58" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>275847.48610485683</v>
+        <v>1622691.2578280803</v>
       </c>
       <c r="H58" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>206667.2619613329</v>
+        <v>226288.69011499471</v>
       </c>
       <c r="I58" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>562234.78885202738</v>
+        <v>730173.90807572263</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>4570805.9900390804</v>
+        <v>3270769.9570165137</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Sullivan","population":9170376.33333333,"food_ins_rate":57.9889721402748,"food_ins_rate_child":0.55610178065016,"snap":6611330.06240562,"snap_percentage":72.0944247225072,"wic":275847.486104857,"free_lunch":206667.261961333,"free_breakfast":562234.788852027,"food_banks":4570805.99003908},</v>
+        <v xml:space="preserve">    {"county_name":"Sullivan","population":9170376.33333333,"food_ins_rate":69.2804858082477,"food_ins_rate_child":46.8404423922288,"snap":1894938.87083868,"snap_percentage":20.6636979984211,"wic":1622691.25782808,"free_lunch":226288.690114995,"free_breakfast":730173.908075723,"food_banks":3270769.95701651},</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3589,39 +3593,39 @@
       </c>
       <c r="C59" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>19.872030424646837</v>
+        <v>6.3826804096280725</v>
       </c>
       <c r="D59" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>13.016665007809426</v>
+        <v>20.688125132444704</v>
       </c>
       <c r="E59" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>9271264.3883966897</v>
+        <v>6895888.931546947</v>
       </c>
       <c r="F59" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>99.319098722611614</v>
+        <v>73.872715185389822</v>
       </c>
       <c r="G59" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2203794.8763005445</v>
+        <v>1661924.039675633</v>
       </c>
       <c r="H59" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>13708.500761611611</v>
+        <v>1029952.6658920045</v>
       </c>
       <c r="I59" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>348024.79064243421</v>
+        <v>670761.71175522974</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2130055.7313137315</v>
+        <v>413990.40947531891</v>
       </c>
       <c r="L59" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Susquehanna","population":9334825.33333333,"food_ins_rate":19.8720304246468,"food_ins_rate_child":13.0166650078094,"snap":9271264.38839669,"snap_percentage":99.3190987226116,"wic":2203794.87630054,"free_lunch":13708.5007616116,"free_breakfast":348024.790642434,"food_banks":2130055.73131373},</v>
+        <v xml:space="preserve">    {"county_name":"Susquehanna","population":9334825.33333333,"food_ins_rate":6.38268040962807,"food_ins_rate_child":20.6881251324447,"snap":6895888.93154695,"snap_percentage":73.8727151853898,"wic":1661924.03967563,"free_lunch":1029952.665892,"free_breakfast":670761.71175523,"food_banks":413990.409475319},</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3633,39 +3637,39 @@
       </c>
       <c r="C60" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>60.7007406366887</v>
+        <v>2.7948889821136857</v>
       </c>
       <c r="D60" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>51.591519008097102</v>
+        <v>18.319615017605251</v>
       </c>
       <c r="E60" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>746017.0315605686</v>
+        <v>7880582.2298401333</v>
       </c>
       <c r="F60" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>7.8534107488902105</v>
+        <v>82.959834123190419</v>
       </c>
       <c r="G60" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>874716.72146143392</v>
+        <v>984695.50300779461</v>
       </c>
       <c r="H60" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>221361.08666674033</v>
+        <v>1375850.7645911938</v>
       </c>
       <c r="I60" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>447659.33290596213</v>
+        <v>788236.90373542311</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1988035.5622896035</v>
+        <v>4601412.1327538835</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Tioga","population":9499274.33333333,"food_ins_rate":60.7007406366887,"food_ins_rate_child":51.5915190080971,"snap":746017.031560569,"snap_percentage":7.85341074889021,"wic":874716.721461434,"free_lunch":221361.08666674,"free_breakfast":447659.332905962,"food_banks":1988035.5622896},</v>
+        <v xml:space="preserve">    {"county_name":"Tioga","population":9499274.33333333,"food_ins_rate":2.79488898211369,"food_ins_rate_child":18.3196150176053,"snap":7880582.22984013,"snap_percentage":82.9598341231904,"wic":984695.503007795,"free_lunch":1375850.76459119,"free_breakfast":788236.903735423,"food_banks":4601412.13275388},</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3677,39 +3681,39 @@
       </c>
       <c r="C61" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>17.78833389469122</v>
+        <v>53.596366650348216</v>
       </c>
       <c r="D61" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>18.568352635498449</v>
+        <v>36.196721182049245</v>
       </c>
       <c r="E61" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3035384.4229485793</v>
+        <v>3137642.3428816153</v>
       </c>
       <c r="F61" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>31.410092344826857</v>
+        <v>32.468255088169428</v>
       </c>
       <c r="G61" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>982808.60575843917</v>
+        <v>1421731.5856646134</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3537852.7664372306</v>
+        <v>3240268.2559417728</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>396913.72346424428</v>
+        <v>683291.358545603</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2312152.0456328732</v>
+        <v>373306.0997732472</v>
       </c>
       <c r="L61" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Union","population":9663723.33333333,"food_ins_rate":17.7883338946912,"food_ins_rate_child":18.5683526354984,"snap":3035384.42294858,"snap_percentage":31.4100923448269,"wic":982808.605758439,"free_lunch":3537852.76643723,"free_breakfast":396913.723464244,"food_banks":2312152.04563287},</v>
+        <v xml:space="preserve">    {"county_name":"Union","population":9663723.33333333,"food_ins_rate":53.5963666503482,"food_ins_rate_child":36.1967211820492,"snap":3137642.34288162,"snap_percentage":32.4682550881694,"wic":1421731.58566461,"free_lunch":3240268.25594177,"free_breakfast":683291.358545603,"food_banks":373306.099773247},</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3721,39 +3725,39 @@
       </c>
       <c r="C62" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>56.140674625522436</v>
+        <v>64.910954028836713</v>
       </c>
       <c r="D62" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>26.914664001769971</v>
+        <v>55.204912154881583</v>
       </c>
       <c r="E62" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1475141.7690543248</v>
+        <v>9645557.7211998571</v>
       </c>
       <c r="F62" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>15.009319322283543</v>
+        <v>98.141927044623387</v>
       </c>
       <c r="G62" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1677877.7495011373</v>
+        <v>700537.31876299717</v>
       </c>
       <c r="H62" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3531979.8774988889</v>
+        <v>2512865.734050137</v>
       </c>
       <c r="I62" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>815579.47248483589</v>
+        <v>652902.61491725082</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3982735.7956256913</v>
+        <v>1736594.24500271</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Venango","population":9828172.33333333,"food_ins_rate":56.1406746255224,"food_ins_rate_child":26.91466400177,"snap":1475141.76905432,"snap_percentage":15.0093193222835,"wic":1677877.74950114,"free_lunch":3531979.87749889,"free_breakfast":815579.472484836,"food_banks":3982735.79562569},</v>
+        <v xml:space="preserve">    {"county_name":"Venango","population":9828172.33333333,"food_ins_rate":64.9109540288367,"food_ins_rate_child":55.2049121548816,"snap":9645557.72119986,"snap_percentage":98.1419270446234,"wic":700537.318762997,"free_lunch":2512865.73405014,"free_breakfast":652902.614917251,"food_banks":1736594.24500271},</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3765,39 +3769,39 @@
       </c>
       <c r="C63" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>28.142920672806383</v>
+        <v>44.147445009391447</v>
       </c>
       <c r="D63" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>7.9210052638475981</v>
+        <v>18.368945668018309</v>
       </c>
       <c r="E63" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3649817.6129697477</v>
+        <v>3518885.1653293925</v>
       </c>
       <c r="F63" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>36.525126803261386</v>
+        <v>35.214835506586397</v>
       </c>
       <c r="G63" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1664903.1702484733</v>
+        <v>2328846.2743920023</v>
       </c>
       <c r="H63" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3522626.4880793761</v>
+        <v>1273201.5887286405</v>
       </c>
       <c r="I63" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>873364.05803692655</v>
+        <v>118159.75424120449</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>16107.226008719224</v>
+        <v>86452.192943038244</v>
       </c>
       <c r="L63" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Warren","population":9992621.33333333,"food_ins_rate":28.1429206728064,"food_ins_rate_child":7.9210052638476,"snap":3649817.61296975,"snap_percentage":36.5251268032614,"wic":1664903.17024847,"free_lunch":3522626.48807938,"free_breakfast":873364.058036927,"food_banks":16107.2260087192},</v>
+        <v xml:space="preserve">    {"county_name":"Warren","population":9992621.33333333,"food_ins_rate":44.1474450093914,"food_ins_rate_child":18.3689456680183,"snap":3518885.16532939,"snap_percentage":35.2148355065864,"wic":2328846.274392,"free_lunch":1273201.58872864,"free_breakfast":118159.754241204,"food_banks":86452.1929430382},</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3809,39 +3813,39 @@
       </c>
       <c r="C64" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>43.619620299777097</v>
+        <v>90.987343366714086</v>
       </c>
       <c r="D64" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>35.417109183625136</v>
+        <v>19.885648198272165</v>
       </c>
       <c r="E64" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2083903.7185509277</v>
+        <v>3760627.4054647605</v>
       </c>
       <c r="F64" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>20.516779446845103</v>
+        <v>37.024725457725715</v>
       </c>
       <c r="G64" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1234848.0441835423</v>
+        <v>1107391.245943405</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>635597.71405168029</v>
+        <v>2597379.673642226</v>
       </c>
       <c r="I64" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>992708.48815770017</v>
+        <v>41166.220770153195</v>
       </c>
       <c r="J64" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2365240.0494779632</v>
+        <v>1584300.1119977192</v>
       </c>
       <c r="L64" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Washington","population":10157070.3333333,"food_ins_rate":43.6196202997771,"food_ins_rate_child":35.4171091836251,"snap":2083903.71855093,"snap_percentage":20.5167794468451,"wic":1234848.04418354,"free_lunch":635597.71405168,"free_breakfast":992708.4881577,"food_banks":2365240.04947796},</v>
+        <v xml:space="preserve">    {"county_name":"Washington","population":10157070.3333333,"food_ins_rate":90.9873433667141,"food_ins_rate_child":19.8856481982722,"snap":3760627.40546476,"snap_percentage":37.0247254577257,"wic":1107391.2459434,"free_lunch":2597379.67364223,"free_breakfast":41166.2207701532,"food_banks":1584300.11199772},</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3853,39 +3857,39 @@
       </c>
       <c r="C65" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>67.960869252310033</v>
+        <v>65.006257690267915</v>
       </c>
       <c r="D65" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>13.306487162879211</v>
+        <v>2.7979857491940563</v>
       </c>
       <c r="E65" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4179474.3141786475</v>
+        <v>3551134.693792901</v>
       </c>
       <c r="F65" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>40.492820671091067</v>
+        <v>34.405154697763606</v>
       </c>
       <c r="G65" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>849624.18953987327</v>
+        <v>2233754.4163064589</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3243313.8678900446</v>
+        <v>940131.46078555577</v>
       </c>
       <c r="I65" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>705176.0554106764</v>
+        <v>914635.55219932366</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2692140.6389423888</v>
+        <v>4788840.4227782981</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Wayne","population":10321519.3333333,"food_ins_rate":67.96086925231,"food_ins_rate_child":13.3064871628792,"snap":4179474.31417865,"snap_percentage":40.4928206710911,"wic":849624.189539873,"free_lunch":3243313.86789004,"free_breakfast":705176.055410676,"food_banks":2692140.63894239},</v>
+        <v xml:space="preserve">    {"county_name":"Wayne","population":10321519.3333333,"food_ins_rate":65.0062576902679,"food_ins_rate_child":2.79798574919406,"snap":3551134.6937929,"snap_percentage":34.4051546977636,"wic":2233754.41630646,"free_lunch":940131.460785556,"free_breakfast":914635.552199324,"food_banks":4788840.4227783},</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3897,39 +3901,39 @@
       </c>
       <c r="C66" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>74.371840133866399</v>
+        <v>69.791147773798144</v>
       </c>
       <c r="D66" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>50.478054215415433</v>
+        <v>44.939617209532663</v>
       </c>
       <c r="E66" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4591597.5513552176</v>
+        <v>9391497.1863019131</v>
       </c>
       <c r="F66" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>43.788016570288754</v>
+        <v>89.562517144437393</v>
       </c>
       <c r="G66" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2854987.1609225473</v>
+        <v>48803.811105629546</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>929492.33654573024</v>
+        <v>1901125.4917719346</v>
       </c>
       <c r="I66" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>366967.87776801316</v>
+        <v>1033209.6998546536</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1976944.9934908252</v>
+        <v>4758826.9724563705</v>
       </c>
       <c r="L66" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Westmoreland","population":10485968.3333333,"food_ins_rate":74.3718401338664,"food_ins_rate_child":50.4780542154154,"snap":4591597.55135522,"snap_percentage":43.7880165702888,"wic":2854987.16092255,"free_lunch":929492.33654573,"free_breakfast":366967.877768013,"food_banks":1976944.99349083},</v>
+        <v xml:space="preserve">    {"county_name":"Westmoreland","population":10485968.3333333,"food_ins_rate":69.7911477737981,"food_ins_rate_child":44.9396172095327,"snap":9391497.18630191,"snap_percentage":89.5625171444374,"wic":48803.8111056295,"free_lunch":1901125.49177193,"free_breakfast":1033209.69985465,"food_banks":4758826.97245637},</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3941,39 +3945,39 @@
       </c>
       <c r="C67" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>28.685521280376701</v>
+        <v>70.571770391435138</v>
       </c>
       <c r="D67" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>44.443304183949252</v>
+        <v>11.810318150117043</v>
       </c>
       <c r="E67" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>703102.68670925533</v>
+        <v>5198990.4605782395</v>
       </c>
       <c r="F67" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>6.6016444680407904</v>
+        <v>48.814898964631389</v>
       </c>
       <c r="G67" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2994716.5779253826</v>
+        <v>738542.10076529894</v>
       </c>
       <c r="H67" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>700496.08374333277</v>
+        <v>369990.5801027313</v>
       </c>
       <c r="I67" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>944140.26420048333</v>
+        <v>749892.30490453297</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2718317.8401419115</v>
+        <v>3968927.6829466848</v>
       </c>
       <c r="L67" t="str">
         <f t="shared" ref="L67:L68" ca="1" si="17">CONCATENATE("    {""",$A$1,""":""",$A67,""",""",$B$1,""":",$B67,",""",$C$1,""":",$C67,",""",$D$1,""":",$D67,",""",$E$1,""":",$E67,",""",$F$1,""":",$F67,",""",$G$1,""":",$G67,",""",$H$1,""":",$H67,",""",$I$1,""":",$I67,",""",$J$1,""":",$J67,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Wyoming","population":10650417.3333333,"food_ins_rate":28.6855212803767,"food_ins_rate_child":44.4433041839493,"snap":703102.686709255,"snap_percentage":6.60164446804079,"wic":2994716.57792538,"free_lunch":700496.083743333,"free_breakfast":944140.264200483,"food_banks":2718317.84014191},</v>
+        <v xml:space="preserve">    {"county_name":"Wyoming","population":10650417.3333333,"food_ins_rate":70.5717703914351,"food_ins_rate_child":11.810318150117,"snap":5198990.46057824,"snap_percentage":48.8148989646314,"wic":738542.100765299,"free_lunch":369990.580102731,"free_breakfast":749892.304904533,"food_banks":3968927.68294668},</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -3985,39 +3989,39 @@
       </c>
       <c r="C68" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>19.523385590154707</v>
+        <v>4.8459161004696156</v>
       </c>
       <c r="D68" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>54.308369060316693</v>
+        <v>31.693069950589408</v>
       </c>
       <c r="E68" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>9311621.7644186113</v>
+        <v>2549531.7851729686</v>
       </c>
       <c r="F68" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>86.100202049826294</v>
+        <v>23.574325438631337</v>
       </c>
       <c r="G68" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>740590.23938354466</v>
+        <v>538646.09215720568</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2813270.4556857129</v>
+        <v>299756.09051681875</v>
       </c>
       <c r="I68" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>583470.6839531603</v>
+        <v>321917.71213293995</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1257330.6727516237</v>
+        <v>1892458.6007830016</v>
       </c>
       <c r="L68" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v xml:space="preserve">    {"county_name":"York","population":10814866.3333333,"food_ins_rate":19.5233855901547,"food_ins_rate_child":54.3083690603167,"snap":9311621.76441861,"snap_percentage":86.1002020498263,"wic":740590.239383545,"free_lunch":2813270.45568571,"free_breakfast":583470.68395316,"food_banks":1257330.67275162},</v>
+        <v xml:space="preserve">    {"county_name":"York","population":10814866.3333333,"food_ins_rate":4.84591610046962,"food_ins_rate_child":31.6930699505894,"snap":2549531.78517297,"snap_percentage":23.5743254386313,"wic":538646.092157206,"free_lunch":299756.090516819,"free_breakfast":321917.71213294,"food_banks":1892458.600783},</v>
       </c>
     </row>
   </sheetData>
@@ -4052,7 +4056,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
         <v>77</v>
@@ -4066,14 +4070,14 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE("    {""",$A$1,""":""",$A2,""",""",$B$1,""":""",$B2,""",""",$C$1,""":""",$C2,"""},")</f>
-        <v xml:space="preserve">    {"name":"county_name","class":"header","description":"County"},</v>
+        <v xml:space="preserve">    {"name":"county_name","class":"header","description":"Hunger In"},</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4081,7 +4085,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -4096,7 +4100,7 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -4111,7 +4115,7 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>81</v>
@@ -4126,7 +4130,7 @@
         <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>82</v>
@@ -4141,7 +4145,7 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>83</v>
@@ -4156,7 +4160,7 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>84</v>
@@ -4171,10 +4175,10 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -4186,7 +4190,7 @@
         <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>85</v>
@@ -4201,7 +4205,7 @@
         <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
added format to numbers in EXCEL
</commit_message>
<xml_diff>
--- a/SourceData/CountyData.xlsx
+++ b/SourceData/CountyData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33180" windowHeight="19800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33180" windowHeight="19800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Fields" sheetId="2" r:id="rId2"/>
+    <sheet name="Calculations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
   <si>
     <t>Adams</t>
   </si>
@@ -299,13 +300,58 @@
   </si>
   <si>
     <t>Hunger In</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>secondary_header</t>
+  </si>
+  <si>
+    <t>How Nutrition Programs Help</t>
+  </si>
+  <si>
+    <t>#,###</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,6 +392,13 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -364,7 +417,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -426,15 +479,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -465,6 +545,19 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -495,6 +588,19 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -696,12 +802,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:E12" totalsRowShown="0">
+  <autoFilter ref="A1:E12"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column"/>
+    <tableColumn id="5" name="name"/>
     <tableColumn id="2" name="class"/>
     <tableColumn id="3" name="description"/>
+    <tableColumn id="4" name="Format"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1031,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L68"/>
+    <sheetView tabSelected="1" topLeftCell="I43" workbookViewId="0">
+      <selection activeCell="L68" sqref="L2:L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1075,6 +1183,7 @@
       <c r="J1" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -1085,39 +1194,39 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C33" ca="1" si="0">RAND()*100</f>
-        <v>41.458591741032095</v>
+        <v>20.69490678557192</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:D33" ca="1" si="1">RAND()/5*300</f>
-        <v>31.274913856770159</v>
+        <v>18.949590822631404</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E33" ca="1" si="2">RAND()*$B2</f>
-        <v>12239.720248255968</v>
+        <v>4971.6656257914174</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" ref="F2:F33" ca="1" si="3">$E2/$B2*100</f>
-        <v>99.147187106164182</v>
+        <v>40.272706567771706</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" ref="G2:G33" ca="1" si="4">$B2*0.3*RAND()</f>
-        <v>2179.3673440666043</v>
+        <v>473.44078138652765</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H33" ca="1" si="5">$B2*0.4*RAND()</f>
-        <v>3097.1719656339255</v>
+        <v>2155.0224444128894</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" ref="I2:I33" ca="1" si="6">$B2*0.1*RAND()</f>
-        <v>607.47543320553302</v>
+        <v>210.53416536919644</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" ref="J2:J33" ca="1" si="7">$B2*0.5*RAND()</f>
-        <v>4983.2365000011632</v>
+        <v>4212.1093673605583</v>
       </c>
       <c r="L2" t="str">
-        <f ca="1">CONCATENATE("    {""",$A$1,""":""",$A2,""",""",$B$1,""":",$B2,",""",$C$1,""":",$C2,",""",$D$1,""":",$D2,",""",$E$1,""":",$E2,",""",$F$1,""":",$F2,",""",$G$1,""":",$G2,",""",$H$1,""":",$H2,",""",$I$1,""":",$I2,",""",$J$1,""":",$J2,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Adams","population":12345,"food_ins_rate":41.4585917410321,"food_ins_rate_child":31.2749138567702,"snap":12239.720248256,"snap_percentage":99.1471871061642,"wic":2179.3673440666,"free_lunch":3097.17196563393,"free_breakfast":607.475433205533,"food_banks":4983.23650000116},</v>
+        <f ca="1">CONCATENATE("    {","""",$A$1,""":""",TEXT($A2,""),""",","""",$B$1,""":""",TEXT($B2,"#,###"),""",","""",$C$1,""":""",TEXT($C2,"#,###"),""",","""",$D$1,""":""",TEXT($D2,"#,###"),""",","""",$E$1,""":""",TEXT($E2,"#,###"),""",","""",$F$1,""":""",TEXT($F2,"#,###"),""",","""",$G$1,""":""",TEXT($G2,"#,###"),""",","""",$H$1,""":""",TEXT($H2,"#,###"),""",","""",$I$1,""":""",TEXT($I2,"#,###"),""",","""",$J$1,""":""",TEXT($J2,"#,###"),"""},")</f>
+        <v xml:space="preserve">    {"county_name":"Adams","population":"12,345","food_ins_rate":"21","food_ins_rate_child":"19","snap":"4,972","snap_percentage":"40","wic":"473","free_lunch":"2,155","free_breakfast":"211","food_banks":"4,212"},</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1129,39 +1238,39 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>58.586738287738207</v>
+        <v>65.405167777756887</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6737893234927554</v>
+        <v>17.959709565536055</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>22790.018591152901</v>
+        <v>9950.2472850103422</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>97.160720460235765</v>
+        <v>42.420904182342866</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>5368.0507982040463</v>
+        <v>3918.1502230963097</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>7029.4031370170605</v>
+        <v>7829.0039364336089</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>1002.2953689311696</v>
+        <v>426.37634513530799</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>4862.2385507056661</v>
+        <v>3427.1332712835133</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L66" ca="1" si="8">CONCATENATE("    {""",$A$1,""":""",$A3,""",""",$B$1,""":",$B3,",""",$C$1,""":",$C3,",""",$D$1,""":",$D3,",""",$E$1,""":",$E3,",""",$F$1,""":",$F3,",""",$G$1,""":",$G3,",""",$H$1,""":",$H3,",""",$I$1,""":",$I3,",""",$J$1,""":",$J3,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Allegheny","population":23456,"food_ins_rate":58.5867382877382,"food_ins_rate_child":5.67378932349276,"snap":22790.0185911529,"snap_percentage":97.1607204602358,"wic":5368.05079820405,"free_lunch":7029.40313701706,"free_breakfast":1002.29536893117,"food_banks":4862.23855070567},</v>
+        <f t="shared" ref="L3:L66" ca="1" si="8">CONCATENATE("    {","""",$A$1,""":""",TEXT($A3,""),""",","""",$B$1,""":""",TEXT($B3,"#,###"),""",","""",$C$1,""":""",TEXT($C3,"#,###"),""",","""",$D$1,""":""",TEXT($D3,"#,###"),""",","""",$E$1,""":""",TEXT($E3,"#,###"),""",","""",$F$1,""":""",TEXT($F3,"#,###"),""",","""",$G$1,""":""",TEXT($G3,"#,###"),""",","""",$H$1,""":""",TEXT($H3,"#,###"),""",","""",$I$1,""":""",TEXT($I3,"#,###"),""",","""",$J$1,""":""",TEXT($J3,"#,###"),"""},")</f>
+        <v xml:space="preserve">    {"county_name":"Allegheny","population":"23,456","food_ins_rate":"65","food_ins_rate_child":"18","snap":"9,950","snap_percentage":"42","wic":"3,918","free_lunch":"7,829","free_breakfast":"426","food_banks":"3,427"},</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1173,39 +1282,39 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>94.513255511326292</v>
+        <v>67.23180183151139</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2858513243607046</v>
+        <v>44.32395768697787</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>90504.628955998021</v>
+        <v>159454.64699611222</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>26.522047032759065</v>
+        <v>46.727594997146383</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>56770.231414441449</v>
+        <v>8512.963394523058</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>93843.195586220711</v>
+        <v>94053.292536670109</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>32573.392037855225</v>
+        <v>32601.96988801891</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>82890.687714335319</v>
+        <v>140944.44764142524</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Armstrong","population":341243,"food_ins_rate":94.5132555113263,"food_ins_rate_child":5.2858513243607,"snap":90504.628955998,"snap_percentage":26.5220470327591,"wic":56770.2314144414,"free_lunch":93843.1955862207,"free_breakfast":32573.3920378552,"food_banks":82890.6877143353},</v>
+        <v xml:space="preserve">    {"county_name":"Armstrong","population":"341,243","food_ins_rate":"67","food_ins_rate_child":"44","snap":"159,455","snap_percentage":"47","wic":"8,513","free_lunch":"94,053","free_breakfast":"32,602","food_banks":"140,944"},</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1217,39 +1326,39 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>56.581886944944472</v>
+        <v>45.627794420172386</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>47.603211762799432</v>
+        <v>47.285335205360745</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>421639.68990952399</v>
+        <v>310028.84854999691</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>92.753818528821</v>
+        <v>68.201263413499618</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>27830.594149276505</v>
+        <v>8220.9094035585713</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>66539.778264051274</v>
+        <v>75697.613663047669</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>1108.1639928854734</v>
+        <v>42917.628933297397</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>199765.7188124939</v>
+        <v>106409.58051465519</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Beaver","population":454579.333333333,"food_ins_rate":56.5818869449445,"food_ins_rate_child":47.6032117627994,"snap":421639.689909524,"snap_percentage":92.753818528821,"wic":27830.5941492765,"free_lunch":66539.7782640513,"free_breakfast":1108.16399288547,"food_banks":199765.718812494},</v>
+        <v xml:space="preserve">    {"county_name":"Beaver","population":"454,579","food_ins_rate":"46","food_ins_rate_child":"47","snap":"310,029","snap_percentage":"68","wic":"8,221","free_lunch":"75,698","free_breakfast":"42,918","food_banks":"106,410"},</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1261,39 +1370,39 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45.899516795551008</v>
+        <v>45.000766202196004</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9157804186767038</v>
+        <v>3.110683196585049</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>305883.45262168068</v>
+        <v>63461.269058992453</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>49.413481766588099</v>
+        <v>10.251755152670849</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>74477.259246345915</v>
+        <v>184855.95980733767</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>177386.77353426843</v>
+        <v>107843.88378874042</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>22913.216332209875</v>
+        <v>5328.8957239255442</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>178904.29326439206</v>
+        <v>173509.14001166384</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bedford","population":619028.333333333,"food_ins_rate":45.899516795551,"food_ins_rate_child":7.9157804186767,"snap":305883.452621681,"snap_percentage":49.4134817665881,"wic":74477.2592463459,"free_lunch":177386.773534268,"free_breakfast":22913.2163322099,"food_banks":178904.293264392},</v>
+        <v xml:space="preserve">    {"county_name":"Bedford","population":"619,028","food_ins_rate":"45","food_ins_rate_child":"3","snap":"63,461","snap_percentage":"10","wic":"184,856","free_lunch":"107,844","free_breakfast":"5,329","food_banks":"173,509"},</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1305,39 +1414,39 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>56.47881632384356</v>
+        <v>15.343266250053322</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>21.109767593956054</v>
+        <v>28.811954027070367</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>58880.584349551289</v>
+        <v>713361.68227331119</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>7.5152888085532332</v>
+        <v>91.050710968023523</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>182931.95261308568</v>
+        <v>189651.36308363819</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>125232.27912124846</v>
+        <v>214789.30454849664</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>59457.879040148451</v>
+        <v>11362.823076136072</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>28720.736980854439</v>
+        <v>369726.07694033888</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Berks","population":783477.333333333,"food_ins_rate":56.4788163238436,"food_ins_rate_child":21.1097675939561,"snap":58880.5843495513,"snap_percentage":7.51528880855323,"wic":182931.952613086,"free_lunch":125232.279121248,"free_breakfast":59457.8790401485,"food_banks":28720.7369808544},</v>
+        <v xml:space="preserve">    {"county_name":"Berks","population":"783,477","food_ins_rate":"15","food_ins_rate_child":"29","snap":"713,362","snap_percentage":"91","wic":"189,651","free_lunch":"214,789","free_breakfast":"11,363","food_banks":"369,726"},</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1349,39 +1458,39 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4736347759086001</v>
+        <v>62.967865314460688</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>36.877130370352496</v>
+        <v>29.580699806091406</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>899043.88035218557</v>
+        <v>864165.37485323823</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>94.843222383193549</v>
+        <v>91.163769215530294</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>43902.728531639194</v>
+        <v>24690.168904963641</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>236988.5180768529</v>
+        <v>67706.969256090219</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>44743.753710414239</v>
+        <v>48127.797628018947</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>311513.73591563554</v>
+        <v>38102.724603273789</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Blair","population":947926.333333333,"food_ins_rate":8.4736347759086,"food_ins_rate_child":36.8771303703525,"snap":899043.880352186,"snap_percentage":94.8432223831935,"wic":43902.7285316392,"free_lunch":236988.518076853,"free_breakfast":44743.7537104142,"food_banks":311513.735915636},</v>
+        <v xml:space="preserve">    {"county_name":"Blair","population":"947,926","food_ins_rate":"63","food_ins_rate_child":"30","snap":"864,165","snap_percentage":"91","wic":"24,690","free_lunch":"67,707","free_breakfast":"48,128","food_banks":"38,103"},</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1393,39 +1502,39 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>50.676975974154281</v>
+        <v>2.4976849124015321</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>57.279512126615309</v>
+        <v>51.528693096490315</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>781168.11945482565</v>
+        <v>158773.04238414069</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>70.225228485963186</v>
+        <v>14.273333615584892</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>136273.02425281669</v>
+        <v>102055.80193540681</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>247333.59015703891</v>
+        <v>105126.87055067529</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>86334.768695962426</v>
+        <v>4151.3211985359167</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>546876.39744595427</v>
+        <v>396200.27730447351</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bradford","population":1112375.33333333,"food_ins_rate":50.6769759741543,"food_ins_rate_child":57.2795121266153,"snap":781168.119454826,"snap_percentage":70.2252284859632,"wic":136273.024252817,"free_lunch":247333.590157039,"free_breakfast":86334.7686959624,"food_banks":546876.397445954},</v>
+        <v xml:space="preserve">    {"county_name":"Bradford","population":"1,112,375","food_ins_rate":"2","food_ins_rate_child":"52","snap":"158,773","snap_percentage":"14","wic":"102,056","free_lunch":"105,127","free_breakfast":"4,151","food_banks":"396,200"},</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1437,39 +1546,39 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>19.881181278818062</v>
+        <v>82.221948828180828</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>40.205084339713231</v>
+        <v>36.787924274551862</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>261603.76059079988</v>
+        <v>208825.87522723895</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>20.488625863500452</v>
+        <v>16.355098330720995</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>302598.42361355858</v>
+        <v>288808.47683125816</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>153158.72268451584</v>
+        <v>266687.11313732527</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>20729.296624419483</v>
+        <v>42415.625586414499</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>225101.46560588505</v>
+        <v>506872.41565063794</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Bucks","population":1276824.33333333,"food_ins_rate":19.8811812788181,"food_ins_rate_child":40.2050843397132,"snap":261603.7605908,"snap_percentage":20.4886258635005,"wic":302598.423613559,"free_lunch":153158.722684516,"free_breakfast":20729.2966244195,"food_banks":225101.465605885},</v>
+        <v xml:space="preserve">    {"county_name":"Bucks","population":"1,276,824","food_ins_rate":"82","food_ins_rate_child":"37","snap":"208,826","snap_percentage":"16","wic":"288,808","free_lunch":"266,687","free_breakfast":"42,416","food_banks":"506,872"},</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1481,39 +1590,39 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3217218137683626</v>
+        <v>62.555854392376439</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0208298444934489</v>
+        <v>27.521984992546635</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>440427.97141340445</v>
+        <v>22296.817097335857</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>30.558254373221281</v>
+        <v>1.5470221075809754</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>188138.17964668403</v>
+        <v>207428.4709790659</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>489129.38639565045</v>
+        <v>573097.29623667372</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>85486.276891398171</v>
+        <v>71144.399625927588</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>592587.55994570826</v>
+        <v>414777.96250898542</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Butler","population":1441273.33333333,"food_ins_rate":2.32172181376836,"food_ins_rate_child":3.02082984449345,"snap":440427.971413404,"snap_percentage":30.5582543732213,"wic":188138.179646684,"free_lunch":489129.38639565,"free_breakfast":85486.2768913982,"food_banks":592587.559945708},</v>
+        <v xml:space="preserve">    {"county_name":"Butler","population":"1,441,273","food_ins_rate":"63","food_ins_rate_child":"28","snap":"22,297","snap_percentage":"2","wic":"207,428","free_lunch":"573,097","free_breakfast":"71,144","food_banks":"414,778"},</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1525,39 +1634,39 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>38.593428923603355</v>
+        <v>4.7871583091224634</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>13.435754364250553</v>
+        <v>54.718148807753494</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1297297.5677333244</v>
+        <v>1391820.639495058</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>80.792148231522404</v>
+        <v>86.678786898714179</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>115681.08081299183</v>
+        <v>289809.73760635749</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>368560.31438890874</v>
+        <v>424004.17954407248</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>81518.844377948088</v>
+        <v>76421.426274993966</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>414433.79298880242</v>
+        <v>612522.97021472838</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cambria","population":1605722.33333333,"food_ins_rate":38.5934289236034,"food_ins_rate_child":13.4357543642506,"snap":1297297.56773332,"snap_percentage":80.7921482315224,"wic":115681.080812992,"free_lunch":368560.314388909,"free_breakfast":81518.8443779481,"food_banks":414433.792988802},</v>
+        <v xml:space="preserve">    {"county_name":"Cambria","population":"1,605,722","food_ins_rate":"5","food_ins_rate_child":"55","snap":"1,391,821","snap_percentage":"87","wic":"289,810","free_lunch":"424,004","free_breakfast":"76,421","food_banks":"612,523"},</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1569,39 +1678,39 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>51.779471037875688</v>
+        <v>19.596961541090195</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>12.975612044169669</v>
+        <v>3.6391222403837609</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>603492.71140806691</v>
+        <v>941151.61880287935</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>34.092333326382423</v>
+        <v>53.167261331175162</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>118460.17858342091</v>
+        <v>394824.35005457303</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>258778.51112531463</v>
+        <v>553247.23139440373</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>122370.78763868658</v>
+        <v>453.15669992612499</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>189789.7819991718</v>
+        <v>271273.0352197226</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cameron","population":1770171.33333333,"food_ins_rate":51.7794710378757,"food_ins_rate_child":12.9756120441697,"snap":603492.711408067,"snap_percentage":34.0923333263824,"wic":118460.178583421,"free_lunch":258778.511125315,"free_breakfast":122370.787638687,"food_banks":189789.781999172},</v>
+        <v xml:space="preserve">    {"county_name":"Cameron","population":"1,770,171","food_ins_rate":"20","food_ins_rate_child":"4","snap":"941,152","snap_percentage":"53","wic":"394,824","free_lunch":"553,247","free_breakfast":"453","food_banks":"271,273"},</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1613,39 +1722,39 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>68.573162920680247</v>
+        <v>81.982153663655538</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43.217661994883578</v>
+        <v>16.204065125059618</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1595518.342079649</v>
+        <v>609114.1874727325</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>82.47191009982761</v>
+        <v>31.484947045048127</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>442811.76732089167</v>
+        <v>50053.273267848082</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>261921.71898879687</v>
+        <v>406136.83560119971</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>52044.906932278398</v>
+        <v>33730.746846380411</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>778232.31670944078</v>
+        <v>945629.23235238553</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Carbon","population":1934620.33333333,"food_ins_rate":68.5731629206802,"food_ins_rate_child":43.2176619948836,"snap":1595518.34207965,"snap_percentage":82.4719100998276,"wic":442811.767320892,"free_lunch":261921.718988797,"free_breakfast":52044.9069322784,"food_banks":778232.316709441},</v>
+        <v xml:space="preserve">    {"county_name":"Carbon","population":"1,934,620","food_ins_rate":"82","food_ins_rate_child":"16","snap":"609,114","snap_percentage":"31","wic":"50,053","free_lunch":"406,137","free_breakfast":"33,731","food_banks":"945,629"},</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1657,39 +1766,39 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>11.296793773441715</v>
+        <v>67.161517025244308</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>31.98124283274413</v>
+        <v>6.2476627824495417</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>102263.72679936053</v>
+        <v>564184.69774654426</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8718603609422146</v>
+        <v>26.877849568247314</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>195551.55150139079</v>
+        <v>36120.655405494377</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>491849.63150304882</v>
+        <v>714690.98042806692</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>22424.102726983372</v>
+        <v>146059.24026232166</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>859709.16333065892</v>
+        <v>668279.48444190086</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Centre","population":2099069.33333333,"food_ins_rate":11.2967937734417,"food_ins_rate_child":31.9812428327441,"snap":102263.726799361,"snap_percentage":4.87186036094221,"wic":195551.551501391,"free_lunch":491849.631503049,"free_breakfast":22424.1027269833,"food_banks":859709.163330659},</v>
+        <v xml:space="preserve">    {"county_name":"Centre","population":"2,099,069","food_ins_rate":"67","food_ins_rate_child":"6","snap":"564,185","snap_percentage":"27","wic":"36,121","free_lunch":"714,691","free_breakfast":"146,059","food_banks":"668,279"},</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1701,39 +1810,39 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>60.315375912119627</v>
+        <v>68.335985806662208</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>44.715757457821418</v>
+        <v>51.318877306004708</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>256577.08404640897</v>
+        <v>2201492.3963182843</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>11.335321665743493</v>
+        <v>97.259755483239033</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>486498.10431539797</v>
+        <v>634934.58358873078</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>188472.58198415465</v>
+        <v>341678.37368088483</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>2899.1447693190576</v>
+        <v>135706.96401230898</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>643192.25084018265</v>
+        <v>642917.11910769681</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Chester","population":2263518.33333333,"food_ins_rate":60.3153759121196,"food_ins_rate_child":44.7157574578214,"snap":256577.084046409,"snap_percentage":11.3353216657435,"wic":486498.104315398,"free_lunch":188472.581984155,"free_breakfast":2899.14476931906,"food_banks":643192.250840183},</v>
+        <v xml:space="preserve">    {"county_name":"Chester","population":"2,263,518","food_ins_rate":"68","food_ins_rate_child":"51","snap":"2,201,492","snap_percentage":"97","wic":"634,935","free_lunch":"341,678","free_breakfast":"135,707","food_banks":"642,917"},</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1745,39 +1854,39 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>47.347627565587224</v>
+        <v>6.1640263675469491</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>32.110899248668332</v>
+        <v>1.9162415071650885</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>196093.29022783783</v>
+        <v>1933796.2760999426</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>8.0764385721212921</v>
+        <v>79.646717216950961</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>322542.14685696951</v>
+        <v>676395.01500819251</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>173776.13143341703</v>
+        <v>768462.64139134903</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>229539.30277967794</v>
+        <v>77176.680203656288</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>423254.16163344914</v>
+        <v>672620.48261809221</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clarion","population":2427967.33333333,"food_ins_rate":47.3476275655872,"food_ins_rate_child":32.1108992486683,"snap":196093.290227838,"snap_percentage":8.07643857212129,"wic":322542.14685697,"free_lunch":173776.131433417,"free_breakfast":229539.302779678,"food_banks":423254.161633449},</v>
+        <v xml:space="preserve">    {"county_name":"Clarion","population":"2,427,967","food_ins_rate":"6","food_ins_rate_child":"2","snap":"1,933,796","snap_percentage":"80","wic":"676,395","free_lunch":"768,463","free_breakfast":"77,177","food_banks":"672,620"},</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1789,39 +1898,39 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>51.468138509750183</v>
+        <v>18.621371336680337</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>50.426488508328454</v>
+        <v>41.781025406887515</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1911504.7527465736</v>
+        <v>1150976.1751381592</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>73.734481925932002</v>
+        <v>44.397813743837723</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>646421.70623156417</v>
+        <v>190917.41448056008</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>209380.00815711074</v>
+        <v>912306.24852237769</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>126921.14267116688</v>
+        <v>242136.13049037743</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1168412.4925603913</v>
+        <v>182395.07150786879</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clearfield","population":2592416.33333333,"food_ins_rate":51.4681385097502,"food_ins_rate_child":50.4264885083285,"snap":1911504.75274657,"snap_percentage":73.734481925932,"wic":646421.706231564,"free_lunch":209380.008157111,"free_breakfast":126921.142671167,"food_banks":1168412.49256039},</v>
+        <v xml:space="preserve">    {"county_name":"Clearfield","population":"2,592,416","food_ins_rate":"19","food_ins_rate_child":"42","snap":"1,150,976","snap_percentage":"44","wic":"190,917","free_lunch":"912,306","free_breakfast":"242,136","food_banks":"182,395"},</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1833,39 +1942,39 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>54.680404794449686</v>
+        <v>95.531889866011468</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2979408417456684</v>
+        <v>35.615519061035556</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2436332.8910841397</v>
+        <v>739731.17803590745</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>88.37330070592769</v>
+        <v>26.832329061989302</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>205140.06344506444</v>
+        <v>338993.97920915065</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>607496.43857938983</v>
+        <v>327598.25220156676</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>23190.385545499077</v>
+        <v>241478.8662724192</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>456024.29064497456</v>
+        <v>464631.44764416496</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Clinton","population":2756865.33333333,"food_ins_rate":54.6804047944497,"food_ins_rate_child":1.29794084174567,"snap":2436332.89108414,"snap_percentage":88.3733007059277,"wic":205140.063445064,"free_lunch":607496.43857939,"free_breakfast":23190.3855454991,"food_banks":456024.290644975},</v>
+        <v xml:space="preserve">    {"county_name":"Clinton","population":"2,756,865","food_ins_rate":"96","food_ins_rate_child":"36","snap":"739,731","snap_percentage":"27","wic":"338,994","free_lunch":"327,598","free_breakfast":"241,479","food_banks":"464,631"},</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1877,39 +1986,39 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>41.818062852804395</v>
+        <v>15.380983515999658</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9458525482828488</v>
+        <v>52.592545408744762</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2821259.7608727496</v>
+        <v>487768.45709402405</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>96.57501518001952</v>
+        <v>16.696883711841505</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>154962.55415561868</v>
+        <v>822565.07192197733</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>515571.87058078591</v>
+        <v>924999.45799657481</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>232583.90151736033</v>
+        <v>159732.61378025851</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>835116.03076987411</v>
+        <v>451368.34151259722</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Columbia","population":2921314.33333333,"food_ins_rate":41.8180628528044,"food_ins_rate_child":3.94585254828285,"snap":2821259.76087275,"snap_percentage":96.5750151800195,"wic":154962.554155619,"free_lunch":515571.870580786,"free_breakfast":232583.90151736,"food_banks":835116.030769874},</v>
+        <v xml:space="preserve">    {"county_name":"Columbia","population":"2,921,314","food_ins_rate":"15","food_ins_rate_child":"53","snap":"487,768","snap_percentage":"17","wic":"822,565","free_lunch":"924,999","free_breakfast":"159,733","food_banks":"451,368"},</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1921,39 +2030,39 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>41.839628104515349</v>
+        <v>91.588947475854653</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56677867150193517</v>
+        <v>8.5117663491714364</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1522454.3960007026</v>
+        <v>1747111.5107718252</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>49.338015639589045</v>
+        <v>56.618454561923429</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>534735.2686316499</v>
+        <v>277070.38298838894</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>724262.05314076226</v>
+        <v>761545.6672416199</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>198080.49483495724</v>
+        <v>34919.897357940536</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>485854.8967208016</v>
+        <v>1453714.376910401</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Crawford","population":3085763.33333333,"food_ins_rate":41.8396281045153,"food_ins_rate_child":0.566778671501935,"snap":1522454.3960007,"snap_percentage":49.338015639589,"wic":534735.26863165,"free_lunch":724262.053140762,"free_breakfast":198080.494834957,"food_banks":485854.896720802},</v>
+        <v xml:space="preserve">    {"county_name":"Crawford","population":"3,085,763","food_ins_rate":"92","food_ins_rate_child":"9","snap":"1,747,112","snap_percentage":"57","wic":"277,070","free_lunch":"761,546","free_breakfast":"34,920","food_banks":"1,453,714"},</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1965,39 +2074,39 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>38.364073856350203</v>
+        <v>80.450681182548905</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>24.591605646303819</v>
+        <v>25.57356471159391</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2290062.0670672641</v>
+        <v>529593.3502761001</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>70.458844906253802</v>
+        <v>16.294115459618709</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>137934.36821345365</v>
+        <v>568445.11095397326</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1106323.767848134</v>
+        <v>135275.58562805681</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>83815.444611258237</v>
+        <v>228508.2424630319</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1295183.3728501159</v>
+        <v>653611.09859596845</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Cumberland","population":3250212.33333333,"food_ins_rate":38.3640738563502,"food_ins_rate_child":24.5916056463038,"snap":2290062.06706726,"snap_percentage":70.4588449062538,"wic":137934.368213454,"free_lunch":1106323.76784813,"free_breakfast":83815.4446112582,"food_banks":1295183.37285012},</v>
+        <v xml:space="preserve">    {"county_name":"Cumberland","population":"3,250,212","food_ins_rate":"80","food_ins_rate_child":"26","snap":"529,593","snap_percentage":"16","wic":"568,445","free_lunch":"135,276","free_breakfast":"228,508","food_banks":"653,611"},</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2009,39 +2118,39 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>61.43851179315093</v>
+        <v>17.769509330227784</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>38.623024262452994</v>
+        <v>2.5556533075327836</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1629967.5603367751</v>
+        <v>694279.19698364055</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>47.734384210384647</v>
+        <v>20.332300313539374</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>137194.1276644287</v>
+        <v>459903.272442432</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>386078.39767081587</v>
+        <v>722379.30716613319</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>103168.86701338648</v>
+        <v>12525.807410831663</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1517736.4029582578</v>
+        <v>1389479.2194770884</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Dauphin","population":3414661.33333333,"food_ins_rate":61.4385117931509,"food_ins_rate_child":38.623024262453,"snap":1629967.56033678,"snap_percentage":47.7343842103846,"wic":137194.127664429,"free_lunch":386078.397670816,"free_breakfast":103168.867013386,"food_banks":1517736.40295826},</v>
+        <v xml:space="preserve">    {"county_name":"Dauphin","population":"3,414,661","food_ins_rate":"18","food_ins_rate_child":"3","snap":"694,279","snap_percentage":"20","wic":"459,903","free_lunch":"722,379","free_breakfast":"12,526","food_banks":"1,389,479"},</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2053,39 +2162,39 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>89.903335885593052</v>
+        <v>6.1544093228125263</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>27.418590992797679</v>
+        <v>35.162087687766331</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1892170.6641147637</v>
+        <v>2827627.5187032036</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>52.8670671728784</v>
+        <v>79.003642116552228</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>390344.19551190373</v>
+        <v>580472.65335096268</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1289922.8510374222</v>
+        <v>110183.56743030848</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>122203.38361026117</v>
+        <v>169453.55608537458</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1707167.6486449135</v>
+        <v>1329564.0811601358</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Delaware","population":3579110.33333333,"food_ins_rate":89.9033358855931,"food_ins_rate_child":27.4185909927977,"snap":1892170.66411476,"snap_percentage":52.8670671728784,"wic":390344.195511904,"free_lunch":1289922.85103742,"free_breakfast":122203.383610261,"food_banks":1707167.64864491},</v>
+        <v xml:space="preserve">    {"county_name":"Delaware","population":"3,579,110","food_ins_rate":"6","food_ins_rate_child":"35","snap":"2,827,628","snap_percentage":"79","wic":"580,473","free_lunch":"110,184","free_breakfast":"169,454","food_banks":"1,329,564"},</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2097,39 +2206,39 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>80.38603761359704</v>
+        <v>11.485310182505081</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>31.303776632250667</v>
+        <v>37.5263742295135</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3167256.1616043877</v>
+        <v>937812.75423049333</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>84.605475153086672</v>
+        <v>25.051366112459839</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>436049.64136435027</v>
+        <v>448557.67373285908</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>145998.88638813447</v>
+        <v>1143428.9341848025</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>206180.45084098124</v>
+        <v>140248.57917502723</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1853749.3749176369</v>
+        <v>781060.48044796032</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Elk","population":3743559.33333333,"food_ins_rate":80.386037613597,"food_ins_rate_child":31.3037766322507,"snap":3167256.16160439,"snap_percentage":84.6054751530867,"wic":436049.64136435,"free_lunch":145998.886388134,"free_breakfast":206180.450840981,"food_banks":1853749.37491764},</v>
+        <v xml:space="preserve">    {"county_name":"Elk","population":"3,743,559","food_ins_rate":"11","food_ins_rate_child":"38","snap":"937,813","snap_percentage":"25","wic":"448,558","free_lunch":"1,143,429","free_breakfast":"140,249","food_banks":"781,060"},</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2141,39 +2250,39 @@
       </c>
       <c r="C26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>93.679390531095734</v>
+        <v>38.959582890129866</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>41.770976519016386</v>
+        <v>0.31746123384554847</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1293223.660872503</v>
+        <v>3604196.855954343</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>33.091630072586092</v>
+        <v>92.225925549144065</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>6865.9103293805356</v>
+        <v>920278.79841919069</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>29078.872946265121</v>
+        <v>372032.91626142926</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>149902.71520597814</v>
+        <v>209365.95316138156</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>199050.7279742728</v>
+        <v>366166.27710326965</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Erie","population":3908008.33333333,"food_ins_rate":93.6793905310957,"food_ins_rate_child":41.7709765190164,"snap":1293223.6608725,"snap_percentage":33.0916300725861,"wic":6865.91032938054,"free_lunch":29078.8729462651,"free_breakfast":149902.715205978,"food_banks":199050.727974273},</v>
+        <v xml:space="preserve">    {"county_name":"Erie","population":"3,908,008","food_ins_rate":"39","food_ins_rate_child":"","snap":"3,604,197","snap_percentage":"92","wic":"920,279","free_lunch":"372,033","free_breakfast":"209,366","food_banks":"366,166"},</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2185,39 +2294,39 @@
       </c>
       <c r="C27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>48.70266821296002</v>
+        <v>63.557124939472978</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>51.497153864789198</v>
+        <v>2.6753628571437704</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2805482.9710079636</v>
+        <v>1469018.8188928021</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>68.889192479560236</v>
+        <v>36.072049346442178</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>543228.58846006833</v>
+        <v>752311.7641427957</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>341214.0611038811</v>
+        <v>1134739.8141306837</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>308255.18696515099</v>
+        <v>311199.34744153923</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>435250.30638820247</v>
+        <v>1726832.5967830317</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Fayette","population":4072457.33333333,"food_ins_rate":48.70266821296,"food_ins_rate_child":51.4971538647892,"snap":2805482.97100796,"snap_percentage":68.8891924795602,"wic":543228.588460068,"free_lunch":341214.061103881,"free_breakfast":308255.186965151,"food_banks":435250.306388202},</v>
+        <v xml:space="preserve">    {"county_name":"Fayette","population":"4,072,457","food_ins_rate":"64","food_ins_rate_child":"3","snap":"1,469,019","snap_percentage":"36","wic":"752,312","free_lunch":"1,134,740","free_breakfast":"311,199","food_banks":"1,726,833"},</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2229,39 +2338,39 @@
       </c>
       <c r="C28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>95.806263696224931</v>
+        <v>17.332857884833651</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>59.370984513046665</v>
+        <v>59.426550024410609</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1891984.279209807</v>
+        <v>2540213.7149591902</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>44.65485262973263</v>
+        <v>59.954445888368525</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>450366.34627320309</v>
+        <v>884359.80614294542</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1622658.8221280782</v>
+        <v>738956.72322086338</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>169714.81771502929</v>
+        <v>125484.53059369896</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>392333.20801926579</v>
+        <v>104327.71504733812</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Forest","population":4236906.33333333,"food_ins_rate":95.8062636962249,"food_ins_rate_child":59.3709845130467,"snap":1891984.27920981,"snap_percentage":44.6548526297326,"wic":450366.346273203,"free_lunch":1622658.82212808,"free_breakfast":169714.817715029,"food_banks":392333.208019266},</v>
+        <v xml:space="preserve">    {"county_name":"Forest","population":"4,236,906","food_ins_rate":"17","food_ins_rate_child":"59","snap":"2,540,214","snap_percentage":"60","wic":"884,360","free_lunch":"738,957","free_breakfast":"125,485","food_banks":"104,328"},</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2273,39 +2382,39 @@
       </c>
       <c r="C29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>30.229130916711988</v>
+        <v>5.3637428193949566</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>16.448941885608548</v>
+        <v>23.352812329165619</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1320072.8147247946</v>
+        <v>3591851.0706356461</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>29.992416307025326</v>
+        <v>81.607841190031507</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>1194067.3112047827</v>
+        <v>53427.549639138699</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1513352.5369227033</v>
+        <v>668902.79154437885</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>236992.83423870758</v>
+        <v>391633.96941674344</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>986305.6699132059</v>
+        <v>732685.76938736287</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Franklin","population":4401355.33333333,"food_ins_rate":30.229130916712,"food_ins_rate_child":16.4489418856085,"snap":1320072.81472479,"snap_percentage":29.9924163070253,"wic":1194067.31120478,"free_lunch":1513352.5369227,"free_breakfast":236992.834238708,"food_banks":986305.669913206},</v>
+        <v xml:space="preserve">    {"county_name":"Franklin","population":"4,401,355","food_ins_rate":"5","food_ins_rate_child":"23","snap":"3,591,851","snap_percentage":"82","wic":"53,428","free_lunch":"668,903","free_breakfast":"391,634","food_banks":"732,686"},</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2317,39 +2426,39 @@
       </c>
       <c r="C30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6739935099318712</v>
+        <v>74.084170861821704</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>12.571477069723207</v>
+        <v>19.058317538860518</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>4305937.4512145156</v>
+        <v>595471.29967793694</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>94.308409578097368</v>
+        <v>13.041980255934549</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>1205003.6794596501</v>
+        <v>360333.05859638366</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>946178.9512248151</v>
+        <v>260889.59576111429</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>403467.84463105845</v>
+        <v>304526.57114226179</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1218608.3558469079</v>
+        <v>1885066.2502251174</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Fulton","population":4565804.33333333,"food_ins_rate":2.67399350993187,"food_ins_rate_child":12.5714770697232,"snap":4305937.45121452,"snap_percentage":94.3084095780974,"wic":1205003.67945965,"free_lunch":946178.951224815,"free_breakfast":403467.844631058,"food_banks":1218608.35584691},</v>
+        <v xml:space="preserve">    {"county_name":"Fulton","population":"4,565,804","food_ins_rate":"74","food_ins_rate_child":"19","snap":"595,471","snap_percentage":"13","wic":"360,333","free_lunch":"260,890","free_breakfast":"304,527","food_banks":"1,885,066"},</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2361,39 +2470,39 @@
       </c>
       <c r="C31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>12.516217864354495</v>
+        <v>6.531152633673754</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>33.640679930523028</v>
+        <v>57.437966797206599</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3498458.1526175006</v>
+        <v>4191031.6713142656</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>73.95921330395629</v>
+        <v>88.600575402182869</v>
       </c>
       <c r="G31" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>426092.88698302588</v>
+        <v>1309068.935620337</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>163811.55041054724</v>
+        <v>1692286.779415926</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>145009.80175187939</v>
+        <v>127700.59235836058</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>704441.00290789083</v>
+        <v>48511.963758414451</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Greene","population":4730253.33333333,"food_ins_rate":12.5162178643545,"food_ins_rate_child":33.640679930523,"snap":3498458.1526175,"snap_percentage":73.9592133039563,"wic":426092.886983026,"free_lunch":163811.550410547,"free_breakfast":145009.801751879,"food_banks":704441.002907891},</v>
+        <v xml:space="preserve">    {"county_name":"Greene","population":"4,730,253","food_ins_rate":"7","food_ins_rate_child":"57","snap":"4,191,032","snap_percentage":"89","wic":"1,309,069","free_lunch":"1,692,287","free_breakfast":"127,701","food_banks":"48,512"},</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2405,39 +2514,39 @@
       </c>
       <c r="C32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>82.383630401516527</v>
+        <v>24.348307089657006</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>51.493260625558598</v>
+        <v>30.745455184775842</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3398321.2869454646</v>
+        <v>1451.5003714600168</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>69.428558786968793</v>
+        <v>2.9654517733901375E-2</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>663339.38411554205</v>
+        <v>769300.04766342998</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1036806.5742620346</v>
+        <v>755782.17565977364</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>433867.14831335563</v>
+        <v>336524.19112649094</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1538468.9728849775</v>
+        <v>1782414.8424067877</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Huntingdon","population":4894702.33333333,"food_ins_rate":82.3836304015165,"food_ins_rate_child":51.4932606255586,"snap":3398321.28694546,"snap_percentage":69.4285587869688,"wic":663339.384115542,"free_lunch":1036806.57426203,"free_breakfast":433867.148313356,"food_banks":1538468.97288498},</v>
+        <v xml:space="preserve">    {"county_name":"Huntingdon","population":"4,894,702","food_ins_rate":"24","food_ins_rate_child":"31","snap":"1,452","snap_percentage":"","wic":"769,300","free_lunch":"755,782","free_breakfast":"336,524","food_banks":"1,782,415"},</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2449,39 +2558,39 @@
       </c>
       <c r="C33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>48.915967192353257</v>
+        <v>25.546072665948593</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>36.408718241713693</v>
+        <v>51.290943585101409</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1120030.371219743</v>
+        <v>1080744.5774006352</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>22.138700691560199</v>
+        <v>21.362171364195255</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>443920.61815436429</v>
+        <v>208878.3563620435</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1841730.5174990506</v>
+        <v>1308614.5572747027</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>24059.416483847232</v>
+        <v>121728.16843017798</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1785357.219256324</v>
+        <v>2052202.7095786966</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Indiana","population":5059151.33333333,"food_ins_rate":48.9159671923533,"food_ins_rate_child":36.4087182417137,"snap":1120030.37121974,"snap_percentage":22.1387006915602,"wic":443920.618154364,"free_lunch":1841730.51749905,"free_breakfast":24059.4164838472,"food_banks":1785357.21925632},</v>
+        <v xml:space="preserve">    {"county_name":"Indiana","population":"5,059,151","food_ins_rate":"26","food_ins_rate_child":"51","snap":"1,080,745","snap_percentage":"21","wic":"208,878","free_lunch":"1,308,615","free_breakfast":"121,728","food_banks":"2,052,203"},</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2493,39 +2602,39 @@
       </c>
       <c r="C34" s="2">
         <f t="shared" ref="C34:C68" ca="1" si="9">RAND()*100</f>
-        <v>44.731856458085673</v>
+        <v>75.165789742232718</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" ref="D34:D68" ca="1" si="10">RAND()/5*300</f>
-        <v>59.247833974968849</v>
+        <v>54.774926138321398</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" ref="E34:E68" ca="1" si="11">RAND()*$B34</f>
-        <v>981924.24341598304</v>
+        <v>2750638.9197183051</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" ref="F34:F68" ca="1" si="12">$E34/$B34*100</f>
-        <v>18.797844030103828</v>
+        <v>52.657913013858838</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" ref="G34:G68" ca="1" si="13">$B34*0.3*RAND()</f>
-        <v>605799.90207983064</v>
+        <v>468737.5022929596</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" ref="H34:H68" ca="1" si="14">$B34*0.4*RAND()</f>
-        <v>758313.28812728415</v>
+        <v>104676.78986413911</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" ref="I34:I68" ca="1" si="15">$B34*0.1*RAND()</f>
-        <v>333922.1017293387</v>
+        <v>134632.16521183343</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" ref="J34:J68" ca="1" si="16">$B34*0.5*RAND()</f>
-        <v>1248694.4349055369</v>
+        <v>766514.71738336748</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Jefferson","population":5223600.33333333,"food_ins_rate":44.7318564580857,"food_ins_rate_child":59.2478339749688,"snap":981924.243415983,"snap_percentage":18.7978440301038,"wic":605799.902079831,"free_lunch":758313.288127284,"free_breakfast":333922.101729339,"food_banks":1248694.43490554},</v>
+        <v xml:space="preserve">    {"county_name":"Jefferson","population":"5,223,600","food_ins_rate":"75","food_ins_rate_child":"55","snap":"2,750,639","snap_percentage":"53","wic":"468,738","free_lunch":"104,677","free_breakfast":"134,632","food_banks":"766,515"},</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2537,39 +2646,39 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>6.888969489726815</v>
+        <v>92.142626998428312</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>28.906173598009666</v>
+        <v>34.777319793882512</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>66590.633857749301</v>
+        <v>3805174.3219790356</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1.2358950287590043</v>
+        <v>70.622484809821799</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>92536.750545643881</v>
+        <v>1384856.2334331528</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2115463.7459848314</v>
+        <v>1459634.7632101579</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>50044.302370462559</v>
+        <v>82673.39146215489</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2674893.9280303884</v>
+        <v>1537173.7639704274</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Juniata","population":5388049.33333333,"food_ins_rate":6.88896948972681,"food_ins_rate_child":28.9061735980097,"snap":66590.6338577493,"snap_percentage":1.235895028759,"wic":92536.7505456439,"free_lunch":2115463.74598483,"free_breakfast":50044.3023704626,"food_banks":2674893.92803039},</v>
+        <v xml:space="preserve">    {"county_name":"Juniata","population":"5,388,049","food_ins_rate":"92","food_ins_rate_child":"35","snap":"3,805,174","snap_percentage":"71","wic":"1,384,856","free_lunch":"1,459,635","free_breakfast":"82,673","food_banks":"1,537,174"},</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2581,39 +2690,39 @@
       </c>
       <c r="C36" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>36.924354926925375</v>
+        <v>77.631040993112038</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>55.964479422340695</v>
+        <v>36.725108689488536</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4909714.9242876852</v>
+        <v>1520148.8786900546</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>88.423528104694398</v>
+        <v>27.377745789929197</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1631949.8346156285</v>
+        <v>1325308.718634187</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>392898.33280602738</v>
+        <v>1404814.2935325275</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>365775.08845406357</v>
+        <v>177789.32777771284</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2278902.3877954967</v>
+        <v>896597.07440692</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lackawanna","population":5552498.33333333,"food_ins_rate":36.9243549269254,"food_ins_rate_child":55.9644794223407,"snap":4909714.92428769,"snap_percentage":88.4235281046944,"wic":1631949.83461563,"free_lunch":392898.332806027,"free_breakfast":365775.088454064,"food_banks":2278902.3877955},</v>
+        <v xml:space="preserve">    {"county_name":"Lackawanna","population":"5,552,498","food_ins_rate":"78","food_ins_rate_child":"37","snap":"1,520,149","snap_percentage":"27","wic":"1,325,309","free_lunch":"1,404,814","free_breakfast":"177,789","food_banks":"896,597"},</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2625,39 +2734,39 @@
       </c>
       <c r="C37" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>46.118830259914091</v>
+        <v>29.18167768907448</v>
       </c>
       <c r="D37" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>41.230600932094248</v>
+        <v>12.307010951536947</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3072690.440455901</v>
+        <v>2306846.2300826008</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>53.747048228697501</v>
+        <v>40.351014196549691</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>377938.92646138219</v>
+        <v>607434.03154894023</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1364126.6316058948</v>
+        <v>1178855.5797674535</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>245386.91429670493</v>
+        <v>18891.793749104792</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1928589.3782266751</v>
+        <v>1703709.1518094079</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lancaster","population":5716947.33333333,"food_ins_rate":46.1188302599141,"food_ins_rate_child":41.2306009320942,"snap":3072690.4404559,"snap_percentage":53.7470482286975,"wic":377938.926461382,"free_lunch":1364126.63160589,"free_breakfast":245386.914296705,"food_banks":1928589.37822668},</v>
+        <v xml:space="preserve">    {"county_name":"Lancaster","population":"5,716,947","food_ins_rate":"29","food_ins_rate_child":"12","snap":"2,306,846","snap_percentage":"40","wic":"607,434","free_lunch":"1,178,856","free_breakfast":"18,892","food_banks":"1,703,709"},</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2669,39 +2778,39 @@
       </c>
       <c r="C38" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>56.615964338046155</v>
+        <v>82.969350723934951</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>24.535695142204339</v>
+        <v>6.0735784202043446</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1982972.1659658288</v>
+        <v>1809320.9445278104</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>33.716009831324577</v>
+        <v>30.763458913206122</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>264257.02172350476</v>
+        <v>1548300.4117773552</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1288242.939057583</v>
+        <v>663875.85741315316</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>269945.07911961124</v>
+        <v>548178.60499609658</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1444714.8766104914</v>
+        <v>1367366.7333138706</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lawrence","population":5881396.33333333,"food_ins_rate":56.6159643380462,"food_ins_rate_child":24.5356951422043,"snap":1982972.16596583,"snap_percentage":33.7160098313246,"wic":264257.021723505,"free_lunch":1288242.93905758,"free_breakfast":269945.079119611,"food_banks":1444714.87661049},</v>
+        <v xml:space="preserve">    {"county_name":"Lawrence","population":"5,881,396","food_ins_rate":"83","food_ins_rate_child":"6","snap":"1,809,321","snap_percentage":"31","wic":"1,548,300","free_lunch":"663,876","free_breakfast":"548,179","food_banks":"1,367,367"},</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2713,39 +2822,39 @@
       </c>
       <c r="C39" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>72.943690416952251</v>
+        <v>7.021789676678047</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>20.895485158415294</v>
+        <v>59.837052388778986</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2977980.7992989365</v>
+        <v>3724431.1249471428</v>
       </c>
       <c r="F39" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>49.25664874157556</v>
+        <v>61.603149263722671</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>777243.43955729879</v>
+        <v>963198.77731936495</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>639099.33015494526</v>
+        <v>839344.95942659897</v>
       </c>
       <c r="I39" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>463336.11050948169</v>
+        <v>267899.49156741571</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1154613.6833935184</v>
+        <v>123232.16352485608</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lebanon","population":6045845.33333333,"food_ins_rate":72.9436904169523,"food_ins_rate_child":20.8954851584153,"snap":2977980.79929894,"snap_percentage":49.2566487415756,"wic":777243.439557299,"free_lunch":639099.330154945,"free_breakfast":463336.110509482,"food_banks":1154613.68339352},</v>
+        <v xml:space="preserve">    {"county_name":"Lebanon","population":"6,045,845","food_ins_rate":"7","food_ins_rate_child":"60","snap":"3,724,431","snap_percentage":"62","wic":"963,199","free_lunch":"839,345","free_breakfast":"267,899","food_banks":"123,232"},</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2757,39 +2866,39 @@
       </c>
       <c r="C40" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>40.108838874294293</v>
+        <v>28.871372478893463</v>
       </c>
       <c r="D40" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>48.257868937441245</v>
+        <v>2.2496931114761121</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>302372.03784377041</v>
+        <v>4009462.8767066505</v>
       </c>
       <c r="F40" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4.8688841722172356</v>
+        <v>64.561559589633816</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>572085.56078867323</v>
+        <v>854986.81459598418</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2460669.0218399758</v>
+        <v>447745.04691318102</v>
       </c>
       <c r="I40" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>32083.365476021874</v>
+        <v>352979.5776001371</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2707348.4224299248</v>
+        <v>291928.15566345112</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lehigh","population":6210294.33333333,"food_ins_rate":40.1088388742943,"food_ins_rate_child":48.2578689374412,"snap":302372.03784377,"snap_percentage":4.86888417221724,"wic":572085.560788673,"free_lunch":2460669.02183998,"free_breakfast":32083.3654760219,"food_banks":2707348.42242992},</v>
+        <v xml:space="preserve">    {"county_name":"Lehigh","population":"6,210,294","food_ins_rate":"29","food_ins_rate_child":"2","snap":"4,009,463","snap_percentage":"65","wic":"854,987","free_lunch":"447,745","free_breakfast":"352,980","food_banks":"291,928"},</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2801,39 +2910,39 @@
       </c>
       <c r="C41" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>99.214153889587791</v>
+        <v>37.622975652221577</v>
       </c>
       <c r="D41" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>32.920585889815477</v>
+        <v>6.9808999311167774</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>339582.35565585952</v>
+        <v>810767.26902920182</v>
       </c>
       <c r="F41" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>5.3269965220433928</v>
+        <v>12.718430007836169</v>
       </c>
       <c r="G41" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1083003.8044366101</v>
+        <v>673942.06094010279</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2366374.4771642587</v>
+        <v>2250257.043606896</v>
       </c>
       <c r="I41" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>446686.85199929815</v>
+        <v>569548.95579992374</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1252864.9226978675</v>
+        <v>1820538.1264474851</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Luzerne","population":6374743.33333333,"food_ins_rate":99.2141538895878,"food_ins_rate_child":32.9205858898155,"snap":339582.35565586,"snap_percentage":5.32699652204339,"wic":1083003.80443661,"free_lunch":2366374.47716426,"free_breakfast":446686.851999298,"food_banks":1252864.92269787},</v>
+        <v xml:space="preserve">    {"county_name":"Luzerne","population":"6,374,743","food_ins_rate":"38","food_ins_rate_child":"7","snap":"810,767","snap_percentage":"13","wic":"673,942","free_lunch":"2,250,257","free_breakfast":"569,549","food_banks":"1,820,538"},</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2845,39 +2954,39 @@
       </c>
       <c r="C42" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>68.809016941462829</v>
+        <v>89.46454290168063</v>
       </c>
       <c r="D42" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>49.185070532726307</v>
+        <v>32.857797384638673</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4037960.1819991581</v>
+        <v>216293.98725818403</v>
       </c>
       <c r="F42" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>61.750136349649495</v>
+        <v>3.3076559953074347</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1885714.739482658</v>
+        <v>1292066.5856253793</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2228603.7891797372</v>
+        <v>500781.7854748182</v>
       </c>
       <c r="I42" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>410537.61383130669</v>
+        <v>215938.65500668914</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1606818.5769046447</v>
+        <v>390010.42988861923</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Lycoming","population":6539192.33333333,"food_ins_rate":68.8090169414628,"food_ins_rate_child":49.1850705327263,"snap":4037960.18199916,"snap_percentage":61.7501363496495,"wic":1885714.73948266,"free_lunch":2228603.78917974,"free_breakfast":410537.613831307,"food_banks":1606818.57690464},</v>
+        <v xml:space="preserve">    {"county_name":"Lycoming","population":"6,539,192","food_ins_rate":"89","food_ins_rate_child":"33","snap":"216,294","snap_percentage":"3","wic":"1,292,067","free_lunch":"500,782","free_breakfast":"215,939","food_banks":"390,010"},</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2889,39 +2998,39 @@
       </c>
       <c r="C43" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>64.11973835365545</v>
+        <v>69.460248137412805</v>
       </c>
       <c r="D43" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>49.260256788505679</v>
+        <v>0.70278117042552823</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1379972.9022332281</v>
+        <v>2416905.2646631654</v>
       </c>
       <c r="F43" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>20.585422662328622</v>
+        <v>36.053618391623878</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1721163.2473356638</v>
+        <v>231745.55728644709</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1198609.5782564161</v>
+        <v>2247030.0159526747</v>
       </c>
       <c r="I43" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>430144.77972968336</v>
+        <v>327150.42431784031</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1738260.3304354087</v>
+        <v>288262.75363644975</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"McKean","population":6703641.33333333,"food_ins_rate":64.1197383536554,"food_ins_rate_child":49.2602567885057,"snap":1379972.90223323,"snap_percentage":20.5854226623286,"wic":1721163.24733566,"free_lunch":1198609.57825642,"free_breakfast":430144.779729683,"food_banks":1738260.33043541},</v>
+        <v xml:space="preserve">    {"county_name":"McKean","population":"6,703,641","food_ins_rate":"69","food_ins_rate_child":"1","snap":"2,416,905","snap_percentage":"36","wic":"231,746","free_lunch":"2,247,030","free_breakfast":"327,150","food_banks":"288,263"},</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2933,39 +3042,39 @@
       </c>
       <c r="C44" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>88.875797565580626</v>
+        <v>26.450622771282283</v>
       </c>
       <c r="D44" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>23.94250073217037</v>
+        <v>12.260381874876982</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>6215838.4431577194</v>
+        <v>2043146.3738383357</v>
       </c>
       <c r="F44" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>90.503155047189807</v>
+        <v>29.74839110548978</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1331100.042869149</v>
+        <v>844975.8105602765</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>556771.93253716989</v>
+        <v>2525974.8120230539</v>
       </c>
       <c r="I44" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>122583.69661096467</v>
+        <v>344968.37558940361</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>411769.32997853647</v>
+        <v>1916346.4007607535</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Mercer","population":6868090.33333333,"food_ins_rate":88.8757975655806,"food_ins_rate_child":23.9425007321704,"snap":6215838.44315772,"snap_percentage":90.5031550471898,"wic":1331100.04286915,"free_lunch":556771.93253717,"free_breakfast":122583.696610965,"food_banks":411769.329978536},</v>
+        <v xml:space="preserve">    {"county_name":"Mercer","population":"6,868,090","food_ins_rate":"26","food_ins_rate_child":"12","snap":"2,043,146","snap_percentage":"30","wic":"844,976","free_lunch":"2,525,975","free_breakfast":"344,968","food_banks":"1,916,346"},</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2977,39 +3086,39 @@
       </c>
       <c r="C45" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>64.130920269302521</v>
+        <v>77.433307192961493</v>
       </c>
       <c r="D45" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6927040766761814</v>
+        <v>58.950816434237744</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1762353.5593061091</v>
+        <v>6832072.3656298155</v>
       </c>
       <c r="F45" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>25.059988658048169</v>
+        <v>97.149436950130834</v>
       </c>
       <c r="G45" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1045319.505735592</v>
+        <v>1621722.4820900755</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1811730.5296935572</v>
+        <v>2673146.9882689598</v>
       </c>
       <c r="I45" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>76604.882598164302</v>
+        <v>280232.28114268935</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>179024.09826824785</v>
+        <v>1513039.1357418906</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Mifflin","population":7032539.33333333,"food_ins_rate":64.1309202693025,"food_ins_rate_child":1.69270407667618,"snap":1762353.55930611,"snap_percentage":25.0599886580482,"wic":1045319.50573559,"free_lunch":1811730.52969356,"free_breakfast":76604.8825981643,"food_banks":179024.098268248},</v>
+        <v xml:space="preserve">    {"county_name":"Mifflin","population":"7,032,539","food_ins_rate":"77","food_ins_rate_child":"59","snap":"6,832,072","snap_percentage":"97","wic":"1,621,722","free_lunch":"2,673,147","free_breakfast":"280,232","food_banks":"1,513,039"},</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -3021,39 +3130,39 @@
       </c>
       <c r="C46" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>77.741610975982354</v>
+        <v>85.171259004608956</v>
       </c>
       <c r="D46" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>59.492699159871165</v>
+        <v>44.205436646462708</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>4724969.6939338176</v>
+        <v>3247189.1139081325</v>
       </c>
       <c r="F46" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>65.652040479901927</v>
+        <v>45.118721380560814</v>
       </c>
       <c r="G46" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>494239.69471980806</v>
+        <v>2111294.645360745</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1903412.4623580782</v>
+        <v>1890144.8014461261</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>87972.99411920266</v>
+        <v>233229.54506445336</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3524435.5007314938</v>
+        <v>1961329.4440545551</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Monroe","population":7196988.33333333,"food_ins_rate":77.7416109759824,"food_ins_rate_child":59.4926991598712,"snap":4724969.69393382,"snap_percentage":65.6520404799019,"wic":494239.694719808,"free_lunch":1903412.46235808,"free_breakfast":87972.9941192027,"food_banks":3524435.50073149},</v>
+        <v xml:space="preserve">    {"county_name":"Monroe","population":"7,196,988","food_ins_rate":"85","food_ins_rate_child":"44","snap":"3,247,189","snap_percentage":"45","wic":"2,111,295","free_lunch":"1,890,145","free_breakfast":"233,230","food_banks":"1,961,329"},</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -3065,39 +3174,39 @@
       </c>
       <c r="C47" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>78.533398650850955</v>
+        <v>28.276168233898602</v>
       </c>
       <c r="D47" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>25.207713780928678</v>
+        <v>54.324162773885526</v>
       </c>
       <c r="E47" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>405911.5088391804</v>
+        <v>1547388.6610786235</v>
       </c>
       <c r="F47" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>5.5140251890914316</v>
+        <v>21.020197428997889</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>725455.66868455661</v>
+        <v>277138.87160754798</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1987419.379157176</v>
+        <v>1637160.650204028</v>
       </c>
       <c r="I47" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>137431.78845179122</v>
+        <v>585058.31467721751</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1897313.7302020125</v>
+        <v>2640434.8500533779</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Montgomery","population":7361437.33333333,"food_ins_rate":78.533398650851,"food_ins_rate_child":25.2077137809287,"snap":405911.50883918,"snap_percentage":5.51402518909143,"wic":725455.668684557,"free_lunch":1987419.37915718,"free_breakfast":137431.788451791,"food_banks":1897313.73020201},</v>
+        <v xml:space="preserve">    {"county_name":"Montgomery","population":"7,361,437","food_ins_rate":"28","food_ins_rate_child":"54","snap":"1,547,389","snap_percentage":"21","wic":"277,139","free_lunch":"1,637,161","free_breakfast":"585,058","food_banks":"2,640,435"},</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -3109,39 +3218,39 @@
       </c>
       <c r="C48" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>32.033953444423481</v>
+        <v>36.901710375152597</v>
       </c>
       <c r="D48" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>44.274480627992006</v>
+        <v>11.096370058070397</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>590189.08394904516</v>
+        <v>3731308.4359072209</v>
       </c>
       <c r="F48" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>7.8421206195342759</v>
+        <v>49.579654417323191</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1879318.8917117002</v>
+        <v>1867060.3350273815</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1288623.5051932479</v>
+        <v>2374288.569353119</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>625796.05463279621</v>
+        <v>249964.26224051823</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2783741.8860831861</v>
+        <v>1336942.6181198354</v>
       </c>
       <c r="L48" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Montour","population":7525886.33333333,"food_ins_rate":32.0339534444235,"food_ins_rate_child":44.274480627992,"snap":590189.083949045,"snap_percentage":7.84212061953428,"wic":1879318.8917117,"free_lunch":1288623.50519325,"free_breakfast":625796.054632796,"food_banks":2783741.88608319},</v>
+        <v xml:space="preserve">    {"county_name":"Montour","population":"7,525,886","food_ins_rate":"37","food_ins_rate_child":"11","snap":"3,731,308","snap_percentage":"50","wic":"1,867,060","free_lunch":"2,374,289","free_breakfast":"249,964","food_banks":"1,336,943"},</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3153,39 +3262,39 @@
       </c>
       <c r="C49" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>46.346036951278322</v>
+        <v>72.721238962416237</v>
       </c>
       <c r="D49" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>18.713210291745007</v>
+        <v>17.104356131660776</v>
       </c>
       <c r="E49" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5014152.8868177244</v>
+        <v>6058523.9973389171</v>
       </c>
       <c r="F49" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>65.200705424172568</v>
+        <v>78.781011942074656</v>
       </c>
       <c r="G49" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>930236.58120120596</v>
+        <v>1241762.2254295612</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2493805.5139749702</v>
+        <v>1972480.3180420699</v>
       </c>
       <c r="I49" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>479988.74249668611</v>
+        <v>94736.136960745993</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>256371.96038328324</v>
+        <v>1154068.198849082</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Northampton","population":7690335.33333333,"food_ins_rate":46.3460369512783,"food_ins_rate_child":18.713210291745,"snap":5014152.88681772,"snap_percentage":65.2007054241726,"wic":930236.581201206,"free_lunch":2493805.51397497,"free_breakfast":479988.742496686,"food_banks":256371.960383283},</v>
+        <v xml:space="preserve">    {"county_name":"Northampton","population":"7,690,335","food_ins_rate":"73","food_ins_rate_child":"17","snap":"6,058,524","snap_percentage":"79","wic":"1,241,762","free_lunch":"1,972,480","free_breakfast":"94,736","food_banks":"1,154,068"},</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3197,39 +3306,39 @@
       </c>
       <c r="C50" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>13.804095799365268</v>
+        <v>48.075376941276026</v>
       </c>
       <c r="D50" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>9.352258607568908</v>
+        <v>18.605752756248744</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2726349.0087564071</v>
+        <v>6023616.2916036025</v>
       </c>
       <c r="F50" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>34.709406306505528</v>
+        <v>76.687226994141596</v>
       </c>
       <c r="G50" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1924028.4956911982</v>
+        <v>1334994.4488773607</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3030073.0276890737</v>
+        <v>2420704.4127844051</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>119332.42099400464</v>
+        <v>493650.52522805781</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3478406.3120919853</v>
+        <v>3080906.5571848433</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Northumberland","population":7854784.33333333,"food_ins_rate":13.8040957993653,"food_ins_rate_child":9.35225860756891,"snap":2726349.00875641,"snap_percentage":34.7094063065055,"wic":1924028.4956912,"free_lunch":3030073.02768907,"free_breakfast":119332.420994005,"food_banks":3478406.31209199},</v>
+        <v xml:space="preserve">    {"county_name":"Northumberland","population":"7,854,784","food_ins_rate":"48","food_ins_rate_child":"19","snap":"6,023,616","snap_percentage":"77","wic":"1,334,994","free_lunch":"2,420,704","free_breakfast":"493,651","food_banks":"3,080,907"},</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3241,39 +3350,39 @@
       </c>
       <c r="C51" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>19.467559282520529</v>
+        <v>75.841908353182447</v>
       </c>
       <c r="D51" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>2.4441152726276072</v>
+        <v>14.647962573307082</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2878011.8265890568</v>
+        <v>5237374.8355567316</v>
       </c>
       <c r="F51" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>35.888865019379132</v>
+        <v>65.310168913363285</v>
       </c>
       <c r="G51" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>426841.92787125503</v>
+        <v>968418.64772630273</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2778610.7969232621</v>
+        <v>2286708.3201709948</v>
       </c>
       <c r="I51" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>781137.73232219962</v>
+        <v>341391.86911904044</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1788364.1637639969</v>
+        <v>3682754.7830257067</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Perry","population":8019233.33333333,"food_ins_rate":19.4675592825205,"food_ins_rate_child":2.44411527262761,"snap":2878011.82658906,"snap_percentage":35.8888650193791,"wic":426841.927871255,"free_lunch":2778610.79692326,"free_breakfast":781137.7323222,"food_banks":1788364.163764},</v>
+        <v xml:space="preserve">    {"county_name":"Perry","population":"8,019,233","food_ins_rate":"76","food_ins_rate_child":"15","snap":"5,237,375","snap_percentage":"65","wic":"968,419","free_lunch":"2,286,708","free_breakfast":"341,392","food_banks":"3,682,755"},</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3285,39 +3394,39 @@
       </c>
       <c r="C52" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>52.955200689133228</v>
+        <v>4.5600958407388088</v>
       </c>
       <c r="D52" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>6.4745779502309864</v>
+        <v>6.9499974153509054</v>
       </c>
       <c r="E52" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>6007440.3643432977</v>
+        <v>1086048.0993012595</v>
       </c>
       <c r="F52" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>73.407545890119877</v>
+        <v>13.27089756255112</v>
       </c>
       <c r="G52" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>512145.35923983698</v>
+        <v>1625080.3993716002</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1706276.7988059928</v>
+        <v>2252640.9029618688</v>
       </c>
       <c r="I52" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>197194.31017971894</v>
+        <v>368568.71289160219</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1914217.8963067243</v>
+        <v>3582558.2727963338</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Philadelphia","population":8183682.33333333,"food_ins_rate":52.9552006891332,"food_ins_rate_child":6.47457795023099,"snap":6007440.3643433,"snap_percentage":73.4075458901199,"wic":512145.359239837,"free_lunch":1706276.79880599,"free_breakfast":197194.310179719,"food_banks":1914217.89630672},</v>
+        <v xml:space="preserve">    {"county_name":"Philadelphia","population":"8,183,682","food_ins_rate":"5","food_ins_rate_child":"7","snap":"1,086,048","snap_percentage":"13","wic":"1,625,080","free_lunch":"2,252,641","free_breakfast":"368,569","food_banks":"3,582,558"},</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3329,39 +3438,39 @@
       </c>
       <c r="C53" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>27.923125888230828</v>
+        <v>75.395624147297141</v>
       </c>
       <c r="D53" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>6.5115486422705837</v>
+        <v>47.276487952433179</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>7731112.6271932218</v>
+        <v>3671616.0806047339</v>
       </c>
       <c r="F53" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>92.608900345441285</v>
+        <v>43.981292746848681</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>950577.32818299253</v>
+        <v>256116.9432087265</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1149890.9772898918</v>
+        <v>1926619.3434887377</v>
       </c>
       <c r="I53" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>367218.64164733252</v>
+        <v>245665.80608108654</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2360907.12577115</v>
+        <v>362617.85886420007</v>
       </c>
       <c r="L53" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Pike","population":8348131.33333333,"food_ins_rate":27.9231258882308,"food_ins_rate_child":6.51154864227058,"snap":7731112.62719322,"snap_percentage":92.6089003454413,"wic":950577.328182993,"free_lunch":1149890.97728989,"free_breakfast":367218.641647333,"food_banks":2360907.12577115},</v>
+        <v xml:space="preserve">    {"county_name":"Pike","population":"8,348,131","food_ins_rate":"75","food_ins_rate_child":"47","snap":"3,671,616","snap_percentage":"44","wic":"256,117","free_lunch":"1,926,619","free_breakfast":"245,666","food_banks":"362,618"},</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3373,39 +3482,39 @@
       </c>
       <c r="C54" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>94.056470514778496</v>
+        <v>64.72181444075072</v>
       </c>
       <c r="D54" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>19.998652436865338</v>
+        <v>35.521350795598075</v>
       </c>
       <c r="E54" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>947247.56589432526</v>
+        <v>5830782.2341492688</v>
       </c>
       <c r="F54" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>11.127619696992685</v>
+        <v>68.496061192130554</v>
       </c>
       <c r="G54" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>420006.33894499374</v>
+        <v>281949.36214416457</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3195737.851179712</v>
+        <v>412354.61129303731</v>
       </c>
       <c r="I54" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>207571.46044182152</v>
+        <v>676658.5404016627</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2884849.9460297157</v>
+        <v>1996861.8048730171</v>
       </c>
       <c r="L54" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Potter","population":8512580.33333333,"food_ins_rate":94.0564705147785,"food_ins_rate_child":19.9986524368653,"snap":947247.565894325,"snap_percentage":11.1276196969927,"wic":420006.338944994,"free_lunch":3195737.85117971,"free_breakfast":207571.460441822,"food_banks":2884849.94602972},</v>
+        <v xml:space="preserve">    {"county_name":"Potter","population":"8,512,580","food_ins_rate":"65","food_ins_rate_child":"36","snap":"5,830,782","snap_percentage":"68","wic":"281,949","free_lunch":"412,355","free_breakfast":"676,659","food_banks":"1,996,862"},</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3417,39 +3526,39 @@
       </c>
       <c r="C55" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>20.647851957134343</v>
+        <v>66.731613041326568</v>
       </c>
       <c r="D55" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>52.798984006621225</v>
+        <v>59.870007170329217</v>
       </c>
       <c r="E55" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2329462.0135621745</v>
+        <v>7337939.1823948957</v>
       </c>
       <c r="F55" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>26.846307924918566</v>
+        <v>84.567412423117688</v>
       </c>
       <c r="G55" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1450374.5716696521</v>
+        <v>190639.48720642706</v>
       </c>
       <c r="H55" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1580811.4430431554</v>
+        <v>1577032.6706641437</v>
       </c>
       <c r="I55" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>473466.75315397378</v>
+        <v>298791.11135544139</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3762998.4408650701</v>
+        <v>1229737.0805520639</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Schuylkill","population":8677029.33333333,"food_ins_rate":20.6478519571343,"food_ins_rate_child":52.7989840066212,"snap":2329462.01356217,"snap_percentage":26.8463079249186,"wic":1450374.57166965,"free_lunch":1580811.44304316,"free_breakfast":473466.753153974,"food_banks":3762998.44086507},</v>
+        <v xml:space="preserve">    {"county_name":"Schuylkill","population":"8,677,029","food_ins_rate":"67","food_ins_rate_child":"60","snap":"7,337,939","snap_percentage":"85","wic":"190,639","free_lunch":"1,577,033","free_breakfast":"298,791","food_banks":"1,229,737"},</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3461,39 +3570,39 @@
       </c>
       <c r="C56" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>98.909555790010373</v>
+        <v>18.640642963976074</v>
       </c>
       <c r="D56" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>31.725351644094513</v>
+        <v>9.284307512843192</v>
       </c>
       <c r="E56" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2030603.0264282504</v>
+        <v>1729750.8427847608</v>
       </c>
       <c r="F56" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>22.966781683699399</v>
+        <v>19.564045486187677</v>
       </c>
       <c r="G56" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2053169.7374524686</v>
+        <v>533726.65004634683</v>
       </c>
       <c r="H56" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>230425.20625236962</v>
+        <v>1430357.470517355</v>
       </c>
       <c r="I56" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>870654.94832878991</v>
+        <v>195915.5384137604</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>64948.970662837717</v>
+        <v>4064734.6330046398</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Snyder","population":8841478.33333333,"food_ins_rate":98.9095557900104,"food_ins_rate_child":31.7253516440945,"snap":2030603.02642825,"snap_percentage":22.9667816836994,"wic":2053169.73745247,"free_lunch":230425.20625237,"free_breakfast":870654.94832879,"food_banks":64948.9706628377},</v>
+        <v xml:space="preserve">    {"county_name":"Snyder","population":"8,841,478","food_ins_rate":"19","food_ins_rate_child":"9","snap":"1,729,751","snap_percentage":"20","wic":"533,727","free_lunch":"1,430,357","free_breakfast":"195,916","food_banks":"4,064,735"},</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3505,39 +3614,39 @@
       </c>
       <c r="C57" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>71.907951009291054</v>
+        <v>2.4918977752475868</v>
       </c>
       <c r="D57" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>6.5474512534119089</v>
+        <v>34.607230187067145</v>
       </c>
       <c r="E57" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>8552613.8724391852</v>
+        <v>2960199.575755123</v>
       </c>
       <c r="F57" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>94.96649879445161</v>
+        <v>32.869458815180948</v>
       </c>
       <c r="G57" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1721735.989541217</v>
+        <v>343190.18076810928</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1429488.5820979017</v>
+        <v>756645.53656992211</v>
       </c>
       <c r="I57" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>239235.05231682365</v>
+        <v>787382.21930397267</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>2000679.3594969308</v>
+        <v>2790712.2197658443</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Somerset","population":9005927.33333333,"food_ins_rate":71.9079510092911,"food_ins_rate_child":6.54745125341191,"snap":8552613.87243919,"snap_percentage":94.9664987944516,"wic":1721735.98954122,"free_lunch":1429488.5820979,"free_breakfast":239235.052316824,"food_banks":2000679.35949693},</v>
+        <v xml:space="preserve">    {"county_name":"Somerset","population":"9,005,927","food_ins_rate":"2","food_ins_rate_child":"35","snap":"2,960,200","snap_percentage":"33","wic":"343,190","free_lunch":"756,646","free_breakfast":"787,382","food_banks":"2,790,712"},</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3549,39 +3658,39 @@
       </c>
       <c r="C58" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>69.280485808247718</v>
+        <v>81.067620665208366</v>
       </c>
       <c r="D58" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>46.840442392228837</v>
+        <v>6.9716005773576111</v>
       </c>
       <c r="E58" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>1894938.8708386819</v>
+        <v>1925736.8362122558</v>
       </c>
       <c r="F58" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>20.663697998421103</v>
+        <v>20.999539890335907</v>
       </c>
       <c r="G58" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1622691.2578280803</v>
+        <v>2594775.0227036588</v>
       </c>
       <c r="H58" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>226288.69011499471</v>
+        <v>3019975.0640911604</v>
       </c>
       <c r="I58" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>730173.90807572263</v>
+        <v>779734.31791289628</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3270769.9570165137</v>
+        <v>1977449.2810240618</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Sullivan","population":9170376.33333333,"food_ins_rate":69.2804858082477,"food_ins_rate_child":46.8404423922288,"snap":1894938.87083868,"snap_percentage":20.6636979984211,"wic":1622691.25782808,"free_lunch":226288.690114995,"free_breakfast":730173.908075723,"food_banks":3270769.95701651},</v>
+        <v xml:space="preserve">    {"county_name":"Sullivan","population":"9,170,376","food_ins_rate":"81","food_ins_rate_child":"7","snap":"1,925,737","snap_percentage":"21","wic":"2,594,775","free_lunch":"3,019,975","free_breakfast":"779,734","food_banks":"1,977,449"},</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3593,39 +3702,39 @@
       </c>
       <c r="C59" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>6.3826804096280725</v>
+        <v>11.170732984135078</v>
       </c>
       <c r="D59" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>20.688125132444704</v>
+        <v>25.803373989511282</v>
       </c>
       <c r="E59" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>6895888.931546947</v>
+        <v>248583.14155083345</v>
       </c>
       <c r="F59" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>73.872715185389822</v>
+        <v>2.6629651083366124</v>
       </c>
       <c r="G59" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1661924.039675633</v>
+        <v>1422364.6145946761</v>
       </c>
       <c r="H59" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1029952.6658920045</v>
+        <v>552551.67780834157</v>
       </c>
       <c r="I59" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>670761.71175522974</v>
+        <v>202198.28609255262</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>413990.40947531891</v>
+        <v>3878810.0965010147</v>
       </c>
       <c r="L59" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Susquehanna","population":9334825.33333333,"food_ins_rate":6.38268040962807,"food_ins_rate_child":20.6881251324447,"snap":6895888.93154695,"snap_percentage":73.8727151853898,"wic":1661924.03967563,"free_lunch":1029952.665892,"free_breakfast":670761.71175523,"food_banks":413990.409475319},</v>
+        <v xml:space="preserve">    {"county_name":"Susquehanna","population":"9,334,825","food_ins_rate":"11","food_ins_rate_child":"26","snap":"248,583","snap_percentage":"3","wic":"1,422,365","free_lunch":"552,552","free_breakfast":"202,198","food_banks":"3,878,810"},</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3637,39 +3746,39 @@
       </c>
       <c r="C60" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>2.7948889821136857</v>
+        <v>13.117280366605522</v>
       </c>
       <c r="D60" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>18.319615017605251</v>
+        <v>52.780113146980362</v>
       </c>
       <c r="E60" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>7880582.2298401333</v>
+        <v>4083731.566895287</v>
       </c>
       <c r="F60" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>82.959834123190419</v>
+        <v>42.989931900011683</v>
       </c>
       <c r="G60" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>984695.50300779461</v>
+        <v>1480603.408630006</v>
       </c>
       <c r="H60" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1375850.7645911938</v>
+        <v>1866256.940043445</v>
       </c>
       <c r="I60" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>788236.90373542311</v>
+        <v>548823.95452349877</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>4601412.1327538835</v>
+        <v>3182490.469652012</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Tioga","population":9499274.33333333,"food_ins_rate":2.79488898211369,"food_ins_rate_child":18.3196150176053,"snap":7880582.22984013,"snap_percentage":82.9598341231904,"wic":984695.503007795,"free_lunch":1375850.76459119,"free_breakfast":788236.903735423,"food_banks":4601412.13275388},</v>
+        <v xml:space="preserve">    {"county_name":"Tioga","population":"9,499,274","food_ins_rate":"13","food_ins_rate_child":"53","snap":"4,083,732","snap_percentage":"43","wic":"1,480,603","free_lunch":"1,866,257","free_breakfast":"548,824","food_banks":"3,182,490"},</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3681,39 +3790,39 @@
       </c>
       <c r="C61" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>53.596366650348216</v>
+        <v>73.46776204954773</v>
       </c>
       <c r="D61" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>36.196721182049245</v>
+        <v>14.736147598340919</v>
       </c>
       <c r="E61" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3137642.3428816153</v>
+        <v>9255860.2560335211</v>
       </c>
       <c r="F61" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>32.468255088169428</v>
+        <v>95.779441699319392</v>
       </c>
       <c r="G61" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1421731.5856646134</v>
+        <v>342571.94543598272</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>3240268.2559417728</v>
+        <v>3182347.0109852739</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>683291.358545603</v>
+        <v>541823.97250442836</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>373306.0997732472</v>
+        <v>2676324.2332467968</v>
       </c>
       <c r="L61" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Union","population":9663723.33333333,"food_ins_rate":53.5963666503482,"food_ins_rate_child":36.1967211820492,"snap":3137642.34288162,"snap_percentage":32.4682550881694,"wic":1421731.58566461,"free_lunch":3240268.25594177,"free_breakfast":683291.358545603,"food_banks":373306.099773247},</v>
+        <v xml:space="preserve">    {"county_name":"Union","population":"9,663,723","food_ins_rate":"73","food_ins_rate_child":"15","snap":"9,255,860","snap_percentage":"96","wic":"342,572","free_lunch":"3,182,347","free_breakfast":"541,824","food_banks":"2,676,324"},</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3725,39 +3834,39 @@
       </c>
       <c r="C62" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>64.910954028836713</v>
+        <v>88.803459528811487</v>
       </c>
       <c r="D62" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>55.204912154881583</v>
+        <v>36.164442229313629</v>
       </c>
       <c r="E62" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>9645557.7211998571</v>
+        <v>5548380.7991018286</v>
       </c>
       <c r="F62" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>98.141927044623387</v>
+        <v>56.453841171301846</v>
       </c>
       <c r="G62" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>700537.31876299717</v>
+        <v>1986757.8469934906</v>
       </c>
       <c r="H62" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2512865.734050137</v>
+        <v>1750420.3448138698</v>
       </c>
       <c r="I62" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>652902.61491725082</v>
+        <v>156818.53686000177</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1736594.24500271</v>
+        <v>664077.53955139953</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Venango","population":9828172.33333333,"food_ins_rate":64.9109540288367,"food_ins_rate_child":55.2049121548816,"snap":9645557.72119986,"snap_percentage":98.1419270446234,"wic":700537.318762997,"free_lunch":2512865.73405014,"free_breakfast":652902.614917251,"food_banks":1736594.24500271},</v>
+        <v xml:space="preserve">    {"county_name":"Venango","population":"9,828,172","food_ins_rate":"89","food_ins_rate_child":"36","snap":"5,548,381","snap_percentage":"56","wic":"1,986,758","free_lunch":"1,750,420","free_breakfast":"156,819","food_banks":"664,078"},</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3769,39 +3878,39 @@
       </c>
       <c r="C63" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>44.147445009391447</v>
+        <v>56.037120153720224</v>
       </c>
       <c r="D63" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>18.368945668018309</v>
+        <v>34.268297091170325</v>
       </c>
       <c r="E63" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3518885.1653293925</v>
+        <v>7665155.2424348881</v>
       </c>
       <c r="F63" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>35.214835506586397</v>
+        <v>76.70815281337147</v>
       </c>
       <c r="G63" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2328846.2743920023</v>
+        <v>857736.11035982217</v>
       </c>
       <c r="H63" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1273201.5887286405</v>
+        <v>2200407.1195051419</v>
       </c>
       <c r="I63" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>118159.75424120449</v>
+        <v>834324.00804670923</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>86452.192943038244</v>
+        <v>3466179.609037545</v>
       </c>
       <c r="L63" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Warren","population":9992621.33333333,"food_ins_rate":44.1474450093914,"food_ins_rate_child":18.3689456680183,"snap":3518885.16532939,"snap_percentage":35.2148355065864,"wic":2328846.274392,"free_lunch":1273201.58872864,"free_breakfast":118159.754241204,"food_banks":86452.1929430382},</v>
+        <v xml:space="preserve">    {"county_name":"Warren","population":"9,992,621","food_ins_rate":"56","food_ins_rate_child":"34","snap":"7,665,155","snap_percentage":"77","wic":"857,736","free_lunch":"2,200,407","free_breakfast":"834,324","food_banks":"3,466,180"},</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3813,39 +3922,39 @@
       </c>
       <c r="C64" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>90.987343366714086</v>
+        <v>5.766734358985004</v>
       </c>
       <c r="D64" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>19.885648198272165</v>
+        <v>32.282917256931185</v>
       </c>
       <c r="E64" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3760627.4054647605</v>
+        <v>4850839.0348927518</v>
       </c>
       <c r="F64" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>37.024725457725715</v>
+        <v>47.758249925407632</v>
       </c>
       <c r="G64" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1107391.245943405</v>
+        <v>2605839.4380822498</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>2597379.673642226</v>
+        <v>1431153.8103824528</v>
       </c>
       <c r="I64" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>41166.220770153195</v>
+        <v>320340.25422007928</v>
       </c>
       <c r="J64" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1584300.1119977192</v>
+        <v>4917129.0576551314</v>
       </c>
       <c r="L64" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Washington","population":10157070.3333333,"food_ins_rate":90.9873433667141,"food_ins_rate_child":19.8856481982722,"snap":3760627.40546476,"snap_percentage":37.0247254577257,"wic":1107391.2459434,"free_lunch":2597379.67364223,"free_breakfast":41166.2207701532,"food_banks":1584300.11199772},</v>
+        <v xml:space="preserve">    {"county_name":"Washington","population":"10,157,070","food_ins_rate":"6","food_ins_rate_child":"32","snap":"4,850,839","snap_percentage":"48","wic":"2,605,839","free_lunch":"1,431,154","free_breakfast":"320,340","food_banks":"4,917,129"},</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3857,39 +3966,39 @@
       </c>
       <c r="C65" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>65.006257690267915</v>
+        <v>70.200556618448729</v>
       </c>
       <c r="D65" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>2.7979857491940563</v>
+        <v>33.578507787199769</v>
       </c>
       <c r="E65" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>3551134.693792901</v>
+        <v>6631640.352169239</v>
       </c>
       <c r="F65" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>34.405154697763606</v>
+        <v>64.250621812550264</v>
       </c>
       <c r="G65" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2233754.4163064589</v>
+        <v>1355263.8889408442</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>940131.46078555577</v>
+        <v>2577794.1075430326</v>
       </c>
       <c r="I65" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>914635.55219932366</v>
+        <v>816682.25356777909</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>4788840.4227782981</v>
+        <v>1160281.460064278</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Wayne","population":10321519.3333333,"food_ins_rate":65.0062576902679,"food_ins_rate_child":2.79798574919406,"snap":3551134.6937929,"snap_percentage":34.4051546977636,"wic":2233754.41630646,"free_lunch":940131.460785556,"free_breakfast":914635.552199324,"food_banks":4788840.4227783},</v>
+        <v xml:space="preserve">    {"county_name":"Wayne","population":"10,321,519","food_ins_rate":"70","food_ins_rate_child":"34","snap":"6,631,640","snap_percentage":"64","wic":"1,355,264","free_lunch":"2,577,794","free_breakfast":"816,682","food_banks":"1,160,281"},</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3901,39 +4010,39 @@
       </c>
       <c r="C66" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>69.791147773798144</v>
+        <v>24.36027915526391</v>
       </c>
       <c r="D66" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>44.939617209532663</v>
+        <v>12.734079683204058</v>
       </c>
       <c r="E66" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>9391497.1863019131</v>
+        <v>10158560.833806252</v>
       </c>
       <c r="F66" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>89.562517144437393</v>
+        <v>96.877660802328876</v>
       </c>
       <c r="G66" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>48803.811105629546</v>
+        <v>1682886.0203024519</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>1901125.4917719346</v>
+        <v>540213.13698481384</v>
       </c>
       <c r="I66" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>1033209.6998546536</v>
+        <v>608406.79620026576</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>4758826.9724563705</v>
+        <v>4658899.2440043157</v>
       </c>
       <c r="L66" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v xml:space="preserve">    {"county_name":"Westmoreland","population":10485968.3333333,"food_ins_rate":69.7911477737981,"food_ins_rate_child":44.9396172095327,"snap":9391497.18630191,"snap_percentage":89.5625171444374,"wic":48803.8111056295,"free_lunch":1901125.49177193,"free_breakfast":1033209.69985465,"food_banks":4758826.97245637},</v>
+        <v xml:space="preserve">    {"county_name":"Westmoreland","population":"10,485,968","food_ins_rate":"24","food_ins_rate_child":"13","snap":"10,158,561","snap_percentage":"97","wic":"1,682,886","free_lunch":"540,213","free_breakfast":"608,407","food_banks":"4,658,899"},</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3945,39 +4054,39 @@
       </c>
       <c r="C67" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>70.571770391435138</v>
+        <v>94.869825331053519</v>
       </c>
       <c r="D67" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>11.810318150117043</v>
+        <v>42.113683932655206</v>
       </c>
       <c r="E67" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>5198990.4605782395</v>
+        <v>10075126.149905926</v>
       </c>
       <c r="F67" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>48.814898964631389</v>
+        <v>94.598416518131657</v>
       </c>
       <c r="G67" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>738542.10076529894</v>
+        <v>97548.770444483293</v>
       </c>
       <c r="H67" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>369990.5801027313</v>
+        <v>957914.32920381636</v>
       </c>
       <c r="I67" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>749892.30490453297</v>
+        <v>601337.85881843616</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>3968927.6829466848</v>
+        <v>1429273.1056316837</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67:L68" ca="1" si="17">CONCATENATE("    {""",$A$1,""":""",$A67,""",""",$B$1,""":",$B67,",""",$C$1,""":",$C67,",""",$D$1,""":",$D67,",""",$E$1,""":",$E67,",""",$F$1,""":",$F67,",""",$G$1,""":",$G67,",""",$H$1,""":",$H67,",""",$I$1,""":",$I67,",""",$J$1,""":",$J67,"},")</f>
-        <v xml:space="preserve">    {"county_name":"Wyoming","population":10650417.3333333,"food_ins_rate":70.5717703914351,"food_ins_rate_child":11.810318150117,"snap":5198990.46057824,"snap_percentage":48.8148989646314,"wic":738542.100765299,"free_lunch":369990.580102731,"free_breakfast":749892.304904533,"food_banks":3968927.68294668},</v>
+        <f t="shared" ref="L67:L68" ca="1" si="17">CONCATENATE("    {","""",$A$1,""":""",TEXT($A67,""),""",","""",$B$1,""":""",TEXT($B67,"#,###"),""",","""",$C$1,""":""",TEXT($C67,"#,###"),""",","""",$D$1,""":""",TEXT($D67,"#,###"),""",","""",$E$1,""":""",TEXT($E67,"#,###"),""",","""",$F$1,""":""",TEXT($F67,"#,###"),""",","""",$G$1,""":""",TEXT($G67,"#,###"),""",","""",$H$1,""":""",TEXT($H67,"#,###"),""",","""",$I$1,""":""",TEXT($I67,"#,###"),""",","""",$J$1,""":""",TEXT($J67,"#,###"),"""},")</f>
+        <v xml:space="preserve">    {"county_name":"Wyoming","population":"10,650,417","food_ins_rate":"95","food_ins_rate_child":"42","snap":"10,075,126","snap_percentage":"95","wic":"97,549","free_lunch":"957,914","free_breakfast":"601,338","food_banks":"1,429,273"},</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -3989,39 +4098,39 @@
       </c>
       <c r="C68" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>4.8459161004696156</v>
+        <v>17.454770208146464</v>
       </c>
       <c r="D68" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>31.693069950589408</v>
+        <v>48.185621516935726</v>
       </c>
       <c r="E68" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>2549531.7851729686</v>
+        <v>7000998.1724091042</v>
       </c>
       <c r="F68" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>23.574325438631337</v>
+        <v>64.7349486958596</v>
       </c>
       <c r="G68" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>538646.09215720568</v>
+        <v>2874064.5900313118</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>299756.09051681875</v>
+        <v>4073639.3800777583</v>
       </c>
       <c r="I68" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>321917.71213293995</v>
+        <v>991161.41098639718</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>1892458.6007830016</v>
+        <v>2491254.0853228751</v>
       </c>
       <c r="L68" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v xml:space="preserve">    {"county_name":"York","population":10814866.3333333,"food_ins_rate":4.84591610046962,"food_ins_rate_child":31.6930699505894,"snap":2549531.78517297,"snap_percentage":23.5743254386313,"wic":538646.092157206,"free_lunch":299756.090516819,"free_breakfast":321917.71213294,"food_banks":1892458.600783},</v>
+        <v xml:space="preserve">    {"county_name":"York","population":"10,814,866","food_ins_rate":"17","food_ins_rate_child":"48","snap":"7,000,998","snap_percentage":"65","wic":"2,874,065","free_lunch":"4,073,639","free_breakfast":"991,161","food_banks":"2,491,254"},</v>
       </c>
     </row>
   </sheetData>
@@ -4040,184 +4149,263 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.33203125" customWidth="1"/>
-    <col min="5" max="5" width="127.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.33203125" customWidth="1"/>
+    <col min="6" max="6" width="127.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>92</v>
       </c>
-      <c r="E2" t="str">
-        <f>CONCATENATE("    {""",$A$1,""":""",$A2,""",""",$B$1,""":""",$B2,""",""",$C$1,""":""",$C2,"""},")</f>
+      <c r="F2" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B2,""",""",$C$1,""":""",$C2,""",""",$D$1,""":""",$D2,"""},")</f>
         <v xml:space="preserve">    {"name":"county_name","class":"header","description":"Hunger In"},</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E11" si="0">CONCATENATE("    {""",$A$1,""":""",$A3,""",""",$B$1,""":""",$B3,""",""",$C$1,""":""",$C3,"""},")</f>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B3,""",""",$C$1,""":""",$C3,""",""",$D$1,""":""",$D3,"""},")</f>
         <v xml:space="preserve">    {"name":"population","class":"primary","description":"Total population"},</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B4,""",""",$C$1,""":""",$C4,""",""",$D$1,""":""",$D4,"""},")</f>
         <v xml:space="preserve">    {"name":"food_ins_rate","class":"primary","description":"Food insecurity rate"},</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s">
         <v>72</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B5,""",""",$C$1,""":""",$C5,""",""",$D$1,""":""",$D5,"""},")</f>
         <v xml:space="preserve">    {"name":"food_ins_rate_child","class":"primary","description":"Child food insecurity rate"},</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6">
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B6,""",""",$C$1,""":""",$C6,""",""",$D$1,""":""",$D6,"""},")</f>
+        <v xml:space="preserve">    {"name":"","class":"secondary_header","description":"How Nutrition Programs Help"},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B7,""",""",$C$1,""":""",$C7,""",""",$D$1,""":""",$D7,"""},")</f>
         <v xml:space="preserve">    {"name":"snap","class":"secondary","description":"SNAP participants"},</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
         <v>73</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B8,""",""",$C$1,""":""",$C8,""",""",$D$1,""":""",$D8,"""},")</f>
         <v xml:space="preserve">    {"name":"snap_percentage","class":"secondary","description":"Percentage of population receiving SNAP"},</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
+      <c r="E9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B9,""",""",$C$1,""":""",$C9,""",""",$D$1,""":""",$D9,"""},")</f>
         <v xml:space="preserve">    {"name":"wic","class":"secondary","description":"Number of WIC participants"},</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
+      <c r="E10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B10,""",""",$C$1,""":""",$C10,""",""",$D$1,""":""",$D10,"""},")</f>
         <v xml:space="preserve">    {"name":"free_lunch","class":"secondary","description":"Number Free and Reduced-Price School Lunch recipients"},</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
         <v>75</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
+      <c r="E11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B11,""",""",$C$1,""":""",$C11,""",""",$D$1,""":""",$D11,"""},")</f>
         <v xml:space="preserve">    {"name":"free_breakfast","class":"secondary","description":"Number of Free and Reduced-Price School Breakfast recipients"},</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" t="s">
         <v>76</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
+      <c r="E12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" t="str">
+        <f>CONCATENATE("    {""",$B$1,""":""",$B12,""",""",$C$1,""":""",$C12,""",""",$D$1,""":""",$D12,"""},")</f>
         <v xml:space="preserve">    {"name":"food_banks","class":"secondary","description":"Number of State Food Purchase Program (Food Banks) participants"},</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="F6" emptyCellReference="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -4227,4 +4415,445 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="39.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="str">
+        <f>IF(Fields!$A2 = "","", CONCATENATE(","""""""",$",Fields!$A2,"$1,"""""":"""""",TEXT($",Fields!$A2,"222,""",Fields!$E2,"""),"""""","""))</f>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""","</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE($B1,$A2)</f>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""","</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="str">
+        <f>IF(Fields!$A3 = "","", CONCATENATE(","""""""",$",Fields!$A3,"$1,"""""":"""""",TEXT($",Fields!$A3,"222,""",Fields!$E3,"""),"""""","""))</f>
+        <v>,"""",$B$1,""":""",TEXT($B222,"#,###"),""","</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B42" si="0">CONCATENATE($B2,$A3)</f>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="str">
+        <f>IF(Fields!$A4 = "","", CONCATENATE(","""""""",$",Fields!$A4,"$1,"""""":"""""",TEXT($",Fields!$A4,"222,""",Fields!$E4,"""),"""""","""))</f>
+        <v>,"""",$C$1,""":""",TEXT($C222,"#,###"),""","</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="str">
+        <f>IF(Fields!$A5 = "","", CONCATENATE(","""""""",$",Fields!$A5,"$1,"""""":"""""",TEXT($",Fields!$A5,"222,""",Fields!$E5,"""),"""""","""))</f>
+        <v>,"""",$D$1,""":""",TEXT($D222,"#,###"),""","</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="str">
+        <f>IF(Fields!$A6 = "","", CONCATENATE(","""""""",$",Fields!$A6,"$1,"""""":"""""",TEXT($",Fields!$A6,"222,""",Fields!$E6,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="str">
+        <f>IF(Fields!$A7 = "","", CONCATENATE(","""""""",$",Fields!$A7,"$1,"""""":"""""",TEXT($",Fields!$A7,"222,""",Fields!$E7,"""),"""""","""))</f>
+        <v>,"""",$E$1,""":""",TEXT($E222,"#,###"),""","</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="str">
+        <f>IF(Fields!$A8 = "","", CONCATENATE(","""""""",$",Fields!$A8,"$1,"""""":"""""",TEXT($",Fields!$A8,"222,""",Fields!$E8,"""),"""""","""))</f>
+        <v>,"""",$F$1,""":""",TEXT($F222,"#,###"),""","</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="str">
+        <f>IF(Fields!$A9 = "","", CONCATENATE(","""""""",$",Fields!$A9,"$1,"""""":"""""",TEXT($",Fields!$A9,"222,""",Fields!$E9,"""),"""""","""))</f>
+        <v>,"""",$G$1,""":""",TEXT($G222,"#,###"),""","</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="str">
+        <f>IF(Fields!$A10 = "","", CONCATENATE(","""""""",$",Fields!$A10,"$1,"""""":"""""",TEXT($",Fields!$A10,"222,""",Fields!$E10,"""),"""""","""))</f>
+        <v>,"""",$H$1,""":""",TEXT($H222,"#,###"),""","</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="str">
+        <f>IF(Fields!$A11 = "","", CONCATENATE(","""""""",$",Fields!$A11,"$1,"""""":"""""",TEXT($",Fields!$A11,"222,""",Fields!$E11,"""),"""""","""))</f>
+        <v>,"""",$I$1,""":""",TEXT($I222,"#,###"),""","</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="str">
+        <f>IF(Fields!$A12 = "","", CONCATENATE(","""""""",$",Fields!$A12,"$1,"""""":"""""",TEXT($",Fields!$A12,"222,""",Fields!$E12,"""),"""""","""))</f>
+        <v>,"""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="str">
+        <f>IF(Fields!$A13 = "","", CONCATENATE(","""""""",$",Fields!$A13,"$1,"""""":"""""",TEXT($",Fields!$A13,"222,""",Fields!$E13,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="str">
+        <f>IF(Fields!$A14 = "","", CONCATENATE(","""""""",$",Fields!$A14,"$1,"""""":"""""",TEXT($",Fields!$A14,"222,""",Fields!$E14,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="str">
+        <f>IF(Fields!$A15 = "","", CONCATENATE(","""""""",$",Fields!$A15,"$1,"""""":"""""",TEXT($",Fields!$A15,"222,""",Fields!$E15,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="str">
+        <f>IF(Fields!$A16 = "","", CONCATENATE(","""""""",$",Fields!$A16,"$1,"""""":"""""",TEXT($",Fields!$A16,"222,""",Fields!$E16,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="str">
+        <f>IF(Fields!$A17 = "","", CONCATENATE(","""""""",$",Fields!$A17,"$1,"""""":"""""",TEXT($",Fields!$A17,"222,""",Fields!$E17,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="str">
+        <f>IF(Fields!$A18 = "","", CONCATENATE(","""""""",$",Fields!$A18,"$1,"""""":"""""",TEXT($",Fields!$A18,"222,""",Fields!$E18,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="str">
+        <f>IF(Fields!$A19 = "","", CONCATENATE(","""""""",$",Fields!$A19,"$1,"""""":"""""",TEXT($",Fields!$A19,"222,""",Fields!$E19,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="str">
+        <f>IF(Fields!$A20 = "","", CONCATENATE(","""""""",$",Fields!$A20,"$1,"""""":"""""",TEXT($",Fields!$A20,"222,""",Fields!$E20,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="str">
+        <f>IF(Fields!$A21 = "","", CONCATENATE(","""""""",$",Fields!$A21,"$1,"""""":"""""",TEXT($",Fields!$A21,"222,""",Fields!$E21,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="str">
+        <f>IF(Fields!$A22 = "","", CONCATENATE(","""""""",$",Fields!$A22,"$1,"""""":"""""",TEXT($",Fields!$A22,"222,""",Fields!$E22,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="str">
+        <f>IF(Fields!$A23 = "","", CONCATENATE(","""""""",$",Fields!$A23,"$1,"""""":"""""",TEXT($",Fields!$A23,"222,""",Fields!$E23,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="str">
+        <f>IF(Fields!$A24 = "","", CONCATENATE(","""""""",$",Fields!$A24,"$1,"""""":"""""",TEXT($",Fields!$A24,"222,""",Fields!$E24,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="str">
+        <f>IF(Fields!$A25 = "","", CONCATENATE(","""""""",$",Fields!$A25,"$1,"""""":"""""",TEXT($",Fields!$A25,"222,""",Fields!$E25,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="str">
+        <f>IF(Fields!$A26 = "","", CONCATENATE(","""""""",$",Fields!$A26,"$1,"""""":"""""",TEXT($",Fields!$A26,"222,""",Fields!$E26,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="str">
+        <f>IF(Fields!$A27 = "","", CONCATENATE(","""""""",$",Fields!$A27,"$1,"""""":"""""",TEXT($",Fields!$A27,"222,""",Fields!$E27,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="str">
+        <f>IF(Fields!$A28 = "","", CONCATENATE(","""""""",$",Fields!$A28,"$1,"""""":"""""",TEXT($",Fields!$A28,"222,""",Fields!$E28,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="str">
+        <f>IF(Fields!$A29 = "","", CONCATENATE(","""""""",$",Fields!$A29,"$1,"""""":"""""",TEXT($",Fields!$A29,"222,""",Fields!$E29,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="str">
+        <f>IF(Fields!$A30 = "","", CONCATENATE(","""""""",$",Fields!$A30,"$1,"""""":"""""",TEXT($",Fields!$A30,"222,""",Fields!$E30,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="str">
+        <f>IF(Fields!$A31 = "","", CONCATENATE(","""""""",$",Fields!$A31,"$1,"""""":"""""",TEXT($",Fields!$A31,"222,""",Fields!$E31,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="str">
+        <f>IF(Fields!$A32 = "","", CONCATENATE(","""""""",$",Fields!$A32,"$1,"""""":"""""",TEXT($",Fields!$A32,"222,""",Fields!$E32,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="str">
+        <f>IF(Fields!$A33 = "","", CONCATENATE(","""""""",$",Fields!$A33,"$1,"""""":"""""",TEXT($",Fields!$A33,"222,""",Fields!$E33,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="str">
+        <f>IF(Fields!$A34 = "","", CONCATENATE(","""""""",$",Fields!$A34,"$1,"""""":"""""",TEXT($",Fields!$A34,"222,""",Fields!$E34,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="str">
+        <f>IF(Fields!$A35 = "","", CONCATENATE(","""""""",$",Fields!$A35,"$1,"""""":"""""",TEXT($",Fields!$A35,"222,""",Fields!$E35,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="str">
+        <f>IF(Fields!$A36 = "","", CONCATENATE(","""""""",$",Fields!$A36,"$1,"""""":"""""",TEXT($",Fields!$A36,"222,""",Fields!$E36,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="str">
+        <f>IF(Fields!$A37 = "","", CONCATENATE(","""""""",$",Fields!$A37,"$1,"""""":"""""",TEXT($",Fields!$A37,"222,""",Fields!$E37,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="str">
+        <f>IF(Fields!$A38 = "","", CONCATENATE(","""""""",$",Fields!$A38,"$1,"""""":"""""",TEXT($",Fields!$A38,"222,""",Fields!$E38,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="str">
+        <f>IF(Fields!$A39 = "","", CONCATENATE(","""""""",$",Fields!$A39,"$1,"""""":"""""",TEXT($",Fields!$A39,"222,""",Fields!$E39,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="str">
+        <f>IF(Fields!$A40 = "","", CONCATENATE(","""""""",$",Fields!$A40,"$1,"""""":"""""",TEXT($",Fields!$A40,"222,""",Fields!$E40,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="str">
+        <f>IF(Fields!$A41 = "","", CONCATENATE(","""""""",$",Fields!$A41,"$1,"""""":"""""",TEXT($",Fields!$A41,"222,""",Fields!$E41,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="str">
+        <f>IF(Fields!$A42 = "","", CONCATENATE(","""""""",$",Fields!$A42,"$1,"""""":"""""",TEXT($",Fields!$A42,"222,""",Fields!$E42,"""),"""""","""))</f>
+        <v/>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>,"""",$A$1,""":""",TEXT($A222,""),""",","""",$B$1,""":""",TEXT($B222,"#,###"),""",","""",$C$1,""":""",TEXT($C222,"#,###"),""",","""",$D$1,""":""",TEXT($D222,"#,###"),""",","""",$E$1,""":""",TEXT($E222,"#,###"),""",","""",$F$1,""":""",TEXT($F222,"#,###"),""",","""",$G$1,""":""",TEXT($G222,"#,###"),""",","""",$H$1,""":""",TEXT($H222,"#,###"),""",","""",$I$1,""":""",TEXT($I222,"#,###"),""",","""",$J$1,""":""",TEXT($J222,"#,###"),""","</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(CONCATENATE("CONCATENATE(""    {""",$B$42,")"),""","")","""},"")"),"222","2")</f>
+        <v>CONCATENATE("    {","""",$A$1,""":""",TEXT($A2,""),""",","""",$B$1,""":""",TEXT($B2,"#,###"),""",","""",$C$1,""":""",TEXT($C2,"#,###"),""",","""",$D$1,""":""",TEXT($D2,"#,###"),""",","""",$E$1,""":""",TEXT($E2,"#,###"),""",","""",$F$1,""":""",TEXT($F2,"#,###"),""",","""",$G$1,""":""",TEXT($G2,"#,###"),""",","""",$H$1,""":""",TEXT($H2,"#,###"),""",","""",$I$1,""":""",TEXT($I2,"#,###"),""",","""",$J$1,""":""",TEXT($J2,"#,###"),"""},")</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>